<commit_message>
Atualização da planilha e controle de erro
Testando o controle de erro
</commit_message>
<xml_diff>
--- a/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
+++ b/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3162c0a97888194f/Documentos/GitHub/algoritmos/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="167" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61A25592-35BB-4437-9C23-11DC8172695B}"/>
+  <xr:revisionPtr revIDLastSave="223" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{955BCC52-E772-460F-B722-57B3E32A6AD7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="53">
   <si>
     <t>op</t>
   </si>
@@ -239,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +301,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -386,7 +392,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -513,6 +519,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutro" xfId="2" builtinId="28"/>
@@ -4305,10 +4312,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="B2:K53"/>
+  <dimension ref="B2:M53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4546,8 +4553,8 @@
       <c r="B9" s="11">
         <v>127</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>41</v>
+      <c r="C9" s="11">
+        <v>1111111</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>11</v>
@@ -4660,8 +4667,8 @@
       <c r="H12" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="18" t="s">
-        <v>3</v>
+      <c r="I12" s="18">
+        <v>0</v>
       </c>
       <c r="J12" s="20" t="s">
         <v>15</v>
@@ -4692,8 +4699,8 @@
       <c r="H13" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="18" t="s">
-        <v>3</v>
+      <c r="I13" s="18">
+        <v>0</v>
       </c>
       <c r="J13" s="20" t="s">
         <v>15</v>
@@ -4724,8 +4731,8 @@
       <c r="H14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="18" t="s">
-        <v>3</v>
+      <c r="I14" s="18">
+        <v>0</v>
       </c>
       <c r="J14" s="20" t="s">
         <v>16</v>
@@ -4756,11 +4763,11 @@
       <c r="H15" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="23" t="s">
-        <v>2</v>
+      <c r="I15" s="23">
+        <v>1</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>8</v>
@@ -4792,13 +4799,13 @@
         <v>2</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K16" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="21">
         <v>-1</v>
       </c>
@@ -4820,8 +4827,8 @@
       <c r="H17" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="23" t="s">
-        <v>3</v>
+      <c r="I17" s="23">
+        <v>0</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>16</v>
@@ -4830,7 +4837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="21">
         <v>-1</v>
       </c>
@@ -4852,8 +4859,8 @@
       <c r="H18" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="23" t="s">
-        <v>2</v>
+      <c r="I18" s="23">
+        <v>1</v>
       </c>
       <c r="J18" s="25" t="s">
         <v>14</v>
@@ -4862,7 +4869,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="21">
         <v>-1</v>
       </c>
@@ -4894,7 +4901,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="26">
         <v>1</v>
       </c>
@@ -4916,8 +4923,8 @@
       <c r="H20" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I20" s="28" t="s">
-        <v>3</v>
+      <c r="I20" s="28">
+        <v>0</v>
       </c>
       <c r="J20" s="30" t="s">
         <v>15</v>
@@ -4925,8 +4932,9 @@
       <c r="K20" s="26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M20" s="46"/>
+    </row>
+    <row r="21" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="26">
         <v>1</v>
       </c>
@@ -4958,7 +4966,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="26">
         <v>1</v>
       </c>
@@ -4980,8 +4988,8 @@
       <c r="H22" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="28" t="s">
-        <v>2</v>
+      <c r="I22" s="28">
+        <v>1</v>
       </c>
       <c r="J22" s="30" t="s">
         <v>17</v>
@@ -4990,7 +4998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26">
         <v>1</v>
       </c>
@@ -5012,8 +5020,8 @@
       <c r="H23" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="28" t="s">
-        <v>3</v>
+      <c r="I23" s="28">
+        <v>0</v>
       </c>
       <c r="J23" s="30" t="s">
         <v>15</v>
@@ -5021,8 +5029,9 @@
       <c r="K23" s="26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M23" s="46"/>
+    </row>
+    <row r="24" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="31">
         <v>127</v>
       </c>
@@ -5044,8 +5053,8 @@
       <c r="H24" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="32" t="s">
-        <v>3</v>
+      <c r="I24" s="32">
+        <v>0</v>
       </c>
       <c r="J24" s="35" t="s">
         <v>16</v>
@@ -5054,7 +5063,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="31">
         <v>127</v>
       </c>
@@ -5076,8 +5085,8 @@
       <c r="H25" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="I25" s="32" t="s">
-        <v>2</v>
+      <c r="I25" s="32">
+        <v>1</v>
       </c>
       <c r="J25" s="35" t="s">
         <v>14</v>
@@ -5086,7 +5095,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="31">
         <v>127</v>
       </c>
@@ -5108,8 +5117,8 @@
       <c r="H26" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="32" t="s">
-        <v>2</v>
+      <c r="I26" s="32">
+        <v>1</v>
       </c>
       <c r="J26" s="35" t="s">
         <v>14</v>
@@ -5118,7 +5127,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -5130,13 +5139,13 @@
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J30" s="36"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J31" s="36"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J32" s="36"/>
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.25">
@@ -5210,7 +5219,7 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C3:D7 F3:H3 J3 I4:J26 I3 F4:H10 F11:H12 F13:H15 F18:H25 F16:H17 F26:H26 C8:D21 C24:D26 C22:D22 C23:D23" numberStoredAsText="1"/>
+    <ignoredError sqref="C3:D7 F3:H3 J3 I4:J11 I3 F4:H10 F11:H12 F13:H15 F18:H25 F16:H17 F26:H26 C8:D8 C24:D26 C22:D22 C23:D23 I19:J19 J12 J13:J15 I21:J21 J20 J26 J23 C10:D21 D9 J24 J25 I16 J16:J17 J18 J22" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Erro no modulo de subtração
Adicionada uma nota no main.c informando o erro
</commit_message>
<xml_diff>
--- a/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
+++ b/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3162c0a97888194f/Documentos/GitHub/algoritmos/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="223" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{955BCC52-E772-460F-B722-57B3E32A6AD7}"/>
+  <xr:revisionPtr revIDLastSave="351" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03E95CE2-9F03-4A94-B9B5-0E1C9EE7B762}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
+    <workbookView xWindow="0" yWindow="1245" windowWidth="13935" windowHeight="11385" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="numeros_binarios_8bits" sheetId="1" r:id="rId1"/>
     <sheet name="Folha de testes" sheetId="3" r:id="rId2"/>
     <sheet name="Tabela_erros_calculadora" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Tabela_erros_calculadora!$A$2:$K$26</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="54">
   <si>
     <t>op</t>
   </si>
@@ -198,6 +223,9 @@
   <si>
     <t>overflow b9</t>
   </si>
+  <si>
+    <t>id</t>
+  </si>
 </sst>
 </file>
 
@@ -239,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,12 +312,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFD9FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
@@ -307,6 +329,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,10 +459,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -418,21 +488,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -494,14 +549,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -519,7 +575,126 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="18" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="19" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutro" xfId="2" builtinId="28"/>
@@ -898,10 +1073,10 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
-      <c r="B2" s="38">
+      <c r="B2" s="33">
         <v>-129</v>
       </c>
-      <c r="C2" s="39" t="str">
+      <c r="C2" s="34" t="str">
         <f>RIGHT(DEC2BIN(B2,8),9)</f>
         <v>101111111</v>
       </c>
@@ -981,12 +1156,12 @@
         <v>01010100</v>
       </c>
       <c r="P3" s="8"/>
-      <c r="R3" s="40" t="s">
+      <c r="R3" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="S3" s="40"/>
-      <c r="T3" s="40"/>
-      <c r="U3" s="40"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
+      <c r="U3" s="36"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
@@ -1030,12 +1205,12 @@
         <v>01010101</v>
       </c>
       <c r="P4" s="8"/>
-      <c r="R4" s="40" t="s">
+      <c r="R4" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="S4" s="40"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="40"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
@@ -1079,12 +1254,12 @@
         <v>01010110</v>
       </c>
       <c r="P5" s="8"/>
-      <c r="R5" s="40" t="s">
+      <c r="R5" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
+      <c r="S5" s="36"/>
+      <c r="T5" s="36"/>
+      <c r="U5" s="36"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
@@ -2883,10 +3058,10 @@
         <v>01001000</v>
       </c>
       <c r="M47" s="8"/>
-      <c r="N47" s="38">
+      <c r="N47" s="33">
         <v>128</v>
       </c>
-      <c r="O47" s="39" t="str">
+      <c r="O47" s="34" t="str">
         <f>"0"&amp;DEC2BIN(N47,8)</f>
         <v>010000000</v>
       </c>
@@ -2926,10 +3101,10 @@
         <v>01001001</v>
       </c>
       <c r="M48" s="8"/>
-      <c r="N48" s="38">
+      <c r="N48" s="33">
         <v>129</v>
       </c>
-      <c r="O48" s="39" t="str">
+      <c r="O48" s="34" t="str">
         <f t="shared" ref="O48:O54" si="11">DEC2BIN(N48,8)</f>
         <v>10000001</v>
       </c>
@@ -2969,10 +3144,10 @@
         <v>01001010</v>
       </c>
       <c r="M49" s="8"/>
-      <c r="N49" s="38">
+      <c r="N49" s="33">
         <v>130</v>
       </c>
-      <c r="O49" s="39" t="str">
+      <c r="O49" s="34" t="str">
         <f t="shared" si="11"/>
         <v>10000010</v>
       </c>
@@ -3012,10 +3187,10 @@
         <v>01001011</v>
       </c>
       <c r="M50" s="8"/>
-      <c r="N50" s="38">
+      <c r="N50" s="33">
         <v>131</v>
       </c>
-      <c r="O50" s="39" t="str">
+      <c r="O50" s="34" t="str">
         <f t="shared" si="11"/>
         <v>10000011</v>
       </c>
@@ -3055,10 +3230,10 @@
         <v>01001100</v>
       </c>
       <c r="M51" s="8"/>
-      <c r="N51" s="38">
+      <c r="N51" s="33">
         <v>132</v>
       </c>
-      <c r="O51" s="39" t="str">
+      <c r="O51" s="34" t="str">
         <f t="shared" si="11"/>
         <v>10000100</v>
       </c>
@@ -3098,10 +3273,10 @@
         <v>01001101</v>
       </c>
       <c r="M52" s="8"/>
-      <c r="N52" s="38">
+      <c r="N52" s="33">
         <v>133</v>
       </c>
-      <c r="O52" s="39" t="str">
+      <c r="O52" s="34" t="str">
         <f t="shared" si="11"/>
         <v>10000101</v>
       </c>
@@ -3141,10 +3316,10 @@
         <v>01001110</v>
       </c>
       <c r="M53" s="8"/>
-      <c r="N53" s="38">
+      <c r="N53" s="33">
         <v>134</v>
       </c>
-      <c r="O53" s="39" t="str">
+      <c r="O53" s="34" t="str">
         <f t="shared" si="11"/>
         <v>10000110</v>
       </c>
@@ -3184,10 +3359,10 @@
         <v>01001111</v>
       </c>
       <c r="M54" s="8"/>
-      <c r="N54" s="38">
+      <c r="N54" s="33">
         <v>135</v>
       </c>
-      <c r="O54" s="39" t="str">
+      <c r="O54" s="34" t="str">
         <f t="shared" si="11"/>
         <v>10000111</v>
       </c>
@@ -3236,90 +3411,90 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
     </row>
     <row r="3" spans="1:22" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="37" t="s">
+      <c r="A3" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="32">
         <v>6</v>
       </c>
-      <c r="E3" s="37">
+      <c r="E3" s="32">
         <v>5</v>
       </c>
-      <c r="F3" s="37">
+      <c r="F3" s="32">
         <v>4</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="32">
         <v>3</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="32">
         <v>2</v>
       </c>
-      <c r="I3" s="37">
-        <v>1</v>
-      </c>
-      <c r="J3" s="37">
+      <c r="I3" s="32">
+        <v>1</v>
+      </c>
+      <c r="J3" s="32">
         <v>0</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="37" t="s">
+      <c r="L3" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="37">
+      <c r="O3" s="32">
         <v>6</v>
       </c>
-      <c r="P3" s="37">
+      <c r="P3" s="32">
         <v>5</v>
       </c>
-      <c r="Q3" s="37">
+      <c r="Q3" s="32">
         <v>4</v>
       </c>
-      <c r="R3" s="37">
+      <c r="R3" s="32">
         <v>3</v>
       </c>
-      <c r="S3" s="37">
+      <c r="S3" s="32">
         <v>2</v>
       </c>
-      <c r="T3" s="37">
-        <v>1</v>
-      </c>
-      <c r="U3" s="37">
+      <c r="T3" s="32">
+        <v>1</v>
+      </c>
+      <c r="U3" s="32">
         <v>0</v>
       </c>
     </row>
@@ -3583,31 +3758,31 @@
       </c>
     </row>
     <row r="9" spans="1:22" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="43" t="s">
+      <c r="L9" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="44"/>
-      <c r="R9" s="44"/>
-      <c r="S9" s="44"/>
-      <c r="T9" s="44"/>
-      <c r="U9" s="45"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="41"/>
       <c r="V9" s="3"/>
     </row>
     <row r="10" spans="1:22" ht="21" x14ac:dyDescent="0.35">
@@ -3634,65 +3809,65 @@
       <c r="U10" s="5"/>
     </row>
     <row r="11" spans="1:22" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="37" t="s">
+      <c r="A11" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="32">
         <v>6</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E11" s="32">
         <v>5</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="32">
         <v>4</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="32">
         <v>3</v>
       </c>
-      <c r="H11" s="37">
+      <c r="H11" s="32">
         <v>2</v>
       </c>
-      <c r="I11" s="37">
-        <v>1</v>
-      </c>
-      <c r="J11" s="37">
+      <c r="I11" s="32">
+        <v>1</v>
+      </c>
+      <c r="J11" s="32">
         <v>0</v>
       </c>
       <c r="K11" s="2"/>
-      <c r="L11" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="M11" s="37" t="s">
+      <c r="L11" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="N11" s="37" t="s">
+      <c r="N11" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="O11" s="37">
+      <c r="O11" s="32">
         <v>6</v>
       </c>
-      <c r="P11" s="37">
+      <c r="P11" s="32">
         <v>5</v>
       </c>
-      <c r="Q11" s="37">
+      <c r="Q11" s="32">
         <v>4</v>
       </c>
-      <c r="R11" s="37">
+      <c r="R11" s="32">
         <v>3</v>
       </c>
-      <c r="S11" s="37">
+      <c r="S11" s="32">
         <v>2</v>
       </c>
-      <c r="T11" s="37">
-        <v>1</v>
-      </c>
-      <c r="U11" s="37">
+      <c r="T11" s="32">
+        <v>1</v>
+      </c>
+      <c r="U11" s="32">
         <v>0</v>
       </c>
     </row>
@@ -3812,29 +3987,29 @@
       <c r="U16" s="1"/>
     </row>
     <row r="17" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="45"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="41"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="43" t="s">
+      <c r="L17" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="44"/>
-      <c r="N17" s="44"/>
-      <c r="O17" s="44"/>
-      <c r="P17" s="44"/>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="44"/>
-      <c r="S17" s="44"/>
-      <c r="T17" s="44"/>
-      <c r="U17" s="45"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="41"/>
     </row>
     <row r="18" spans="1:21" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
@@ -3860,65 +4035,65 @@
       <c r="U18" s="5"/>
     </row>
     <row r="19" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="37" t="s">
+      <c r="A19" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="37">
+      <c r="D19" s="32">
         <v>6</v>
       </c>
-      <c r="E19" s="37">
+      <c r="E19" s="32">
         <v>5</v>
       </c>
-      <c r="F19" s="37">
+      <c r="F19" s="32">
         <v>4</v>
       </c>
-      <c r="G19" s="37">
+      <c r="G19" s="32">
         <v>3</v>
       </c>
-      <c r="H19" s="37">
+      <c r="H19" s="32">
         <v>2</v>
       </c>
-      <c r="I19" s="37">
-        <v>1</v>
-      </c>
-      <c r="J19" s="37">
+      <c r="I19" s="32">
+        <v>1</v>
+      </c>
+      <c r="J19" s="32">
         <v>0</v>
       </c>
       <c r="K19" s="2"/>
-      <c r="L19" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="M19" s="37" t="s">
+      <c r="L19" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="N19" s="37" t="s">
+      <c r="N19" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="O19" s="37">
+      <c r="O19" s="32">
         <v>6</v>
       </c>
-      <c r="P19" s="37">
+      <c r="P19" s="32">
         <v>5</v>
       </c>
-      <c r="Q19" s="37">
+      <c r="Q19" s="32">
         <v>4</v>
       </c>
-      <c r="R19" s="37">
+      <c r="R19" s="32">
         <v>3</v>
       </c>
-      <c r="S19" s="37">
+      <c r="S19" s="32">
         <v>2</v>
       </c>
-      <c r="T19" s="37">
-        <v>1</v>
-      </c>
-      <c r="U19" s="37">
+      <c r="T19" s="32">
+        <v>1</v>
+      </c>
+      <c r="U19" s="32">
         <v>0</v>
       </c>
     </row>
@@ -4038,31 +4213,31 @@
       <c r="U24" s="1"/>
     </row>
     <row r="25" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="45"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="41"/>
       <c r="K25" s="2"/>
-      <c r="L25" s="43" t="s">
+      <c r="L25" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="44"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="44"/>
-      <c r="P25" s="44"/>
-      <c r="Q25" s="44"/>
-      <c r="R25" s="44"/>
-      <c r="S25" s="44"/>
-      <c r="T25" s="44"/>
-      <c r="U25" s="45"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="40"/>
+      <c r="S25" s="40"/>
+      <c r="T25" s="40"/>
+      <c r="U25" s="41"/>
     </row>
     <row r="26" spans="1:21" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
@@ -4088,65 +4263,65 @@
       <c r="U26" s="5"/>
     </row>
     <row r="27" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="37" t="s">
+      <c r="A27" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="37">
+      <c r="D27" s="32">
         <v>6</v>
       </c>
-      <c r="E27" s="37">
+      <c r="E27" s="32">
         <v>5</v>
       </c>
-      <c r="F27" s="37">
+      <c r="F27" s="32">
         <v>4</v>
       </c>
-      <c r="G27" s="37">
+      <c r="G27" s="32">
         <v>3</v>
       </c>
-      <c r="H27" s="37">
+      <c r="H27" s="32">
         <v>2</v>
       </c>
-      <c r="I27" s="37">
-        <v>1</v>
-      </c>
-      <c r="J27" s="37">
+      <c r="I27" s="32">
+        <v>1</v>
+      </c>
+      <c r="J27" s="32">
         <v>0</v>
       </c>
       <c r="K27" s="2"/>
-      <c r="L27" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="M27" s="37" t="s">
+      <c r="L27" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="M27" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="37" t="s">
+      <c r="N27" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="O27" s="37">
+      <c r="O27" s="32">
         <v>6</v>
       </c>
-      <c r="P27" s="37">
+      <c r="P27" s="32">
         <v>5</v>
       </c>
-      <c r="Q27" s="37">
+      <c r="Q27" s="32">
         <v>4</v>
       </c>
-      <c r="R27" s="37">
+      <c r="R27" s="32">
         <v>3</v>
       </c>
-      <c r="S27" s="37">
+      <c r="S27" s="32">
         <v>2</v>
       </c>
-      <c r="T27" s="37">
-        <v>1</v>
-      </c>
-      <c r="U27" s="37">
+      <c r="T27" s="32">
+        <v>1</v>
+      </c>
+      <c r="U27" s="32">
         <v>0</v>
       </c>
     </row>
@@ -4266,29 +4441,29 @@
       <c r="U32" s="1"/>
     </row>
     <row r="33" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="45"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="41"/>
       <c r="K33" s="2"/>
-      <c r="L33" s="43" t="s">
+      <c r="L33" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="M33" s="44"/>
-      <c r="N33" s="44"/>
-      <c r="O33" s="44"/>
-      <c r="P33" s="44"/>
-      <c r="Q33" s="44"/>
-      <c r="R33" s="44"/>
-      <c r="S33" s="44"/>
-      <c r="T33" s="44"/>
-      <c r="U33" s="45"/>
+      <c r="M33" s="40"/>
+      <c r="N33" s="40"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="40"/>
+      <c r="Q33" s="40"/>
+      <c r="R33" s="40"/>
+      <c r="S33" s="40"/>
+      <c r="T33" s="40"/>
+      <c r="U33" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4309,13 +4484,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED239D7-98B0-43DB-AD6A-A78832542F2A}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="B2:M53"/>
+  <dimension ref="A2:O53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4323,9 +4498,16 @@
     <col min="2" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="13.140625" style="6" customWidth="1"/>
     <col min="5" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="B2" s="10" t="s">
         <v>33</v>
       </c>
@@ -4357,221 +4539,333 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11">
+    <row r="3" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="42">
+        <v>1</v>
+      </c>
+      <c r="B3" s="42">
         <v>-128</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="42">
         <v>-1</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="44" cm="1">
+        <f t="array" aca="1" ref="G3" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
         <v>-129</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11">
+      <c r="K3" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="str">
+        <f ca="1">DEC2BIN(G3,10)</f>
+        <v>1101111111</v>
+      </c>
+      <c r="N3" t="str">
+        <f ca="1">RIGHT(M3,9)</f>
+        <v>101111111</v>
+      </c>
+      <c r="O3" t="b">
+        <f ca="1">N3=H3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="47">
+        <v>2</v>
+      </c>
+      <c r="B4" s="47">
         <v>-128</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="11">
-        <v>1</v>
-      </c>
-      <c r="F4" s="13" t="s">
+      <c r="E4" s="47">
+        <v>1</v>
+      </c>
+      <c r="F4" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="48" cm="1">
+        <f t="array" aca="1" ref="G4" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
         <v>-129</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11">
+      <c r="K4" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" t="b">
+        <f>I4=LEFT(H4,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" ref="M4:M26" ca="1" si="0">DEC2BIN(G4,10)</f>
+        <v>1101111111</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" ref="N4:N26" ca="1" si="1">RIGHT(M4,9)</f>
+        <v>101111111</v>
+      </c>
+      <c r="O4" t="b">
+        <f t="shared" ref="O4:O26" ca="1" si="2">N4=H4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="52">
+        <v>3</v>
+      </c>
+      <c r="B5" s="52">
         <v>-128</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="52">
         <v>127</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="53">
+        <f>B5-E5</f>
         <v>-255</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="11">
+      <c r="K5" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" t="b">
+        <f>I5=LEFT(H5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="0"/>
+        <v>1100000001</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="1"/>
+        <v>100000001</v>
+      </c>
+      <c r="O5" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="57">
+        <v>4</v>
+      </c>
+      <c r="B6" s="57">
         <v>-1</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="57">
         <v>-128</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="59" cm="1">
+        <f t="array" aca="1" ref="G6" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
         <v>-129</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11">
-        <v>1</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="K6" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>1101111111</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>101111111</v>
+      </c>
+      <c r="O6" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="62">
+        <v>5</v>
+      </c>
+      <c r="B7" s="62">
+        <v>1</v>
+      </c>
+      <c r="C7" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="62">
         <v>-128</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="63" cm="1">
+        <f t="array" aca="1" ref="G7" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
         <v>129</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11">
-        <v>1</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="K7" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" t="b">
+        <f>I7=LEFT(H7,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0010000001</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>010000001</v>
+      </c>
+      <c r="O7" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="67">
+        <v>6</v>
+      </c>
+      <c r="B8" s="67">
+        <v>1</v>
+      </c>
+      <c r="C8" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="67">
         <v>127</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="69" cm="1">
+        <f t="array" aca="1" ref="G8" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
         <v>128</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="J8" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0010000000</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>010000000</v>
+      </c>
+      <c r="O8" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
       <c r="B9" s="11">
         <v>127</v>
       </c>
-      <c r="C9" s="11">
-        <v>1111111</v>
-      </c>
-      <c r="D9" s="12" t="s">
+      <c r="C9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="11">
         <v>-128</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="12" cm="1">
+        <f t="array" aca="1" ref="G9" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
         <v>255</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="13" t="s">
         <v>2</v>
       </c>
       <c r="J9" s="15" t="s">
@@ -4580,415 +4874,651 @@
       <c r="K9" s="11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11">
+      <c r="L9" t="b">
+        <f t="shared" ref="L9:L10" si="3">I9=LEFT(H9,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0011111111</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>011111111</v>
+      </c>
+      <c r="O9" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>8</v>
+      </c>
+      <c r="B10" s="16">
         <v>127</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="16">
         <v>-1</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="17" cm="1">
+        <f t="array" aca="1" ref="G10" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
         <v>128</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11">
+      <c r="K10" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0010000000</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>010000000</v>
+      </c>
+      <c r="O10" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>9</v>
+      </c>
+      <c r="B11" s="21">
         <v>127</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="11">
-        <v>1</v>
-      </c>
-      <c r="F11" s="13" t="s">
+      <c r="E11" s="21">
+        <v>1</v>
+      </c>
+      <c r="F11" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="22" cm="1">
+        <f t="array" aca="1" ref="G11" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
         <v>128</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16">
+      <c r="K11" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0010000000</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>010000000</v>
+      </c>
+      <c r="O11" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="42">
+        <v>1</v>
+      </c>
+      <c r="B12" s="42">
         <v>-128</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="42">
         <v>-1</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="44" cm="1">
+        <f t="array" aca="1" ref="G12" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
         <v>-127</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="18">
-        <v>0</v>
-      </c>
-      <c r="J12" s="20" t="s">
+      <c r="I12" s="43">
+        <v>0</v>
+      </c>
+      <c r="J12" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="K12" s="42" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
+      <c r="L12" t="b">
+        <f>I12=LEFT(H12,1)</f>
+        <v>0</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>1110000001</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>110000001</v>
+      </c>
+      <c r="O12" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="47">
+        <v>2</v>
+      </c>
+      <c r="B13" s="47">
         <v>-128</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="16">
-        <v>1</v>
-      </c>
-      <c r="F13" s="17" t="s">
+      <c r="E13" s="47">
+        <v>1</v>
+      </c>
+      <c r="F13" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="48" cm="1">
+        <f t="array" aca="1" ref="G13" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
         <v>-127</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="18">
-        <v>0</v>
-      </c>
-      <c r="J13" s="20" t="s">
+      <c r="I13" s="49">
+        <v>0</v>
+      </c>
+      <c r="J13" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="K13" s="47" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
+      <c r="M13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>1110000001</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>110000001</v>
+      </c>
+      <c r="O13" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="52">
+        <v>3</v>
+      </c>
+      <c r="B14" s="52">
         <v>-128</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="52">
         <v>127</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="52">
+        <f>B14+E14</f>
         <v>-1</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="18">
-        <v>0</v>
-      </c>
-      <c r="J14" s="20" t="s">
+      <c r="I14" s="54">
+        <v>0</v>
+      </c>
+      <c r="J14" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="16" t="s">
+      <c r="K14" s="52" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="21">
+      <c r="M14" t="str">
+        <f t="shared" si="0"/>
+        <v>1111111111</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="1"/>
+        <v>111111111</v>
+      </c>
+      <c r="O14" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="57">
+        <v>4</v>
+      </c>
+      <c r="B15" s="57">
         <v>-1</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="57">
         <v>-128</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="59" cm="1">
+        <f t="array" aca="1" ref="G15" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
         <v>127</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="23">
-        <v>1</v>
-      </c>
-      <c r="J15" s="25" t="s">
+      <c r="I15" s="58">
+        <v>1</v>
+      </c>
+      <c r="J15" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="21" t="s">
+      <c r="K15" s="57" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="21">
+      <c r="L15" t="b">
+        <f>I15=LEFT(H15,1)</f>
+        <v>0</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0001111111</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>001111111</v>
+      </c>
+      <c r="O15" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="72">
+        <v>10</v>
+      </c>
+      <c r="B16" s="72">
         <v>-1</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="21">
-        <v>1</v>
-      </c>
-      <c r="F16" s="22" t="s">
+      <c r="E16" s="72">
+        <v>1</v>
+      </c>
+      <c r="F16" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="23">
-        <v>0</v>
-      </c>
-      <c r="H16" s="24" t="s">
+      <c r="G16" s="73" cm="1">
+        <f t="array" aca="1" ref="G16" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="J16" s="25" t="s">
+      <c r="J16" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="K16" s="21" t="s">
+      <c r="K16" s="72" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="21">
+      <c r="M16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0000000000</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>000000000</v>
+      </c>
+      <c r="O16" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="72">
+        <v>10</v>
+      </c>
+      <c r="B17" s="72">
         <v>-1</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="21">
-        <v>1</v>
-      </c>
-      <c r="F17" s="22" t="s">
+      <c r="E17" s="72">
+        <v>1</v>
+      </c>
+      <c r="F17" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="73" cm="1">
+        <f t="array" aca="1" ref="G17" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
         <v>-2</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="23">
-        <v>0</v>
-      </c>
-      <c r="J17" s="25" t="s">
+      <c r="I17" s="74">
+        <v>0</v>
+      </c>
+      <c r="J17" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="K17" s="21" t="s">
+      <c r="K17" s="72" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="21">
+      <c r="L17" t="b">
+        <f>I17=LEFT(H17,1)</f>
+        <v>0</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>1111111110</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>111111110</v>
+      </c>
+      <c r="O17" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="77">
+        <v>11</v>
+      </c>
+      <c r="B18" s="77">
         <v>-1</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="77">
         <v>127</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="77" cm="1">
+        <f t="array" aca="1" ref="G18" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
         <v>126</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="H18" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="23">
-        <v>1</v>
-      </c>
-      <c r="J18" s="25" t="s">
+      <c r="I18" s="79">
+        <v>1</v>
+      </c>
+      <c r="J18" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="21" t="s">
+      <c r="K18" s="77" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="21">
+      <c r="M18" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0001111110</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>001111110</v>
+      </c>
+      <c r="O18" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="77">
+        <v>11</v>
+      </c>
+      <c r="B19" s="77">
         <v>-1</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="77">
         <v>127</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="77" cm="1">
+        <f t="array" aca="1" ref="G19" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
         <v>-128</v>
       </c>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="I19" s="23" t="s">
+      <c r="I19" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="J19" s="25" t="s">
+      <c r="J19" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="21" t="s">
+      <c r="K19" s="77" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="26">
-        <v>1</v>
-      </c>
-      <c r="C20" s="27" t="s">
+      <c r="L19" t="b">
+        <f>I19=LEFT(H19,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>1110000000</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>110000000</v>
+      </c>
+      <c r="O19" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="62">
+        <v>5</v>
+      </c>
+      <c r="B20" s="62">
+        <v>1</v>
+      </c>
+      <c r="C20" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="62">
         <v>-128</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="28">
+      <c r="G20" s="63" cm="1">
+        <f t="array" aca="1" ref="G20" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
         <v>-127</v>
       </c>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="I20" s="28">
-        <v>0</v>
-      </c>
-      <c r="J20" s="30" t="s">
+      <c r="I20" s="64">
+        <v>0</v>
+      </c>
+      <c r="J20" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="K20" s="26" t="s">
+      <c r="K20" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="46"/>
-    </row>
-    <row r="21" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="26">
-        <v>1</v>
-      </c>
-      <c r="C21" s="27" t="s">
+      <c r="L20" s="35"/>
+      <c r="M20" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>1110000001</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>110000001</v>
+      </c>
+      <c r="O20" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="67">
+        <v>6</v>
+      </c>
+      <c r="B21" s="67">
+        <v>1</v>
+      </c>
+      <c r="C21" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="26">
-        <v>-1</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" s="28">
-        <v>2</v>
-      </c>
-      <c r="H21" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="J21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="K21" s="26" t="s">
+      <c r="E21" s="67">
+        <v>127</v>
+      </c>
+      <c r="F21" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="67" cm="1">
+        <f t="array" aca="1" ref="G21" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
+        <v>-126</v>
+      </c>
+      <c r="H21" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="68">
+        <v>0</v>
+      </c>
+      <c r="J21" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="67" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L21" t="b">
+        <f>I21=LEFT(H21,1)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>1110000010</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>110000010</v>
+      </c>
+      <c r="O21" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="26">
+        <v>12</v>
+      </c>
       <c r="B22" s="26">
         <v>1</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="27" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="26">
         <v>-1</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="28">
+      <c r="G22" s="28" cm="1">
+        <f t="array" aca="1" ref="G22" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
         <v>0</v>
       </c>
       <c r="H22" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="28">
+      <c r="I22" s="27">
         <v>1</v>
       </c>
       <c r="J22" s="30" t="s">
@@ -4997,137 +5527,226 @@
       <c r="K22" s="26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M22" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0000000000</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>000000000</v>
+      </c>
+      <c r="O22" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="26">
+        <v>12</v>
+      </c>
       <c r="B23" s="26">
         <v>1</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="27" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="26">
-        <v>127</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="28">
-        <v>-126</v>
+        <v>-1</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="28" cm="1">
+        <f t="array" aca="1" ref="G23" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
+        <v>2</v>
       </c>
       <c r="H23" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="28">
-        <v>0</v>
-      </c>
-      <c r="J23" s="30" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="I23" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="K23" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="46"/>
-    </row>
-    <row r="24" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="31">
+      <c r="L23" t="b">
+        <f>I23=LEFT(H23,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0000000010</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>000000010</v>
+      </c>
+      <c r="O23" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>7</v>
+      </c>
+      <c r="B24" s="11">
         <v>127</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="31">
+      <c r="E24" s="11">
         <v>-128</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="F24" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="12" cm="1">
+        <f t="array" aca="1" ref="G24" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
         <v>-1</v>
       </c>
-      <c r="H24" s="34" t="s">
+      <c r="H24" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="32">
-        <v>0</v>
-      </c>
-      <c r="J24" s="35" t="s">
+      <c r="I24" s="13">
+        <v>0</v>
+      </c>
+      <c r="J24" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="K24" s="31" t="s">
+      <c r="K24" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="31">
+      <c r="M24" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>1111111111</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>111111111</v>
+      </c>
+      <c r="O24" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
+        <v>8</v>
+      </c>
+      <c r="B25" s="16">
         <v>127</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="32" t="s">
+      <c r="D25" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="31">
+      <c r="E25" s="16">
         <v>-1</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="32">
+      <c r="G25" s="17" cm="1">
+        <f t="array" aca="1" ref="G25" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
         <v>126</v>
       </c>
-      <c r="H25" s="34" t="s">
+      <c r="H25" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="I25" s="32">
-        <v>1</v>
-      </c>
-      <c r="J25" s="35" t="s">
+      <c r="I25" s="18">
+        <v>1</v>
+      </c>
+      <c r="J25" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="31" t="s">
+      <c r="K25" s="16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="31">
+      <c r="M25" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0001111110</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>001111110</v>
+      </c>
+      <c r="O25" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
+        <v>9</v>
+      </c>
+      <c r="B26" s="21">
         <v>127</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="31">
-        <v>1</v>
-      </c>
-      <c r="F26" s="33" t="s">
+      <c r="E26" s="21">
+        <v>1</v>
+      </c>
+      <c r="F26" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="32">
+      <c r="G26" s="22" cm="1">
+        <f t="array" aca="1" ref="G26" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
         <v>126</v>
       </c>
-      <c r="H26" s="34" t="s">
+      <c r="H26" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="32">
-        <v>1</v>
-      </c>
-      <c r="J26" s="35" t="s">
+      <c r="I26" s="23">
+        <v>1</v>
+      </c>
+      <c r="J26" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="31" t="s">
+      <c r="K26" s="21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L26" t="b">
+        <f>I26=LEFT(H26,1)</f>
+        <v>0</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0001111110</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>001111110</v>
+      </c>
+      <c r="O26" t="b">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M28" t="str">
+        <f ca="1">DEC2BIN(G12)</f>
+        <v>1110000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -5139,87 +5758,95 @@
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J30" s="36"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J31" s="36"/>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J32" s="36"/>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J30" s="31"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J31" s="31"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J32" s="31"/>
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J33" s="36"/>
+      <c r="J33" s="31"/>
     </row>
     <row r="34" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J34" s="36"/>
+      <c r="J34" s="31"/>
     </row>
     <row r="35" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J35" s="36"/>
+      <c r="J35" s="31"/>
     </row>
     <row r="36" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J36" s="36"/>
+      <c r="J36" s="31"/>
     </row>
     <row r="37" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J37" s="36"/>
+      <c r="J37" s="31"/>
     </row>
     <row r="38" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J38" s="36"/>
+      <c r="J38" s="31"/>
     </row>
     <row r="39" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J39" s="36"/>
+      <c r="J39" s="31"/>
     </row>
     <row r="40" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J40" s="36"/>
+      <c r="J40" s="31"/>
     </row>
     <row r="41" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J41" s="36"/>
+      <c r="J41" s="31"/>
     </row>
     <row r="42" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J42" s="36"/>
+      <c r="J42" s="31"/>
     </row>
     <row r="43" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J43" s="36"/>
+      <c r="J43" s="31"/>
     </row>
     <row r="44" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J44" s="36"/>
+      <c r="J44" s="31"/>
     </row>
     <row r="45" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J45" s="36"/>
+      <c r="J45" s="31"/>
     </row>
     <row r="46" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J46" s="36"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J47" s="36"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J48" s="36"/>
+      <c r="J48" s="31"/>
     </row>
     <row r="49" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J49" s="36"/>
+      <c r="J49" s="31"/>
     </row>
     <row r="50" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J50" s="36"/>
+      <c r="J50" s="31"/>
     </row>
     <row r="51" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J51" s="36"/>
+      <c r="J51" s="31"/>
     </row>
     <row r="52" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J52" s="36"/>
+      <c r="J52" s="31"/>
     </row>
     <row r="53" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J53" s="36"/>
+      <c r="J53" s="31"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:K26">
-    <sortCondition ref="K3:K26"/>
-    <sortCondition ref="B3:B26"/>
+  <autoFilter ref="A2:K26" xr:uid="{CED239D7-98B0-43DB-AD6A-A78832542F2A}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="menos"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K26">
+      <sortCondition ref="K3:K26"/>
+      <sortCondition ref="B3:B26"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K26">
+    <sortCondition ref="A3:A26"/>
+    <sortCondition ref="D3:D26"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="C3:D7 F3:H3 J3 I4:J11 I3 F4:H10 F11:H12 F13:H15 F18:H25 F16:H17 F26:H26 C8:D8 C24:D26 C22:D22 C23:D23 I19:J19 J12 J13:J15 I21:J21 J20 J26 J23 C10:D21 D9 J24 J25 I16 J16:J17 J18 J22" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
3 testes falhando. testesub 4, 5 e 7
falhando testesub 4, 5  e 7
</commit_message>
<xml_diff>
--- a/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
+++ b/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3162c0a97888194f/Documentos/GitHub/algoritmos/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="351" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03E95CE2-9F03-4A94-B9B5-0E1C9EE7B762}"/>
+  <xr:revisionPtr revIDLastSave="883" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{766B64A2-0EB3-4122-9189-45A272610943}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1245" windowWidth="13935" windowHeight="11385" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
+    <workbookView xWindow="1275" yWindow="2580" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="numeros_binarios_8bits" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Tabela_erros_calculadora" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Tabela_erros_calculadora!$A$2:$K$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Tabela_erros_calculadora!$B$2:$L$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,18 +63,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="37">
   <si>
     <t>op</t>
   </si>
   <si>
     <t>erro</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>vai um</t>
@@ -107,82 +101,10 @@
     <t>status</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>00</t>
-  </si>
-  <si>
-    <t>b8b7</t>
-  </si>
-  <si>
-    <t>000000010</t>
-  </si>
-  <si>
-    <t>110000001</t>
-  </si>
-  <si>
-    <t>111111111</t>
-  </si>
-  <si>
-    <t>110000010</t>
-  </si>
-  <si>
-    <t>000000000</t>
-  </si>
-  <si>
-    <t>001111110</t>
-  </si>
-  <si>
-    <t>001111111</t>
-  </si>
-  <si>
-    <t>110000000</t>
-  </si>
-  <si>
-    <t>111111110</t>
-  </si>
-  <si>
-    <t>010000000</t>
-  </si>
-  <si>
-    <t>010000001</t>
-  </si>
-  <si>
-    <t>011111111</t>
-  </si>
-  <si>
-    <t>101111111</t>
-  </si>
-  <si>
-    <t>100000001</t>
-  </si>
-  <si>
-    <t>Valor 1</t>
-  </si>
-  <si>
-    <t>Valor 2</t>
-  </si>
-  <si>
-    <t>operação</t>
-  </si>
-  <si>
-    <t>Resultado</t>
-  </si>
-  <si>
     <t>V1 binário</t>
   </si>
   <si>
     <t>V2 binário</t>
-  </si>
-  <si>
-    <t>Res 9 bits</t>
   </si>
   <si>
     <t>10000000</t>
@@ -221,17 +143,44 @@
     <t>Valores válidos são entre -128 e +127</t>
   </si>
   <si>
-    <t>overflow b9</t>
+    <t>id</t>
   </si>
   <si>
-    <t>id</t>
+    <t>Res 10 bits</t>
+  </si>
+  <si>
+    <t>sinal b10</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>Res</t>
+  </si>
+  <si>
+    <t>overflow b9b8</t>
+  </si>
+  <si>
+    <t>teste</t>
+  </si>
+  <si>
+    <t>char * actual = soma(input1, input2);</t>
+  </si>
+  <si>
+    <t>CuAssertStrEquals (tc, expected, actual);</t>
+  </si>
+  <si>
+    <t>}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,8 +215,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,8 +335,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -456,13 +417,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="dashed">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -497,12 +467,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -512,12 +476,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -527,12 +485,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -540,12 +492,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -556,7 +502,98 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -575,124 +612,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="13" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="15" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="16" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="18" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="19" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1028,14 +957,14 @@
   <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.140625" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.140625" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" style="6" customWidth="1"/>
@@ -1050,7 +979,9 @@
     <col min="15" max="15" width="11.28515625" style="6" customWidth="1"/>
     <col min="16" max="16" width="2.140625" customWidth="1"/>
     <col min="17" max="17" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="9.7109375" customWidth="1"/>
+    <col min="18" max="19" width="9.7109375" customWidth="1"/>
+    <col min="20" max="20" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1073,12 +1004,12 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
-      <c r="B2" s="33">
+      <c r="B2" s="25">
         <v>-129</v>
       </c>
-      <c r="C2" s="34" t="str">
-        <f>RIGHT(DEC2BIN(B2,8),9)</f>
-        <v>101111111</v>
+      <c r="C2" s="56" t="str">
+        <f>RIGHT(DEC2BIN(B2,8),10)</f>
+        <v>1101111111</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2">
@@ -1119,9 +1050,9 @@
       <c r="B3">
         <v>-128</v>
       </c>
-      <c r="C3" s="6" t="str">
-        <f>"0"&amp;RIGHT(DEC2BIN(B3,8),8)</f>
-        <v>010000000</v>
+      <c r="C3" s="57" t="str">
+        <f>RIGHT(DEC2BIN(B3,8),10)</f>
+        <v>1110000000</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3">
@@ -1156,19 +1087,19 @@
         <v>01010100</v>
       </c>
       <c r="P3" s="8"/>
-      <c r="R3" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
+      <c r="R3" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4">
         <v>-127</v>
       </c>
-      <c r="C4" s="6" t="str">
+      <c r="C4" s="58" t="str">
         <f t="shared" ref="C4" si="3">RIGHT(DEC2BIN(B4,8),8)</f>
         <v>10000001</v>
       </c>
@@ -1205,19 +1136,19 @@
         <v>01010101</v>
       </c>
       <c r="P4" s="8"/>
-      <c r="R4" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
+      <c r="R4" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5">
         <v>-126</v>
       </c>
-      <c r="C5" s="6" t="str">
+      <c r="C5" s="58" t="str">
         <f t="shared" ref="C5:C26" si="4">RIGHT(DEC2BIN(B5,8),8)</f>
         <v>10000010</v>
       </c>
@@ -1254,19 +1185,19 @@
         <v>01010110</v>
       </c>
       <c r="P5" s="8"/>
-      <c r="R5" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="S5" s="36"/>
-      <c r="T5" s="36"/>
-      <c r="U5" s="36"/>
+      <c r="R5" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6">
         <v>-125</v>
       </c>
-      <c r="C6" s="6" t="str">
+      <c r="C6" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10000011</v>
       </c>
@@ -1309,7 +1240,7 @@
       <c r="B7">
         <v>-124</v>
       </c>
-      <c r="C7" s="6" t="str">
+      <c r="C7" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10000100</v>
       </c>
@@ -1352,7 +1283,7 @@
       <c r="B8">
         <v>-123</v>
       </c>
-      <c r="C8" s="6" t="str">
+      <c r="C8" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10000101</v>
       </c>
@@ -1395,7 +1326,7 @@
       <c r="B9">
         <v>-122</v>
       </c>
-      <c r="C9" s="6" t="str">
+      <c r="C9" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10000110</v>
       </c>
@@ -1432,13 +1363,20 @@
         <v>01011010</v>
       </c>
       <c r="P9" s="8"/>
+      <c r="S9">
+        <v>-127</v>
+      </c>
+      <c r="T9" t="str">
+        <f>DEC2BIN(S9)</f>
+        <v>1110000001</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10">
         <v>-121</v>
       </c>
-      <c r="C10" s="6" t="str">
+      <c r="C10" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10000111</v>
       </c>
@@ -1475,13 +1413,20 @@
         <v>01011011</v>
       </c>
       <c r="P10" s="8"/>
+      <c r="T10" s="55">
+        <v>1110000000</v>
+      </c>
+      <c r="U10">
+        <f>BIN2DEC(T10)</f>
+        <v>-128</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11">
         <v>-120</v>
       </c>
-      <c r="C11" s="6" t="str">
+      <c r="C11" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10001000</v>
       </c>
@@ -1524,7 +1469,7 @@
       <c r="B12">
         <v>-119</v>
       </c>
-      <c r="C12" s="6" t="str">
+      <c r="C12" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10001001</v>
       </c>
@@ -1567,7 +1512,7 @@
       <c r="B13">
         <v>-118</v>
       </c>
-      <c r="C13" s="6" t="str">
+      <c r="C13" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10001010</v>
       </c>
@@ -1610,7 +1555,7 @@
       <c r="B14">
         <v>-117</v>
       </c>
-      <c r="C14" s="6" t="str">
+      <c r="C14" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10001011</v>
       </c>
@@ -1653,7 +1598,7 @@
       <c r="B15">
         <v>-116</v>
       </c>
-      <c r="C15" s="6" t="str">
+      <c r="C15" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10001100</v>
       </c>
@@ -1696,7 +1641,7 @@
       <c r="B16">
         <v>-115</v>
       </c>
-      <c r="C16" s="6" t="str">
+      <c r="C16" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10001101</v>
       </c>
@@ -1739,7 +1684,7 @@
       <c r="B17">
         <v>-114</v>
       </c>
-      <c r="C17" s="6" t="str">
+      <c r="C17" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10001110</v>
       </c>
@@ -1782,7 +1727,7 @@
       <c r="B18">
         <v>-113</v>
       </c>
-      <c r="C18" s="6" t="str">
+      <c r="C18" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10001111</v>
       </c>
@@ -1825,7 +1770,7 @@
       <c r="B19">
         <v>-112</v>
       </c>
-      <c r="C19" s="6" t="str">
+      <c r="C19" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10010000</v>
       </c>
@@ -1868,7 +1813,7 @@
       <c r="B20">
         <v>-111</v>
       </c>
-      <c r="C20" s="6" t="str">
+      <c r="C20" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10010001</v>
       </c>
@@ -1911,7 +1856,7 @@
       <c r="B21">
         <v>-110</v>
       </c>
-      <c r="C21" s="6" t="str">
+      <c r="C21" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10010010</v>
       </c>
@@ -1954,7 +1899,7 @@
       <c r="B22">
         <v>-109</v>
       </c>
-      <c r="C22" s="6" t="str">
+      <c r="C22" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10010011</v>
       </c>
@@ -1997,7 +1942,7 @@
       <c r="B23">
         <v>-108</v>
       </c>
-      <c r="C23" s="6" t="str">
+      <c r="C23" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10010100</v>
       </c>
@@ -2040,7 +1985,7 @@
       <c r="B24">
         <v>-107</v>
       </c>
-      <c r="C24" s="6" t="str">
+      <c r="C24" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10010101</v>
       </c>
@@ -2083,7 +2028,7 @@
       <c r="B25">
         <v>-106</v>
       </c>
-      <c r="C25" s="6" t="str">
+      <c r="C25" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10010110</v>
       </c>
@@ -2126,7 +2071,7 @@
       <c r="B26">
         <v>-105</v>
       </c>
-      <c r="C26" s="6" t="str">
+      <c r="C26" s="58" t="str">
         <f t="shared" si="4"/>
         <v>10010111</v>
       </c>
@@ -2169,7 +2114,7 @@
       <c r="B27">
         <v>-104</v>
       </c>
-      <c r="C27" s="6" t="str">
+      <c r="C27" s="58" t="str">
         <f t="shared" ref="C27:C54" si="6">RIGHT(DEC2BIN(B27,8),8)</f>
         <v>10011000</v>
       </c>
@@ -2212,7 +2157,7 @@
       <c r="B28">
         <v>-103</v>
       </c>
-      <c r="C28" s="6" t="str">
+      <c r="C28" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10011001</v>
       </c>
@@ -2255,7 +2200,7 @@
       <c r="B29">
         <v>-102</v>
       </c>
-      <c r="C29" s="6" t="str">
+      <c r="C29" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10011010</v>
       </c>
@@ -2298,7 +2243,7 @@
       <c r="B30">
         <v>-101</v>
       </c>
-      <c r="C30" s="6" t="str">
+      <c r="C30" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10011011</v>
       </c>
@@ -2341,7 +2286,7 @@
       <c r="B31">
         <v>-100</v>
       </c>
-      <c r="C31" s="6" t="str">
+      <c r="C31" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10011100</v>
       </c>
@@ -2384,7 +2329,7 @@
       <c r="B32">
         <v>-99</v>
       </c>
-      <c r="C32" s="6" t="str">
+      <c r="C32" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10011101</v>
       </c>
@@ -2427,7 +2372,7 @@
       <c r="B33">
         <v>-98</v>
       </c>
-      <c r="C33" s="6" t="str">
+      <c r="C33" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10011110</v>
       </c>
@@ -2470,7 +2415,7 @@
       <c r="B34">
         <v>-97</v>
       </c>
-      <c r="C34" s="6" t="str">
+      <c r="C34" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10011111</v>
       </c>
@@ -2513,7 +2458,7 @@
       <c r="B35">
         <v>-96</v>
       </c>
-      <c r="C35" s="6" t="str">
+      <c r="C35" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10100000</v>
       </c>
@@ -2556,7 +2501,7 @@
       <c r="B36">
         <v>-95</v>
       </c>
-      <c r="C36" s="6" t="str">
+      <c r="C36" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10100001</v>
       </c>
@@ -2599,7 +2544,7 @@
       <c r="B37">
         <v>-94</v>
       </c>
-      <c r="C37" s="6" t="str">
+      <c r="C37" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10100010</v>
       </c>
@@ -2642,7 +2587,7 @@
       <c r="B38">
         <v>-93</v>
       </c>
-      <c r="C38" s="6" t="str">
+      <c r="C38" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10100011</v>
       </c>
@@ -2685,7 +2630,7 @@
       <c r="B39">
         <v>-92</v>
       </c>
-      <c r="C39" s="6" t="str">
+      <c r="C39" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10100100</v>
       </c>
@@ -2728,7 +2673,7 @@
       <c r="B40">
         <v>-91</v>
       </c>
-      <c r="C40" s="6" t="str">
+      <c r="C40" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10100101</v>
       </c>
@@ -2771,7 +2716,7 @@
       <c r="B41">
         <v>-90</v>
       </c>
-      <c r="C41" s="6" t="str">
+      <c r="C41" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10100110</v>
       </c>
@@ -2814,7 +2759,7 @@
       <c r="B42">
         <v>-89</v>
       </c>
-      <c r="C42" s="6" t="str">
+      <c r="C42" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10100111</v>
       </c>
@@ -2857,7 +2802,7 @@
       <c r="B43">
         <v>-88</v>
       </c>
-      <c r="C43" s="6" t="str">
+      <c r="C43" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10101000</v>
       </c>
@@ -2900,7 +2845,7 @@
       <c r="B44">
         <v>-87</v>
       </c>
-      <c r="C44" s="6" t="str">
+      <c r="C44" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10101001</v>
       </c>
@@ -2943,7 +2888,7 @@
       <c r="B45">
         <v>-86</v>
       </c>
-      <c r="C45" s="6" t="str">
+      <c r="C45" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10101010</v>
       </c>
@@ -2986,7 +2931,7 @@
       <c r="B46">
         <v>-85</v>
       </c>
-      <c r="C46" s="6" t="str">
+      <c r="C46" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10101011</v>
       </c>
@@ -3029,7 +2974,7 @@
       <c r="B47">
         <v>-84</v>
       </c>
-      <c r="C47" s="6" t="str">
+      <c r="C47" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10101100</v>
       </c>
@@ -3058,10 +3003,10 @@
         <v>01001000</v>
       </c>
       <c r="M47" s="8"/>
-      <c r="N47" s="33">
+      <c r="N47" s="25">
         <v>128</v>
       </c>
-      <c r="O47" s="34" t="str">
+      <c r="O47" s="26" t="str">
         <f>"0"&amp;DEC2BIN(N47,8)</f>
         <v>010000000</v>
       </c>
@@ -3072,7 +3017,7 @@
       <c r="B48">
         <v>-83</v>
       </c>
-      <c r="C48" s="6" t="str">
+      <c r="C48" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10101101</v>
       </c>
@@ -3101,10 +3046,10 @@
         <v>01001001</v>
       </c>
       <c r="M48" s="8"/>
-      <c r="N48" s="33">
+      <c r="N48" s="25">
         <v>129</v>
       </c>
-      <c r="O48" s="34" t="str">
+      <c r="O48" s="26" t="str">
         <f t="shared" ref="O48:O54" si="11">DEC2BIN(N48,8)</f>
         <v>10000001</v>
       </c>
@@ -3115,7 +3060,7 @@
       <c r="B49">
         <v>-82</v>
       </c>
-      <c r="C49" s="6" t="str">
+      <c r="C49" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10101110</v>
       </c>
@@ -3144,10 +3089,10 @@
         <v>01001010</v>
       </c>
       <c r="M49" s="8"/>
-      <c r="N49" s="33">
+      <c r="N49" s="25">
         <v>130</v>
       </c>
-      <c r="O49" s="34" t="str">
+      <c r="O49" s="26" t="str">
         <f t="shared" si="11"/>
         <v>10000010</v>
       </c>
@@ -3158,7 +3103,7 @@
       <c r="B50">
         <v>-81</v>
       </c>
-      <c r="C50" s="6" t="str">
+      <c r="C50" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10101111</v>
       </c>
@@ -3187,10 +3132,10 @@
         <v>01001011</v>
       </c>
       <c r="M50" s="8"/>
-      <c r="N50" s="33">
+      <c r="N50" s="25">
         <v>131</v>
       </c>
-      <c r="O50" s="34" t="str">
+      <c r="O50" s="26" t="str">
         <f t="shared" si="11"/>
         <v>10000011</v>
       </c>
@@ -3201,7 +3146,7 @@
       <c r="B51">
         <v>-80</v>
       </c>
-      <c r="C51" s="6" t="str">
+      <c r="C51" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10110000</v>
       </c>
@@ -3230,10 +3175,10 @@
         <v>01001100</v>
       </c>
       <c r="M51" s="8"/>
-      <c r="N51" s="33">
+      <c r="N51" s="25">
         <v>132</v>
       </c>
-      <c r="O51" s="34" t="str">
+      <c r="O51" s="26" t="str">
         <f t="shared" si="11"/>
         <v>10000100</v>
       </c>
@@ -3244,7 +3189,7 @@
       <c r="B52">
         <v>-79</v>
       </c>
-      <c r="C52" s="6" t="str">
+      <c r="C52" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10110001</v>
       </c>
@@ -3273,10 +3218,10 @@
         <v>01001101</v>
       </c>
       <c r="M52" s="8"/>
-      <c r="N52" s="33">
+      <c r="N52" s="25">
         <v>133</v>
       </c>
-      <c r="O52" s="34" t="str">
+      <c r="O52" s="26" t="str">
         <f t="shared" si="11"/>
         <v>10000101</v>
       </c>
@@ -3287,7 +3232,7 @@
       <c r="B53">
         <v>-78</v>
       </c>
-      <c r="C53" s="6" t="str">
+      <c r="C53" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10110010</v>
       </c>
@@ -3316,10 +3261,10 @@
         <v>01001110</v>
       </c>
       <c r="M53" s="8"/>
-      <c r="N53" s="33">
+      <c r="N53" s="25">
         <v>134</v>
       </c>
-      <c r="O53" s="34" t="str">
+      <c r="O53" s="26" t="str">
         <f t="shared" si="11"/>
         <v>10000110</v>
       </c>
@@ -3330,7 +3275,7 @@
       <c r="B54">
         <v>-77</v>
       </c>
-      <c r="C54" s="6" t="str">
+      <c r="C54" s="58" t="str">
         <f t="shared" si="6"/>
         <v>10110011</v>
       </c>
@@ -3359,10 +3304,10 @@
         <v>01001111</v>
       </c>
       <c r="M54" s="8"/>
-      <c r="N54" s="33">
+      <c r="N54" s="25">
         <v>135</v>
       </c>
-      <c r="O54" s="34" t="str">
+      <c r="O54" s="26" t="str">
         <f t="shared" si="11"/>
         <v>10000111</v>
       </c>
@@ -3411,90 +3356,90 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
+      <c r="A1" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="60"/>
+      <c r="T1" s="60"/>
+      <c r="U1" s="60"/>
     </row>
     <row r="3" spans="1:22" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="32" t="s">
+      <c r="A3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="24">
+        <v>6</v>
+      </c>
+      <c r="E3" s="24">
+        <v>5</v>
+      </c>
+      <c r="F3" s="24">
         <v>4</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="32">
+      <c r="G3" s="24">
+        <v>3</v>
+      </c>
+      <c r="H3" s="24">
+        <v>2</v>
+      </c>
+      <c r="I3" s="24">
+        <v>1</v>
+      </c>
+      <c r="J3" s="24">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="24">
         <v>6</v>
       </c>
-      <c r="E3" s="32">
+      <c r="P3" s="24">
         <v>5</v>
       </c>
-      <c r="F3" s="32">
+      <c r="Q3" s="24">
         <v>4</v>
       </c>
-      <c r="G3" s="32">
+      <c r="R3" s="24">
         <v>3</v>
       </c>
-      <c r="H3" s="32">
+      <c r="S3" s="24">
         <v>2</v>
       </c>
-      <c r="I3" s="32">
-        <v>1</v>
-      </c>
-      <c r="J3" s="32">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="N3" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="O3" s="32">
-        <v>6</v>
-      </c>
-      <c r="P3" s="32">
-        <v>5</v>
-      </c>
-      <c r="Q3" s="32">
-        <v>4</v>
-      </c>
-      <c r="R3" s="32">
-        <v>3</v>
-      </c>
-      <c r="S3" s="32">
-        <v>2</v>
-      </c>
-      <c r="T3" s="32">
-        <v>1</v>
-      </c>
-      <c r="U3" s="32">
+      <c r="T3" s="24">
+        <v>1</v>
+      </c>
+      <c r="U3" s="24">
         <v>0</v>
       </c>
     </row>
@@ -3530,7 +3475,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="4"/>
       <c r="M4" s="1" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="N4" s="1">
         <v>1</v>
@@ -3589,7 +3534,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="4"/>
       <c r="M5" s="1" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="N5" s="1">
         <v>0</v>
@@ -3686,7 +3631,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="2"/>
       <c r="L7" s="4" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="M7" s="1">
         <v>0</v>
@@ -3758,31 +3703,31 @@
       </c>
     </row>
     <row r="9" spans="1:22" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
+      <c r="A9" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="40"/>
-      <c r="S9" s="40"/>
-      <c r="T9" s="40"/>
-      <c r="U9" s="41"/>
+      <c r="L9" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="64"/>
       <c r="V9" s="3"/>
     </row>
     <row r="10" spans="1:22" ht="21" x14ac:dyDescent="0.35">
@@ -3809,65 +3754,65 @@
       <c r="U10" s="5"/>
     </row>
     <row r="11" spans="1:22" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="32" t="s">
+      <c r="A11" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="24">
+        <v>6</v>
+      </c>
+      <c r="E11" s="24">
+        <v>5</v>
+      </c>
+      <c r="F11" s="24">
         <v>4</v>
       </c>
-      <c r="C11" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="32">
+      <c r="G11" s="24">
+        <v>3</v>
+      </c>
+      <c r="H11" s="24">
+        <v>2</v>
+      </c>
+      <c r="I11" s="24">
+        <v>1</v>
+      </c>
+      <c r="J11" s="24">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="24">
         <v>6</v>
       </c>
-      <c r="E11" s="32">
+      <c r="P11" s="24">
         <v>5</v>
       </c>
-      <c r="F11" s="32">
+      <c r="Q11" s="24">
         <v>4</v>
       </c>
-      <c r="G11" s="32">
+      <c r="R11" s="24">
         <v>3</v>
       </c>
-      <c r="H11" s="32">
+      <c r="S11" s="24">
         <v>2</v>
       </c>
-      <c r="I11" s="32">
-        <v>1</v>
-      </c>
-      <c r="J11" s="32">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="M11" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="N11" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="O11" s="32">
-        <v>6</v>
-      </c>
-      <c r="P11" s="32">
-        <v>5</v>
-      </c>
-      <c r="Q11" s="32">
-        <v>4</v>
-      </c>
-      <c r="R11" s="32">
-        <v>3</v>
-      </c>
-      <c r="S11" s="32">
-        <v>2</v>
-      </c>
-      <c r="T11" s="32">
-        <v>1</v>
-      </c>
-      <c r="U11" s="32">
+      <c r="T11" s="24">
+        <v>1</v>
+      </c>
+      <c r="U11" s="24">
         <v>0</v>
       </c>
     </row>
@@ -3987,29 +3932,29 @@
       <c r="U16" s="1"/>
     </row>
     <row r="17" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="41"/>
+      <c r="A17" s="62"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="64"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="M17" s="40"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="40"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="40"/>
-      <c r="S17" s="40"/>
-      <c r="T17" s="40"/>
-      <c r="U17" s="41"/>
+      <c r="L17" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="M17" s="63"/>
+      <c r="N17" s="63"/>
+      <c r="O17" s="63"/>
+      <c r="P17" s="63"/>
+      <c r="Q17" s="63"/>
+      <c r="R17" s="63"/>
+      <c r="S17" s="63"/>
+      <c r="T17" s="63"/>
+      <c r="U17" s="64"/>
     </row>
     <row r="18" spans="1:21" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
@@ -4035,65 +3980,65 @@
       <c r="U18" s="5"/>
     </row>
     <row r="19" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="32" t="s">
+      <c r="A19" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="24">
+        <v>6</v>
+      </c>
+      <c r="E19" s="24">
+        <v>5</v>
+      </c>
+      <c r="F19" s="24">
         <v>4</v>
       </c>
-      <c r="C19" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="32">
+      <c r="G19" s="24">
+        <v>3</v>
+      </c>
+      <c r="H19" s="24">
+        <v>2</v>
+      </c>
+      <c r="I19" s="24">
+        <v>1</v>
+      </c>
+      <c r="J19" s="24">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="O19" s="24">
         <v>6</v>
       </c>
-      <c r="E19" s="32">
+      <c r="P19" s="24">
         <v>5</v>
       </c>
-      <c r="F19" s="32">
+      <c r="Q19" s="24">
         <v>4</v>
       </c>
-      <c r="G19" s="32">
+      <c r="R19" s="24">
         <v>3</v>
       </c>
-      <c r="H19" s="32">
+      <c r="S19" s="24">
         <v>2</v>
       </c>
-      <c r="I19" s="32">
-        <v>1</v>
-      </c>
-      <c r="J19" s="32">
-        <v>0</v>
-      </c>
-      <c r="K19" s="2"/>
-      <c r="L19" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="M19" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="N19" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="O19" s="32">
-        <v>6</v>
-      </c>
-      <c r="P19" s="32">
-        <v>5</v>
-      </c>
-      <c r="Q19" s="32">
-        <v>4</v>
-      </c>
-      <c r="R19" s="32">
-        <v>3</v>
-      </c>
-      <c r="S19" s="32">
-        <v>2</v>
-      </c>
-      <c r="T19" s="32">
-        <v>1</v>
-      </c>
-      <c r="U19" s="32">
+      <c r="T19" s="24">
+        <v>1</v>
+      </c>
+      <c r="U19" s="24">
         <v>0</v>
       </c>
     </row>
@@ -4213,31 +4158,31 @@
       <c r="U24" s="1"/>
     </row>
     <row r="25" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="41"/>
+      <c r="A25" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="63"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="64"/>
       <c r="K25" s="2"/>
-      <c r="L25" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="M25" s="40"/>
-      <c r="N25" s="40"/>
-      <c r="O25" s="40"/>
-      <c r="P25" s="40"/>
-      <c r="Q25" s="40"/>
-      <c r="R25" s="40"/>
-      <c r="S25" s="40"/>
-      <c r="T25" s="40"/>
-      <c r="U25" s="41"/>
+      <c r="L25" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25" s="63"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="63"/>
+      <c r="P25" s="63"/>
+      <c r="Q25" s="63"/>
+      <c r="R25" s="63"/>
+      <c r="S25" s="63"/>
+      <c r="T25" s="63"/>
+      <c r="U25" s="64"/>
     </row>
     <row r="26" spans="1:21" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
@@ -4263,65 +4208,65 @@
       <c r="U26" s="5"/>
     </row>
     <row r="27" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="32" t="s">
+      <c r="A27" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="24">
+        <v>6</v>
+      </c>
+      <c r="E27" s="24">
+        <v>5</v>
+      </c>
+      <c r="F27" s="24">
         <v>4</v>
       </c>
-      <c r="C27" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="32">
+      <c r="G27" s="24">
+        <v>3</v>
+      </c>
+      <c r="H27" s="24">
+        <v>2</v>
+      </c>
+      <c r="I27" s="24">
+        <v>1</v>
+      </c>
+      <c r="J27" s="24">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2"/>
+      <c r="L27" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M27" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N27" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="O27" s="24">
         <v>6</v>
       </c>
-      <c r="E27" s="32">
+      <c r="P27" s="24">
         <v>5</v>
       </c>
-      <c r="F27" s="32">
+      <c r="Q27" s="24">
         <v>4</v>
       </c>
-      <c r="G27" s="32">
+      <c r="R27" s="24">
         <v>3</v>
       </c>
-      <c r="H27" s="32">
+      <c r="S27" s="24">
         <v>2</v>
       </c>
-      <c r="I27" s="32">
-        <v>1</v>
-      </c>
-      <c r="J27" s="32">
-        <v>0</v>
-      </c>
-      <c r="K27" s="2"/>
-      <c r="L27" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="M27" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="N27" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="O27" s="32">
-        <v>6</v>
-      </c>
-      <c r="P27" s="32">
-        <v>5</v>
-      </c>
-      <c r="Q27" s="32">
-        <v>4</v>
-      </c>
-      <c r="R27" s="32">
-        <v>3</v>
-      </c>
-      <c r="S27" s="32">
-        <v>2</v>
-      </c>
-      <c r="T27" s="32">
-        <v>1</v>
-      </c>
-      <c r="U27" s="32">
+      <c r="T27" s="24">
+        <v>1</v>
+      </c>
+      <c r="U27" s="24">
         <v>0</v>
       </c>
     </row>
@@ -4441,29 +4386,29 @@
       <c r="U32" s="1"/>
     </row>
     <row r="33" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="41"/>
+      <c r="A33" s="62"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="64"/>
       <c r="K33" s="2"/>
-      <c r="L33" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="M33" s="40"/>
-      <c r="N33" s="40"/>
-      <c r="O33" s="40"/>
-      <c r="P33" s="40"/>
-      <c r="Q33" s="40"/>
-      <c r="R33" s="40"/>
-      <c r="S33" s="40"/>
-      <c r="T33" s="40"/>
-      <c r="U33" s="41"/>
+      <c r="L33" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="M33" s="63"/>
+      <c r="N33" s="63"/>
+      <c r="O33" s="63"/>
+      <c r="P33" s="63"/>
+      <c r="Q33" s="63"/>
+      <c r="R33" s="63"/>
+      <c r="S33" s="63"/>
+      <c r="T33" s="63"/>
+      <c r="U33" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4484,1368 +4429,1399 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED239D7-98B0-43DB-AD6A-A78832542F2A}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A2:O53"/>
+  <dimension ref="A2:M59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="6" customWidth="1"/>
-    <col min="5" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="J2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="27">
+        <v>1</v>
+      </c>
+      <c r="B3" s="27">
+        <v>1</v>
+      </c>
+      <c r="C3" s="27">
+        <v>-128</v>
+      </c>
+      <c r="D3" s="27">
+        <v>10000000</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="27">
+        <v>-1</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="29">
+        <v>-129</v>
+      </c>
+      <c r="I3" s="27" t="str">
+        <f>DEC2BIN(H3,10)</f>
+        <v>1101111111</v>
+      </c>
+      <c r="J3" s="27" t="str">
+        <f t="shared" ref="J3:J26" si="0">MID(I3,1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="27" t="str">
+        <f t="shared" ref="K3:K26" si="1">MID(I3,2,2)</f>
+        <v>10</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27">
+        <v>2</v>
+      </c>
+      <c r="B4" s="27">
+        <v>1</v>
+      </c>
+      <c r="C4" s="27">
+        <v>-128</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="27">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="29">
+        <v>-127</v>
+      </c>
+      <c r="I4" s="27" t="str">
+        <f t="shared" ref="I4:I26" si="2">DEC2BIN(H4,10)</f>
+        <v>1110000001</v>
+      </c>
+      <c r="J4" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K4" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30">
+        <v>3</v>
+      </c>
+      <c r="B5" s="30">
+        <v>2</v>
+      </c>
+      <c r="C5" s="30">
+        <v>-128</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="30">
+        <v>1</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="31">
+        <v>-127</v>
+      </c>
+      <c r="I5" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v>1110000001</v>
+      </c>
+      <c r="J5" s="30" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30">
+        <v>4</v>
+      </c>
+      <c r="B6" s="30">
+        <v>2</v>
+      </c>
+      <c r="C6" s="30">
+        <v>-128</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="30">
+        <v>1</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="31">
+        <v>-129</v>
+      </c>
+      <c r="I6" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v>1101111111</v>
+      </c>
+      <c r="J6" s="30" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="30" t="str">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L6" s="30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33">
+        <v>5</v>
+      </c>
+      <c r="B7" s="33">
+        <v>3</v>
+      </c>
+      <c r="C7" s="33">
+        <v>-128</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="33">
+        <v>127</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="33">
+        <v>-1</v>
+      </c>
+      <c r="I7" s="33" t="str">
+        <f t="shared" si="2"/>
+        <v>1111111111</v>
+      </c>
+      <c r="J7" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K7" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="L7" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33">
+        <v>6</v>
+      </c>
+      <c r="B8" s="33">
+        <v>3</v>
+      </c>
+      <c r="C8" s="33">
+        <v>-128</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="33">
+        <v>127</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="34">
+        <v>-255</v>
+      </c>
+      <c r="I8" s="33" t="str">
+        <f t="shared" si="2"/>
+        <v>1100000001</v>
+      </c>
+      <c r="J8" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="33" t="str">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L8" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="36">
+        <v>7</v>
+      </c>
+      <c r="B9" s="36">
+        <v>4</v>
+      </c>
+      <c r="C9" s="36">
+        <v>-1</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="36">
+        <v>-128</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="38">
+        <v>-129</v>
+      </c>
+      <c r="I9" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v>1101111111</v>
+      </c>
+      <c r="J9" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="36" t="str">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L9" s="36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="52">
+        <v>8</v>
+      </c>
+      <c r="B10" s="52">
+        <v>4</v>
+      </c>
+      <c r="C10" s="52">
+        <v>-1</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="52">
+        <v>-128</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="54">
+        <v>127</v>
+      </c>
+      <c r="I10" s="52" t="str">
+        <f t="shared" si="2"/>
+        <v>0001111111</v>
+      </c>
+      <c r="J10" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L10" s="52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="39">
+        <v>9</v>
+      </c>
+      <c r="B11" s="39">
+        <v>5</v>
+      </c>
+      <c r="C11" s="39">
+        <v>1</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="39">
+        <v>-128</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="40">
+        <v>-127</v>
+      </c>
+      <c r="I11" s="39" t="str">
+        <f t="shared" si="2"/>
+        <v>1110000001</v>
+      </c>
+      <c r="J11" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K11" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="L11" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="66"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="39">
+        <v>10</v>
+      </c>
+      <c r="B12" s="39">
+        <v>5</v>
+      </c>
+      <c r="C12" s="39">
+        <v>1</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="39">
+        <v>-128</v>
+      </c>
+      <c r="G12" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="40">
+        <v>129</v>
+      </c>
+      <c r="I12" s="39" t="str">
+        <f t="shared" si="2"/>
+        <v>0010000001</v>
+      </c>
+      <c r="J12" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="L12" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="66"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="42">
+        <v>11</v>
+      </c>
+      <c r="B13" s="42">
+        <v>6</v>
+      </c>
+      <c r="C13" s="42">
+        <v>1</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="42">
+        <v>127</v>
+      </c>
+      <c r="G13" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="44">
+        <v>128</v>
+      </c>
+      <c r="I13" s="42" t="str">
+        <f t="shared" si="2"/>
+        <v>0010000000</v>
+      </c>
+      <c r="J13" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="42" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="L13" s="42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="42">
+        <v>12</v>
+      </c>
+      <c r="B14" s="42">
+        <v>6</v>
+      </c>
+      <c r="C14" s="42">
+        <v>1</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="42">
+        <v>127</v>
+      </c>
+      <c r="G14" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="42">
+        <v>-126</v>
+      </c>
+      <c r="I14" s="42" t="str">
+        <f t="shared" si="2"/>
+        <v>1110000010</v>
+      </c>
+      <c r="J14" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K14" s="42" t="str">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="L14" s="42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>13</v>
+      </c>
+      <c r="B15" s="11">
+        <v>7</v>
+      </c>
+      <c r="C15" s="11">
+        <v>127</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="11">
+        <v>-128</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="12">
+        <v>-1</v>
+      </c>
+      <c r="I15" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>1111111111</v>
+      </c>
+      <c r="J15" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K15" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>14</v>
+      </c>
+      <c r="B16" s="11">
+        <v>7</v>
+      </c>
+      <c r="C16" s="11">
+        <v>127</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="11">
+        <v>-128</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="12">
+        <v>255</v>
+      </c>
+      <c r="I16" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>0011111111</v>
+      </c>
+      <c r="J16" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>15</v>
+      </c>
+      <c r="B17" s="14">
+        <v>8</v>
+      </c>
+      <c r="C17" s="14">
+        <v>127</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="15">
+        <v>126</v>
+      </c>
+      <c r="I17" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>0001111110</v>
+      </c>
+      <c r="J17" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>16</v>
+      </c>
+      <c r="B18" s="14">
+        <v>8</v>
+      </c>
+      <c r="C18" s="14">
+        <v>127</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="14">
+        <v>-1</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="15">
+        <v>128</v>
+      </c>
+      <c r="I18" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>0010000000</v>
+      </c>
+      <c r="J18" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>17</v>
+      </c>
+      <c r="B19" s="17">
+        <v>9</v>
+      </c>
+      <c r="C19" s="17">
+        <v>127</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="17">
+        <v>1</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="18">
+        <v>128</v>
+      </c>
+      <c r="I19" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>0010000000</v>
+      </c>
+      <c r="J19" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
         <v>18</v>
       </c>
-      <c r="K2" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42">
-        <v>1</v>
-      </c>
-      <c r="B3" s="42">
+      <c r="B20" s="17">
+        <v>9</v>
+      </c>
+      <c r="C20" s="17">
+        <v>127</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="17">
+        <v>1</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="18">
+        <v>126</v>
+      </c>
+      <c r="I20" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>0001111110</v>
+      </c>
+      <c r="J20" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="45">
+        <v>19</v>
+      </c>
+      <c r="B21" s="45">
+        <v>10</v>
+      </c>
+      <c r="C21" s="45">
+        <v>-1</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="45">
+        <v>1</v>
+      </c>
+      <c r="G21" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="46">
+        <v>0</v>
+      </c>
+      <c r="I21" s="45" t="str">
+        <f t="shared" si="2"/>
+        <v>0000000000</v>
+      </c>
+      <c r="J21" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L21" s="45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="45">
+        <v>20</v>
+      </c>
+      <c r="B22" s="45">
+        <v>10</v>
+      </c>
+      <c r="C22" s="45">
+        <v>-1</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="45">
+        <v>1</v>
+      </c>
+      <c r="G22" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="46">
+        <v>-2</v>
+      </c>
+      <c r="I22" s="45" t="str">
+        <f t="shared" si="2"/>
+        <v>1111111110</v>
+      </c>
+      <c r="J22" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K22" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="L22" s="45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="48">
+        <v>21</v>
+      </c>
+      <c r="B23" s="48">
+        <v>11</v>
+      </c>
+      <c r="C23" s="48">
+        <v>-1</v>
+      </c>
+      <c r="D23" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="48">
+        <v>127</v>
+      </c>
+      <c r="G23" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="48">
+        <v>126</v>
+      </c>
+      <c r="I23" s="48" t="str">
+        <f t="shared" si="2"/>
+        <v>0001111110</v>
+      </c>
+      <c r="J23" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="48" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L23" s="48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="48">
+        <v>22</v>
+      </c>
+      <c r="B24" s="48">
+        <v>11</v>
+      </c>
+      <c r="C24" s="48">
+        <v>-1</v>
+      </c>
+      <c r="D24" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="48">
+        <v>127</v>
+      </c>
+      <c r="G24" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="48">
         <v>-128</v>
       </c>
-      <c r="C3" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="43" t="s">
+      <c r="I24" s="48" t="str">
+        <f t="shared" si="2"/>
+        <v>1110000000</v>
+      </c>
+      <c r="J24" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K24" s="48" t="str">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="L24" s="48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="20">
+        <v>23</v>
+      </c>
+      <c r="B25" s="20">
         <v>12</v>
       </c>
-      <c r="E3" s="42">
+      <c r="C25" s="20">
+        <v>1</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="20">
         <v>-1</v>
       </c>
-      <c r="F3" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="44" cm="1">
-        <f t="array" aca="1" ref="G3" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
-        <v>-129</v>
-      </c>
-      <c r="H3" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="43" t="s">
+      <c r="G25" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="22">
+        <v>0</v>
+      </c>
+      <c r="I25" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>0000000000</v>
+      </c>
+      <c r="J25" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L25" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20">
+        <v>24</v>
+      </c>
+      <c r="B26" s="20">
+        <v>12</v>
+      </c>
+      <c r="C26" s="20">
+        <v>1</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="20">
+        <v>-1</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="22">
+        <v>2</v>
+      </c>
+      <c r="I26" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>0000000010</v>
+      </c>
+      <c r="J26" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L26" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="67" t="str" cm="1">
+        <f t="array" aca="1" ref="A28" ca="1">"void TesteSoma"&amp;INDIRECT("A"&amp;K28+2)&amp;"(CuTest *tc){"</f>
+        <v>void TesteSoma3(CuTest *tc){</v>
+      </c>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="K28" s="51">
         <v>3</v>
       </c>
-      <c r="J3" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" t="str">
-        <f ca="1">DEC2BIN(G3,10)</f>
-        <v>1101111111</v>
-      </c>
-      <c r="N3" t="str">
-        <f ca="1">RIGHT(M3,9)</f>
-        <v>101111111</v>
-      </c>
-      <c r="O3" t="b">
-        <f ca="1">N3=H3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47">
-        <v>2</v>
-      </c>
-      <c r="B4" s="47">
-        <v>-128</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="47">
-        <v>1</v>
-      </c>
-      <c r="F4" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="48" cm="1">
-        <f t="array" aca="1" ref="G4" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
-        <v>-129</v>
-      </c>
-      <c r="H4" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="49" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" t="b">
-        <f>I4=LEFT(H4,1)</f>
-        <v>1</v>
-      </c>
-      <c r="M4" t="str">
-        <f t="shared" ref="M4:M26" ca="1" si="0">DEC2BIN(G4,10)</f>
-        <v>1101111111</v>
-      </c>
-      <c r="N4" t="str">
-        <f t="shared" ref="N4:N26" ca="1" si="1">RIGHT(M4,9)</f>
-        <v>101111111</v>
-      </c>
-      <c r="O4" t="b">
-        <f t="shared" ref="O4:O26" ca="1" si="2">N4=H4</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52">
-        <v>3</v>
-      </c>
-      <c r="B5" s="52">
-        <v>-128</v>
-      </c>
-      <c r="C5" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="54" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="52">
-        <v>127</v>
-      </c>
-      <c r="F5" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="53">
-        <f>B5-E5</f>
-        <v>-255</v>
-      </c>
-      <c r="H5" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" t="b">
-        <f>I5=LEFT(H5,1)</f>
-        <v>1</v>
-      </c>
-      <c r="M5" t="str">
-        <f t="shared" si="0"/>
-        <v>1100000001</v>
-      </c>
-      <c r="N5" t="str">
-        <f t="shared" si="1"/>
-        <v>100000001</v>
-      </c>
-      <c r="O5" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57">
-        <v>4</v>
-      </c>
-      <c r="B6" s="57">
-        <v>-1</v>
-      </c>
-      <c r="C6" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="57">
-        <v>-128</v>
-      </c>
-      <c r="F6" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="59" cm="1">
-        <f t="array" aca="1" ref="G6" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
-        <v>-129</v>
-      </c>
-      <c r="H6" s="60" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="58" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6" s="61" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>1101111111</v>
-      </c>
-      <c r="N6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>101111111</v>
-      </c>
-      <c r="O6" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="62">
-        <v>5</v>
-      </c>
-      <c r="B7" s="62">
-        <v>1</v>
-      </c>
-      <c r="C7" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="62">
-        <v>-128</v>
-      </c>
-      <c r="F7" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="63" cm="1">
-        <f t="array" aca="1" ref="G7" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
-        <v>129</v>
-      </c>
-      <c r="H7" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="66" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" t="b">
-        <f>I7=LEFT(H7,1)</f>
-        <v>1</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>0010000001</v>
-      </c>
-      <c r="N7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>010000001</v>
-      </c>
-      <c r="O7" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="67">
-        <v>6</v>
-      </c>
-      <c r="B8" s="67">
-        <v>1</v>
-      </c>
-      <c r="C8" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="68" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="67">
-        <v>127</v>
-      </c>
-      <c r="F8" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="69" cm="1">
-        <f t="array" aca="1" ref="G8" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
-        <v>128</v>
-      </c>
-      <c r="H8" s="70" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="71" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="M8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>0010000000</v>
-      </c>
-      <c r="N8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>010000000</v>
-      </c>
-      <c r="O8" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
-        <v>7</v>
-      </c>
-      <c r="B9" s="11">
-        <v>127</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="11">
-        <v>-128</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="12" cm="1">
-        <f t="array" aca="1" ref="G9" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
-        <v>255</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" t="b">
-        <f t="shared" ref="L9:L10" si="3">I9=LEFT(H9,1)</f>
-        <v>1</v>
-      </c>
-      <c r="M9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>0011111111</v>
-      </c>
-      <c r="N9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>011111111</v>
-      </c>
-      <c r="O9" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
-        <v>8</v>
-      </c>
-      <c r="B10" s="16">
-        <v>127</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="16">
-        <v>-1</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="17" cm="1">
-        <f t="array" aca="1" ref="G10" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
-        <v>128</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="L10" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M10" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>0010000000</v>
-      </c>
-      <c r="N10" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>010000000</v>
-      </c>
-      <c r="O10" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
-        <v>9</v>
-      </c>
-      <c r="B11" s="21">
-        <v>127</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="21">
-        <v>1</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="22" cm="1">
-        <f t="array" aca="1" ref="G11" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
-        <v>128</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="M11" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>0010000000</v>
-      </c>
-      <c r="N11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>010000000</v>
-      </c>
-      <c r="O11" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="42">
-        <v>1</v>
-      </c>
-      <c r="B12" s="42">
-        <v>-128</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="42">
-        <v>-1</v>
-      </c>
-      <c r="F12" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="44" cm="1">
-        <f t="array" aca="1" ref="G12" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
-        <v>-127</v>
-      </c>
-      <c r="H12" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="43">
-        <v>0</v>
-      </c>
-      <c r="J12" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="L12" t="b">
-        <f>I12=LEFT(H12,1)</f>
-        <v>0</v>
-      </c>
-      <c r="M12" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>1110000001</v>
-      </c>
-      <c r="N12" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>110000001</v>
-      </c>
-      <c r="O12" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47">
-        <v>2</v>
-      </c>
-      <c r="B13" s="47">
-        <v>-128</v>
-      </c>
-      <c r="C13" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="47">
-        <v>1</v>
-      </c>
-      <c r="F13" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="48" cm="1">
-        <f t="array" aca="1" ref="G13" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
-        <v>-127</v>
-      </c>
-      <c r="H13" s="50" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="49">
-        <v>0</v>
-      </c>
-      <c r="J13" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="M13" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>1110000001</v>
-      </c>
-      <c r="N13" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>110000001</v>
-      </c>
-      <c r="O13" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52">
-        <v>3</v>
-      </c>
-      <c r="B14" s="52">
-        <v>-128</v>
-      </c>
-      <c r="C14" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="52">
-        <v>127</v>
-      </c>
-      <c r="F14" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="52">
-        <f>B14+E14</f>
-        <v>-1</v>
-      </c>
-      <c r="H14" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="54">
-        <v>0</v>
-      </c>
-      <c r="J14" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="K14" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="M14" t="str">
-        <f t="shared" si="0"/>
-        <v>1111111111</v>
-      </c>
-      <c r="N14" t="str">
-        <f t="shared" si="1"/>
-        <v>111111111</v>
-      </c>
-      <c r="O14" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="57">
-        <v>4</v>
-      </c>
-      <c r="B15" s="57">
-        <v>-1</v>
-      </c>
-      <c r="C15" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="57">
-        <v>-128</v>
-      </c>
-      <c r="F15" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="59" cm="1">
-        <f t="array" aca="1" ref="G15" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
-        <v>127</v>
-      </c>
-      <c r="H15" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="58">
-        <v>1</v>
-      </c>
-      <c r="J15" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="L15" t="b">
-        <f>I15=LEFT(H15,1)</f>
-        <v>0</v>
-      </c>
-      <c r="M15" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>0001111111</v>
-      </c>
-      <c r="N15" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>001111111</v>
-      </c>
-      <c r="O15" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="72">
-        <v>10</v>
-      </c>
-      <c r="B16" s="72">
-        <v>-1</v>
-      </c>
-      <c r="C16" s="73" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="74" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="72">
-        <v>1</v>
-      </c>
-      <c r="F16" s="73" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="73" cm="1">
-        <f t="array" aca="1" ref="G16" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="75" t="s">
-        <v>23</v>
-      </c>
-      <c r="I16" s="74" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="76" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" s="72" t="s">
-        <v>8</v>
-      </c>
-      <c r="M16" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>0000000000</v>
-      </c>
-      <c r="N16" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>000000000</v>
-      </c>
-      <c r="O16" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="72">
-        <v>10</v>
-      </c>
-      <c r="B17" s="72">
-        <v>-1</v>
-      </c>
-      <c r="C17" s="73" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="74" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="72">
-        <v>1</v>
-      </c>
-      <c r="F17" s="73" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="73" cm="1">
-        <f t="array" aca="1" ref="G17" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
-        <v>-2</v>
-      </c>
-      <c r="H17" s="75" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" s="74">
-        <v>0</v>
-      </c>
-      <c r="J17" s="76" t="s">
-        <v>16</v>
-      </c>
-      <c r="K17" s="72" t="s">
-        <v>8</v>
-      </c>
-      <c r="L17" t="b">
-        <f>I17=LEFT(H17,1)</f>
-        <v>0</v>
-      </c>
-      <c r="M17" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>1111111110</v>
-      </c>
-      <c r="N17" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>111111110</v>
-      </c>
-      <c r="O17" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="77">
-        <v>11</v>
-      </c>
-      <c r="B18" s="77">
-        <v>-1</v>
-      </c>
-      <c r="C18" s="78" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="79" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="77">
-        <v>127</v>
-      </c>
-      <c r="F18" s="77" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" s="77" cm="1">
-        <f t="array" aca="1" ref="G18" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
-        <v>126</v>
-      </c>
-      <c r="H18" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="I18" s="79">
-        <v>1</v>
-      </c>
-      <c r="J18" s="81" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18" s="77" t="s">
-        <v>8</v>
-      </c>
-      <c r="M18" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>0001111110</v>
-      </c>
-      <c r="N18" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>001111110</v>
-      </c>
-      <c r="O18" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="77">
-        <v>11</v>
-      </c>
-      <c r="B19" s="77">
-        <v>-1</v>
-      </c>
-      <c r="C19" s="78" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="79" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="77">
-        <v>127</v>
-      </c>
-      <c r="F19" s="77" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" s="77" cm="1">
-        <f t="array" aca="1" ref="G19" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
-        <v>-128</v>
-      </c>
-      <c r="H19" s="80" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="79" t="s">
-        <v>3</v>
-      </c>
-      <c r="J19" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" s="77" t="s">
-        <v>8</v>
-      </c>
-      <c r="L19" t="b">
-        <f>I19=LEFT(H19,1)</f>
-        <v>1</v>
-      </c>
-      <c r="M19" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>1110000000</v>
-      </c>
-      <c r="N19" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>110000000</v>
-      </c>
-      <c r="O19" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="62">
-        <v>5</v>
-      </c>
-      <c r="B20" s="62">
-        <v>1</v>
-      </c>
-      <c r="C20" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="62">
-        <v>-128</v>
-      </c>
-      <c r="F20" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="63" cm="1">
-        <f t="array" aca="1" ref="G20" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
-        <v>-127</v>
-      </c>
-      <c r="H20" s="65" t="s">
-        <v>20</v>
-      </c>
-      <c r="I20" s="64">
-        <v>0</v>
-      </c>
-      <c r="J20" s="66" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="L20" s="35"/>
-      <c r="M20" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>1110000001</v>
-      </c>
-      <c r="N20" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>110000001</v>
-      </c>
-      <c r="O20" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="67">
-        <v>6</v>
-      </c>
-      <c r="B21" s="67">
-        <v>1</v>
-      </c>
-      <c r="C21" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="68" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="67">
-        <v>127</v>
-      </c>
-      <c r="F21" s="67" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="67" cm="1">
-        <f t="array" aca="1" ref="G21" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
-        <v>-126</v>
-      </c>
-      <c r="H21" s="70" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="68">
-        <v>0</v>
-      </c>
-      <c r="J21" s="71" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="L21" t="b">
-        <f>I21=LEFT(H21,1)</f>
-        <v>0</v>
-      </c>
-      <c r="M21" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>1110000010</v>
-      </c>
-      <c r="N21" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>110000010</v>
-      </c>
-      <c r="O21" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26">
-        <v>12</v>
-      </c>
-      <c r="B22" s="26">
-        <v>1</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="26">
-        <v>-1</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="28" cm="1">
-        <f t="array" aca="1" ref="G22" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" s="27">
-        <v>1</v>
-      </c>
-      <c r="J22" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="M22" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>0000000000</v>
-      </c>
-      <c r="N22" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>000000000</v>
-      </c>
-      <c r="O22" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26">
-        <v>12</v>
-      </c>
-      <c r="B23" s="26">
-        <v>1</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="26">
-        <v>-1</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="28" cm="1">
-        <f t="array" aca="1" ref="G23" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
-        <v>2</v>
-      </c>
-      <c r="H23" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="I23" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="J23" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="K23" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="L23" t="b">
-        <f>I23=LEFT(H23,1)</f>
-        <v>1</v>
-      </c>
-      <c r="M23" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>0000000010</v>
-      </c>
-      <c r="N23" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>000000010</v>
-      </c>
-      <c r="O23" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
-        <v>7</v>
-      </c>
-      <c r="B24" s="11">
-        <v>127</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="11">
-        <v>-128</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G24" s="12" cm="1">
-        <f t="array" aca="1" ref="G24" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
-        <v>-1</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I24" s="13">
-        <v>0</v>
-      </c>
-      <c r="J24" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="M24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>1111111111</v>
-      </c>
-      <c r="N24" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>111111111</v>
-      </c>
-      <c r="O24" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="15.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16">
-        <v>8</v>
-      </c>
-      <c r="B25" s="16">
-        <v>127</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="16">
-        <v>-1</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="G25" s="17" cm="1">
-        <f t="array" aca="1" ref="G25" ca="1">INDIRECT("B"&amp;ROW())+INDIRECT("E"&amp;ROW())</f>
-        <v>126</v>
-      </c>
-      <c r="H25" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="I25" s="18">
-        <v>1</v>
-      </c>
-      <c r="J25" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="K25" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="M25" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>0001111110</v>
-      </c>
-      <c r="N25" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>001111110</v>
-      </c>
-      <c r="O25" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21">
-        <v>9</v>
-      </c>
-      <c r="B26" s="21">
-        <v>127</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="21">
-        <v>1</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="G26" s="22" cm="1">
-        <f t="array" aca="1" ref="G26" ca="1">INDIRECT("B"&amp;ROW())-INDIRECT("E"&amp;ROW())</f>
-        <v>126</v>
-      </c>
-      <c r="H26" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="I26" s="23">
-        <v>1</v>
-      </c>
-      <c r="J26" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="K26" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="L26" t="b">
-        <f>I26=LEFT(H26,1)</f>
-        <v>0</v>
-      </c>
-      <c r="M26" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>0001111110</v>
-      </c>
-      <c r="N26" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>001111110</v>
-      </c>
-      <c r="O26" t="b">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M28" t="str">
-        <f ca="1">DEC2BIN(G12)</f>
-        <v>1110000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="67" t="str" cm="1">
+        <f t="array" aca="1" ref="A29" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;3+(K28-1)*2)&amp;""";"</f>
+        <v>char * input1 = "10000000";</v>
+      </c>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J30" s="31"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J31" s="31"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J32" s="31"/>
-    </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J33" s="31"/>
-    </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J34" s="31"/>
-    </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J35" s="31"/>
-    </row>
-    <row r="36" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J36" s="31"/>
-    </row>
-    <row r="37" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J37" s="31"/>
-    </row>
-    <row r="38" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J38" s="31"/>
-    </row>
-    <row r="39" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J39" s="31"/>
-    </row>
-    <row r="40" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J40" s="31"/>
-    </row>
-    <row r="41" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J41" s="31"/>
-    </row>
-    <row r="42" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J42" s="31"/>
-    </row>
-    <row r="43" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J43" s="31"/>
-    </row>
-    <row r="44" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J44" s="31"/>
-    </row>
-    <row r="45" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J45" s="31"/>
-    </row>
-    <row r="46" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J46" s="31"/>
-    </row>
-    <row r="47" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J47" s="31"/>
-    </row>
-    <row r="48" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J48" s="31"/>
-    </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J49" s="31"/>
-    </row>
-    <row r="50" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J50" s="31"/>
-    </row>
-    <row r="51" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J51" s="31"/>
-    </row>
-    <row r="52" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J52" s="31"/>
-    </row>
-    <row r="53" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J53" s="31"/>
+      <c r="L29" s="7"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="67" t="str" cm="1">
+        <f t="array" aca="1" ref="A30" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;3+(K28-1)*2)&amp;""";"</f>
+        <v>char * input2 = "01111111";</v>
+      </c>
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="K30" s="23"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="67" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="K31" s="23"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="67" t="str" cm="1">
+        <f t="array" aca="1" ref="A32" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;3+(K28-1)*2)&amp;""";"</f>
+        <v>char * expected = "1111111111";</v>
+      </c>
+      <c r="B32" s="67"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
+      <c r="K32" s="23"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="67"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="K33" s="23"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="67" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="67"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="67"/>
+      <c r="K34" s="23"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="68"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
+      <c r="K35" s="23"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="67" t="str" cm="1">
+        <f t="array" aca="1" ref="A36" ca="1">"void TesteSub"&amp;INDIRECT("A"&amp;K28+2)&amp;"(CuTest *tc){"</f>
+        <v>void TesteSub3(CuTest *tc){</v>
+      </c>
+      <c r="B36" s="67"/>
+      <c r="C36" s="67"/>
+      <c r="D36" s="67"/>
+      <c r="K36" s="23"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="67" t="str" cm="1">
+        <f t="array" aca="1" ref="A37" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;4+(K28-1)*2)&amp;""";"</f>
+        <v>char * input1 = "10000000";</v>
+      </c>
+      <c r="B37" s="67"/>
+      <c r="C37" s="67"/>
+      <c r="D37" s="67"/>
+      <c r="K37" s="23"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="67" t="str" cm="1">
+        <f t="array" aca="1" ref="A38" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;4+(K28-1)*2)&amp;""";"</f>
+        <v>char * input2 = "01111111";</v>
+      </c>
+      <c r="B38" s="67"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
+      <c r="K38" s="23"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="67" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="67"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="67"/>
+      <c r="K39" s="23"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="67" t="str" cm="1">
+        <f t="array" aca="1" ref="A40" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;4+(K28-1)*2)&amp;""";"</f>
+        <v>char * expected = "1100000001";</v>
+      </c>
+      <c r="B40" s="67"/>
+      <c r="C40" s="67"/>
+      <c r="D40" s="67"/>
+      <c r="K40" s="23"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="67"/>
+      <c r="C41" s="67"/>
+      <c r="D41" s="67"/>
+      <c r="K41" s="23"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="67" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="67"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67"/>
+      <c r="K42" s="23"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="60"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="K43" s="23"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="65" t="str" cm="1">
+        <f t="array" aca="1" ref="A44" ca="1">"void TesteSoma"&amp;INDIRECT("A"&amp;K28+3)&amp;"(CuTest *tc){"</f>
+        <v>void TesteSoma4(CuTest *tc){</v>
+      </c>
+      <c r="B44" s="65"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="65"/>
+      <c r="K44" s="23"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="65" t="str" cm="1">
+        <f t="array" aca="1" ref="A45" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;5+(K28-1)*2)&amp;""";"</f>
+        <v>char * input1 = "11111111";</v>
+      </c>
+      <c r="B45" s="65"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65"/>
+      <c r="K45" s="23"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="65" t="str" cm="1">
+        <f t="array" aca="1" ref="A46" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;5+(K28-1)*2)&amp;""";"</f>
+        <v>char * input2 = "10000000";</v>
+      </c>
+      <c r="B46" s="65"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="65"/>
+      <c r="K46" s="23"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="65"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="65"/>
+      <c r="K47" s="23"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="65" t="str" cm="1">
+        <f t="array" aca="1" ref="A48" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;5+(K28-1)*2)&amp;""";"</f>
+        <v>char * expected = "1101111111";</v>
+      </c>
+      <c r="B48" s="65"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="65"/>
+      <c r="K48" s="23"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="65"/>
+      <c r="K49" s="23"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" s="65"/>
+      <c r="C50" s="65"/>
+      <c r="D50" s="65"/>
+      <c r="K50" s="23"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="60"/>
+      <c r="B51" s="60"/>
+      <c r="C51" s="60"/>
+      <c r="D51" s="60"/>
+      <c r="K51" s="23"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="65" t="str" cm="1">
+        <f t="array" aca="1" ref="A52" ca="1">"void TesteSub"&amp;INDIRECT("A"&amp;K28+3)&amp;"(CuTest *tc){"</f>
+        <v>void TesteSub4(CuTest *tc){</v>
+      </c>
+      <c r="B52" s="65"/>
+      <c r="C52" s="65"/>
+      <c r="D52" s="65"/>
+      <c r="K52" s="23"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="65" t="str" cm="1">
+        <f t="array" aca="1" ref="A53" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;6+(K28-1)*2)&amp;""";"</f>
+        <v>char * input1 = "11111111";</v>
+      </c>
+      <c r="B53" s="65"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="65"/>
+      <c r="K53" s="23"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="65" t="str" cm="1">
+        <f t="array" aca="1" ref="A54" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;6+(K28-1)*2)&amp;""";"</f>
+        <v>char * input2 = "10000000";</v>
+      </c>
+      <c r="B54" s="65"/>
+      <c r="C54" s="65"/>
+      <c r="D54" s="65"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="65"/>
+      <c r="C55" s="65"/>
+      <c r="D55" s="65"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="65" t="str" cm="1">
+        <f t="array" aca="1" ref="A56" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;6+(K28-1)*2)&amp;""";"</f>
+        <v>char * expected = "0001111111";</v>
+      </c>
+      <c r="B56" s="65"/>
+      <c r="C56" s="65"/>
+      <c r="D56" s="65"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" s="65"/>
+      <c r="C57" s="65"/>
+      <c r="D57" s="65"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58" s="65"/>
+      <c r="C58" s="65"/>
+      <c r="D58" s="65"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="60"/>
+      <c r="B59" s="60"/>
+      <c r="C59" s="60"/>
+      <c r="D59" s="60"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:K26" xr:uid="{CED239D7-98B0-43DB-AD6A-A78832542F2A}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="menos"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K26">
-      <sortCondition ref="K3:K26"/>
+  <autoFilter ref="B2:L26" xr:uid="{CED239D7-98B0-43DB-AD6A-A78832542F2A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:L26">
       <sortCondition ref="B3:B26"/>
+      <sortCondition ref="E3:E26"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K26">
-    <sortCondition ref="A3:A26"/>
-    <sortCondition ref="D3:D26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:L26">
+    <sortCondition ref="B3:B26"/>
+    <sortCondition ref="E3:E26"/>
   </sortState>
+  <mergeCells count="33">
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:D47"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Refatorando e colocando teste unitário.
Refatorando e colocando teste unitário.
Está com erro em 3 testes unitários de subtração
</commit_message>
<xml_diff>
--- a/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
+++ b/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3162c0a97888194f/Documentos/GitHub/algoritmos/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="883" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{766B64A2-0EB3-4122-9189-45A272610943}"/>
+  <xr:revisionPtr revIDLastSave="895" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A06FD2E-CD51-4329-B564-28AD62830E2B}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="2580" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
+    <workbookView xWindow="-90" yWindow="4230" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="numeros_binarios_8bits" sheetId="1" r:id="rId1"/>
@@ -146,12 +146,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>Res 10 bits</t>
-  </si>
-  <si>
-    <t>sinal b10</t>
-  </si>
-  <si>
     <t>V1</t>
   </si>
   <si>
@@ -174,6 +168,12 @@
   </si>
   <si>
     <t>}</t>
+  </si>
+  <si>
+    <t>Res 9 bits</t>
+  </si>
+  <si>
+    <t>sinal b9</t>
   </si>
 </sst>
 </file>
@@ -615,13 +615,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -956,8 +956,8 @@
   </sheetPr>
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4432,10 +4432,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A2:M59"/>
+  <dimension ref="A2:N59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4457,15 +4457,15 @@
     <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>12</v>
@@ -4474,28 +4474,28 @@
         <v>0</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <v>1</v>
       </c>
@@ -4521,22 +4521,25 @@
         <v>-129</v>
       </c>
       <c r="I3" s="27" t="str">
-        <f>DEC2BIN(H3,10)</f>
-        <v>1101111111</v>
+        <f>RIGHT(DEC2BIN(H3,10),9)</f>
+        <v>101111111</v>
       </c>
       <c r="J3" s="27" t="str">
-        <f t="shared" ref="J3:J26" si="0">MID(I3,1,1)</f>
+        <f>MID(I3,1,1)</f>
         <v>1</v>
       </c>
       <c r="K3" s="27" t="str">
-        <f t="shared" ref="K3:K26" si="1">MID(I3,2,2)</f>
+        <f>MID(I3,1,2)</f>
         <v>10</v>
       </c>
       <c r="L3" s="27" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <v>2</v>
       </c>
@@ -4562,22 +4565,25 @@
         <v>-127</v>
       </c>
       <c r="I4" s="27" t="str">
-        <f t="shared" ref="I4:I26" si="2">DEC2BIN(H4,10)</f>
-        <v>1110000001</v>
+        <f>RIGHT(DEC2BIN(H4,10),9)</f>
+        <v>110000001</v>
       </c>
       <c r="J4" s="27" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I4,1,1)</f>
         <v>1</v>
       </c>
       <c r="K4" s="27" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I4,1,2)</f>
         <v>11</v>
       </c>
       <c r="L4" s="27" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>3</v>
       </c>
@@ -4603,22 +4609,25 @@
         <v>-127</v>
       </c>
       <c r="I5" s="30" t="str">
-        <f t="shared" si="2"/>
-        <v>1110000001</v>
+        <f>RIGHT(DEC2BIN(H5,10),9)</f>
+        <v>110000001</v>
       </c>
       <c r="J5" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I5,1,1)</f>
         <v>1</v>
       </c>
       <c r="K5" s="30" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I5,1,2)</f>
         <v>11</v>
       </c>
       <c r="L5" s="30" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>4</v>
       </c>
@@ -4644,22 +4653,25 @@
         <v>-129</v>
       </c>
       <c r="I6" s="30" t="str">
-        <f t="shared" si="2"/>
-        <v>1101111111</v>
+        <f>RIGHT(DEC2BIN(H6,10),9)</f>
+        <v>101111111</v>
       </c>
       <c r="J6" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I6,1,1)</f>
         <v>1</v>
       </c>
       <c r="K6" s="30" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I6,1,2)</f>
         <v>10</v>
       </c>
       <c r="L6" s="30" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>-128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
         <v>5</v>
       </c>
@@ -4685,22 +4697,22 @@
         <v>-1</v>
       </c>
       <c r="I7" s="33" t="str">
-        <f t="shared" si="2"/>
-        <v>1111111111</v>
+        <f>RIGHT(DEC2BIN(H7,10),9)</f>
+        <v>111111111</v>
       </c>
       <c r="J7" s="33" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I7,1,1)</f>
         <v>1</v>
       </c>
       <c r="K7" s="33" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I7,1,2)</f>
         <v>11</v>
       </c>
       <c r="L7" s="33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
         <v>6</v>
       </c>
@@ -4726,22 +4738,22 @@
         <v>-255</v>
       </c>
       <c r="I8" s="33" t="str">
-        <f t="shared" si="2"/>
-        <v>1100000001</v>
+        <f>RIGHT(DEC2BIN(H8,10),9)</f>
+        <v>100000001</v>
       </c>
       <c r="J8" s="33" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I8,1,1)</f>
         <v>1</v>
       </c>
       <c r="K8" s="33" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I8,1,2)</f>
         <v>10</v>
       </c>
       <c r="L8" s="33" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36">
         <v>7</v>
       </c>
@@ -4767,22 +4779,22 @@
         <v>-129</v>
       </c>
       <c r="I9" s="36" t="str">
-        <f t="shared" si="2"/>
-        <v>1101111111</v>
+        <f>RIGHT(DEC2BIN(H9,10),9)</f>
+        <v>101111111</v>
       </c>
       <c r="J9" s="36" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I9,1,1)</f>
         <v>1</v>
       </c>
       <c r="K9" s="36" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I9,1,2)</f>
         <v>10</v>
       </c>
       <c r="L9" s="36" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="52">
         <v>8</v>
       </c>
@@ -4808,22 +4820,22 @@
         <v>127</v>
       </c>
       <c r="I10" s="52" t="str">
-        <f t="shared" si="2"/>
-        <v>0001111111</v>
+        <f>RIGHT(DEC2BIN(H10,10),9)</f>
+        <v>001111111</v>
       </c>
       <c r="J10" s="52" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I10,1,1)</f>
         <v>0</v>
       </c>
       <c r="K10" s="52" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I10,1,2)</f>
         <v>00</v>
       </c>
       <c r="L10" s="52" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="39">
         <v>9</v>
       </c>
@@ -4849,23 +4861,23 @@
         <v>-127</v>
       </c>
       <c r="I11" s="39" t="str">
-        <f t="shared" si="2"/>
-        <v>1110000001</v>
+        <f>RIGHT(DEC2BIN(H11,10),9)</f>
+        <v>110000001</v>
       </c>
       <c r="J11" s="39" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I11,1,1)</f>
         <v>1</v>
       </c>
       <c r="K11" s="39" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I11,1,2)</f>
         <v>11</v>
       </c>
       <c r="L11" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="M11" s="66"/>
-    </row>
-    <row r="12" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="68"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="39">
         <v>10</v>
       </c>
@@ -4891,23 +4903,23 @@
         <v>129</v>
       </c>
       <c r="I12" s="39" t="str">
-        <f t="shared" si="2"/>
-        <v>0010000001</v>
+        <f>RIGHT(DEC2BIN(H12,10),9)</f>
+        <v>010000001</v>
       </c>
       <c r="J12" s="39" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I12,1,1)</f>
         <v>0</v>
       </c>
       <c r="K12" s="39" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I12,1,2)</f>
         <v>01</v>
       </c>
       <c r="L12" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="M12" s="66"/>
-    </row>
-    <row r="13" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="68"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>11</v>
       </c>
@@ -4933,22 +4945,22 @@
         <v>128</v>
       </c>
       <c r="I13" s="42" t="str">
-        <f t="shared" si="2"/>
-        <v>0010000000</v>
+        <f>RIGHT(DEC2BIN(H13,10),9)</f>
+        <v>010000000</v>
       </c>
       <c r="J13" s="42" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I13,1,1)</f>
         <v>0</v>
       </c>
       <c r="K13" s="42" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I13,1,2)</f>
         <v>01</v>
       </c>
       <c r="L13" s="42" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>12</v>
       </c>
@@ -4974,22 +4986,22 @@
         <v>-126</v>
       </c>
       <c r="I14" s="42" t="str">
-        <f t="shared" si="2"/>
-        <v>1110000010</v>
+        <f>RIGHT(DEC2BIN(H14,10),9)</f>
+        <v>110000010</v>
       </c>
       <c r="J14" s="42" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I14,1,1)</f>
         <v>1</v>
       </c>
       <c r="K14" s="42" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I14,1,2)</f>
         <v>11</v>
       </c>
       <c r="L14" s="42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>13</v>
       </c>
@@ -5015,22 +5027,22 @@
         <v>-1</v>
       </c>
       <c r="I15" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>1111111111</v>
+        <f>RIGHT(DEC2BIN(H15,10),9)</f>
+        <v>111111111</v>
       </c>
       <c r="J15" s="11" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I15,1,1)</f>
         <v>1</v>
       </c>
       <c r="K15" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I15,1,2)</f>
         <v>11</v>
       </c>
       <c r="L15" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>14</v>
       </c>
@@ -5056,15 +5068,15 @@
         <v>255</v>
       </c>
       <c r="I16" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>0011111111</v>
+        <f>RIGHT(DEC2BIN(H16,10),9)</f>
+        <v>011111111</v>
       </c>
       <c r="J16" s="11" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I16,1,1)</f>
         <v>0</v>
       </c>
       <c r="K16" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I16,1,2)</f>
         <v>01</v>
       </c>
       <c r="L16" s="11" t="s">
@@ -5097,15 +5109,15 @@
         <v>126</v>
       </c>
       <c r="I17" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>0001111110</v>
+        <f>RIGHT(DEC2BIN(H17,10),9)</f>
+        <v>001111110</v>
       </c>
       <c r="J17" s="14" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I17,1,1)</f>
         <v>0</v>
       </c>
       <c r="K17" s="14" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I17,1,2)</f>
         <v>00</v>
       </c>
       <c r="L17" s="14" t="s">
@@ -5138,15 +5150,15 @@
         <v>128</v>
       </c>
       <c r="I18" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>0010000000</v>
+        <f>RIGHT(DEC2BIN(H18,10),9)</f>
+        <v>010000000</v>
       </c>
       <c r="J18" s="14" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I18,1,1)</f>
         <v>0</v>
       </c>
       <c r="K18" s="14" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I18,1,2)</f>
         <v>01</v>
       </c>
       <c r="L18" s="14" t="s">
@@ -5179,15 +5191,15 @@
         <v>128</v>
       </c>
       <c r="I19" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>0010000000</v>
+        <f>RIGHT(DEC2BIN(H19,10),9)</f>
+        <v>010000000</v>
       </c>
       <c r="J19" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I19,1,1)</f>
         <v>0</v>
       </c>
       <c r="K19" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I19,1,2)</f>
         <v>01</v>
       </c>
       <c r="L19" s="17" t="s">
@@ -5220,15 +5232,15 @@
         <v>126</v>
       </c>
       <c r="I20" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>0001111110</v>
+        <f>RIGHT(DEC2BIN(H20,10),9)</f>
+        <v>001111110</v>
       </c>
       <c r="J20" s="17" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I20,1,1)</f>
         <v>0</v>
       </c>
       <c r="K20" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I20,1,2)</f>
         <v>00</v>
       </c>
       <c r="L20" s="17" t="s">
@@ -5261,15 +5273,15 @@
         <v>0</v>
       </c>
       <c r="I21" s="45" t="str">
-        <f t="shared" si="2"/>
-        <v>0000000000</v>
+        <f>RIGHT(DEC2BIN(H21,10),9)</f>
+        <v>000000000</v>
       </c>
       <c r="J21" s="45" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I21,1,1)</f>
         <v>0</v>
       </c>
       <c r="K21" s="45" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I21,1,2)</f>
         <v>00</v>
       </c>
       <c r="L21" s="45" t="s">
@@ -5302,15 +5314,15 @@
         <v>-2</v>
       </c>
       <c r="I22" s="45" t="str">
-        <f t="shared" si="2"/>
-        <v>1111111110</v>
+        <f>RIGHT(DEC2BIN(H22,10),9)</f>
+        <v>111111110</v>
       </c>
       <c r="J22" s="45" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I22,1,1)</f>
         <v>1</v>
       </c>
       <c r="K22" s="45" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I22,1,2)</f>
         <v>11</v>
       </c>
       <c r="L22" s="45" t="s">
@@ -5343,15 +5355,15 @@
         <v>126</v>
       </c>
       <c r="I23" s="48" t="str">
-        <f t="shared" si="2"/>
-        <v>0001111110</v>
+        <f>RIGHT(DEC2BIN(H23,10),9)</f>
+        <v>001111110</v>
       </c>
       <c r="J23" s="48" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I23,1,1)</f>
         <v>0</v>
       </c>
       <c r="K23" s="48" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I23,1,2)</f>
         <v>00</v>
       </c>
       <c r="L23" s="48" t="s">
@@ -5384,15 +5396,15 @@
         <v>-128</v>
       </c>
       <c r="I24" s="48" t="str">
-        <f t="shared" si="2"/>
-        <v>1110000000</v>
+        <f>RIGHT(DEC2BIN(H24,10),9)</f>
+        <v>110000000</v>
       </c>
       <c r="J24" s="48" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I24,1,1)</f>
         <v>1</v>
       </c>
       <c r="K24" s="48" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I24,1,2)</f>
         <v>11</v>
       </c>
       <c r="L24" s="48" t="s">
@@ -5425,15 +5437,15 @@
         <v>0</v>
       </c>
       <c r="I25" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v>0000000000</v>
+        <f>RIGHT(DEC2BIN(H25,10),9)</f>
+        <v>000000000</v>
       </c>
       <c r="J25" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I25,1,1)</f>
         <v>0</v>
       </c>
       <c r="K25" s="20" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I25,1,2)</f>
         <v>00</v>
       </c>
       <c r="L25" s="20" t="s">
@@ -5466,15 +5478,15 @@
         <v>2</v>
       </c>
       <c r="I26" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v>0000000010</v>
+        <f>RIGHT(DEC2BIN(H26,10),9)</f>
+        <v>000000010</v>
       </c>
       <c r="J26" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f>MID(I26,1,1)</f>
         <v>0</v>
       </c>
       <c r="K26" s="20" t="str">
-        <f t="shared" si="1"/>
+        <f>MID(I26,1,2)</f>
         <v>00</v>
       </c>
       <c r="L26" s="20" t="s">
@@ -5482,149 +5494,149 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="67" t="str" cm="1">
+      <c r="A28" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A28" ca="1">"void TesteSoma"&amp;INDIRECT("A"&amp;K28+2)&amp;"(CuTest *tc){"</f>
         <v>void TesteSoma3(CuTest *tc){</v>
       </c>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
       <c r="K28" s="51">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="67" t="str" cm="1">
+      <c r="A29" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A29" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;3+(K28-1)*2)&amp;""";"</f>
         <v>char * input1 = "10000000";</v>
       </c>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
       <c r="E29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="67" t="str" cm="1">
+      <c r="A30" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A30" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;3+(K28-1)*2)&amp;""";"</f>
         <v>char * input2 = "01111111";</v>
       </c>
-      <c r="B30" s="67"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
       <c r="K30" s="23"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="67" t="s">
+      <c r="A31" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="K31" s="23"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="66" t="str" cm="1">
+        <f t="array" aca="1" ref="A32" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;3+(K28-1)*2)&amp;""";"</f>
+        <v>char * expected = "111111111";</v>
+      </c>
+      <c r="B32" s="66"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="66"/>
+      <c r="K32" s="23"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="66"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
+      <c r="K33" s="23"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="67"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="K31" s="23"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="A32" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;3+(K28-1)*2)&amp;""";"</f>
-        <v>char * expected = "1111111111";</v>
-      </c>
-      <c r="B32" s="67"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="K32" s="23"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="67" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="K33" s="23"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="67"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
       <c r="K34" s="23"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="68"/>
-      <c r="B35" s="68"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="68"/>
+      <c r="A35" s="67"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="67"/>
+      <c r="D35" s="67"/>
       <c r="K35" s="23"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="67" t="str" cm="1">
+      <c r="A36" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A36" ca="1">"void TesteSub"&amp;INDIRECT("A"&amp;K28+2)&amp;"(CuTest *tc){"</f>
         <v>void TesteSub3(CuTest *tc){</v>
       </c>
-      <c r="B36" s="67"/>
-      <c r="C36" s="67"/>
-      <c r="D36" s="67"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
       <c r="K36" s="23"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="67" t="str" cm="1">
+      <c r="A37" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A37" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;4+(K28-1)*2)&amp;""";"</f>
         <v>char * input1 = "10000000";</v>
       </c>
-      <c r="B37" s="67"/>
-      <c r="C37" s="67"/>
-      <c r="D37" s="67"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
       <c r="K37" s="23"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="67" t="str" cm="1">
+      <c r="A38" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A38" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;4+(K28-1)*2)&amp;""";"</f>
         <v>char * input2 = "01111111";</v>
       </c>
-      <c r="B38" s="67"/>
-      <c r="C38" s="67"/>
-      <c r="D38" s="67"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
       <c r="K38" s="23"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="67" t="s">
+      <c r="A39" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="66"/>
+      <c r="C39" s="66"/>
+      <c r="D39" s="66"/>
+      <c r="K39" s="23"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="66" t="str" cm="1">
+        <f t="array" aca="1" ref="A40" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;4+(K28-1)*2)&amp;""";"</f>
+        <v>char * expected = "100000001";</v>
+      </c>
+      <c r="B40" s="66"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
+      <c r="K40" s="23"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="66"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66"/>
+      <c r="K41" s="23"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="67"/>
-      <c r="C39" s="67"/>
-      <c r="D39" s="67"/>
-      <c r="K39" s="23"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="67" t="str" cm="1">
-        <f t="array" aca="1" ref="A40" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;4+(K28-1)*2)&amp;""";"</f>
-        <v>char * expected = "1100000001";</v>
-      </c>
-      <c r="B40" s="67"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="67"/>
-      <c r="K40" s="23"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="67" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" s="67"/>
-      <c r="C41" s="67"/>
-      <c r="D41" s="67"/>
-      <c r="K41" s="23"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="67"/>
-      <c r="C42" s="67"/>
-      <c r="D42" s="67"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="66"/>
       <c r="K42" s="23"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -5666,7 +5678,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="65" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B47" s="65"/>
       <c r="C47" s="65"/>
@@ -5676,7 +5688,7 @@
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A48" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;5+(K28-1)*2)&amp;""";"</f>
-        <v>char * expected = "1101111111";</v>
+        <v>char * expected = "101111111";</v>
       </c>
       <c r="B48" s="65"/>
       <c r="C48" s="65"/>
@@ -5685,7 +5697,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B49" s="65"/>
       <c r="C49" s="65"/>
@@ -5694,7 +5706,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="65" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B50" s="65"/>
       <c r="C50" s="65"/>
@@ -5739,7 +5751,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="65" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B55" s="65"/>
       <c r="C55" s="65"/>
@@ -5748,7 +5760,7 @@
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A56" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;6+(K28-1)*2)&amp;""";"</f>
-        <v>char * expected = "0001111111";</v>
+        <v>char * expected = "001111111";</v>
       </c>
       <c r="B56" s="65"/>
       <c r="C56" s="65"/>
@@ -5756,7 +5768,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B57" s="65"/>
       <c r="C57" s="65"/>
@@ -5764,7 +5776,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="65" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B58" s="65"/>
       <c r="C58" s="65"/>
@@ -5788,6 +5800,8 @@
     <sortCondition ref="E3:E26"/>
   </sortState>
   <mergeCells count="33">
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A46:D46"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="A48:D48"/>
     <mergeCell ref="M11:M12"/>
@@ -5803,7 +5817,7 @@
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A47:D47"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A43:D43"/>
     <mergeCell ref="A59:D59"/>
@@ -5819,8 +5833,6 @@
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="A44:D44"/>
     <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:D47"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Passa no teste mas falta tratar overflow e regra de sinal. Multiplicação está por fazer.
Passa no teste mas falta tratar overflow e regra de sinal. Multiplicação está por fazer.
</commit_message>
<xml_diff>
--- a/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
+++ b/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3162c0a97888194f/Documentos/GitHub/algoritmos/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="895" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A06FD2E-CD51-4329-B564-28AD62830E2B}"/>
+  <xr:revisionPtr revIDLastSave="916" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2ACF37C3-393F-4491-98D0-5134FBAFEC64}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="4230" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
+    <workbookView xWindow="3465" yWindow="4485" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="numeros_binarios_8bits" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="44">
   <si>
     <t>op</t>
   </si>
@@ -175,6 +175,27 @@
   <si>
     <t>sinal b9</t>
   </si>
+  <si>
+    <t>101111111</t>
+  </si>
+  <si>
+    <t>1110000001</t>
+  </si>
+  <si>
+    <t>1111111111</t>
+  </si>
+  <si>
+    <t>overflow</t>
+  </si>
+  <si>
+    <t>(v2 =  c2)&amp;(msb = 0): resetar msb</t>
+  </si>
+  <si>
+    <t>(v2 = c2)&amp;(msb = 1): erro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(v2 = c2)&amp;(msb = 1): erro </t>
+  </si>
 </sst>
 </file>
 
@@ -222,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,12 +299,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,15 +517,24 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -523,39 +547,39 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -565,23 +589,14 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -612,18 +627,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutro" xfId="2" builtinId="28"/>
@@ -4432,10 +4445,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A2:N59"/>
+  <dimension ref="A2:M59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4457,7 +4470,7 @@
     <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
@@ -4495,7 +4508,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <v>1</v>
       </c>
@@ -4521,25 +4534,22 @@
         <v>-129</v>
       </c>
       <c r="I3" s="27" t="str">
-        <f>RIGHT(DEC2BIN(H3,10),9)</f>
+        <f t="shared" ref="I3:I26" si="0">RIGHT(DEC2BIN(H3,10),9)</f>
         <v>101111111</v>
       </c>
       <c r="J3" s="27" t="str">
-        <f>MID(I3,1,1)</f>
+        <f t="shared" ref="J3:J26" si="1">MID(I3,1,1)</f>
         <v>1</v>
       </c>
       <c r="K3" s="27" t="str">
-        <f>MID(I3,1,2)</f>
+        <f t="shared" ref="K3:K26" si="2">MID(I3,1,2)</f>
         <v>10</v>
       </c>
       <c r="L3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="N3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <v>2</v>
       </c>
@@ -4565,25 +4575,22 @@
         <v>-127</v>
       </c>
       <c r="I4" s="27" t="str">
-        <f>RIGHT(DEC2BIN(H4,10),9)</f>
+        <f t="shared" si="0"/>
         <v>110000001</v>
       </c>
       <c r="J4" s="27" t="str">
-        <f>MID(I4,1,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K4" s="27" t="str">
-        <f>MID(I4,1,2)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>3</v>
       </c>
@@ -4609,25 +4616,22 @@
         <v>-127</v>
       </c>
       <c r="I5" s="30" t="str">
-        <f>RIGHT(DEC2BIN(H5,10),9)</f>
+        <f t="shared" si="0"/>
         <v>110000001</v>
       </c>
       <c r="J5" s="30" t="str">
-        <f>MID(I5,1,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K5" s="30" t="str">
-        <f>MID(I5,1,2)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="N5">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>4</v>
       </c>
@@ -4653,25 +4657,22 @@
         <v>-129</v>
       </c>
       <c r="I6" s="30" t="str">
-        <f>RIGHT(DEC2BIN(H6,10),9)</f>
+        <f t="shared" si="0"/>
         <v>101111111</v>
       </c>
       <c r="J6" s="30" t="str">
-        <f>MID(I6,1,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K6" s="30" t="str">
-        <f>MID(I6,1,2)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="L6" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="N6">
-        <v>-128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
         <v>5</v>
       </c>
@@ -4697,22 +4698,22 @@
         <v>-1</v>
       </c>
       <c r="I7" s="33" t="str">
-        <f>RIGHT(DEC2BIN(H7,10),9)</f>
+        <f t="shared" si="0"/>
         <v>111111111</v>
       </c>
       <c r="J7" s="33" t="str">
-        <f>MID(I7,1,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K7" s="33" t="str">
-        <f>MID(I7,1,2)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L7" s="33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
         <v>6</v>
       </c>
@@ -4738,22 +4739,22 @@
         <v>-255</v>
       </c>
       <c r="I8" s="33" t="str">
-        <f>RIGHT(DEC2BIN(H8,10),9)</f>
+        <f t="shared" si="0"/>
         <v>100000001</v>
       </c>
       <c r="J8" s="33" t="str">
-        <f>MID(I8,1,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K8" s="33" t="str">
-        <f>MID(I8,1,2)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="L8" s="33" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36">
         <v>7</v>
       </c>
@@ -4779,22 +4780,22 @@
         <v>-129</v>
       </c>
       <c r="I9" s="36" t="str">
-        <f>RIGHT(DEC2BIN(H9,10),9)</f>
+        <f t="shared" si="0"/>
         <v>101111111</v>
       </c>
       <c r="J9" s="36" t="str">
-        <f>MID(I9,1,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K9" s="36" t="str">
-        <f>MID(I9,1,2)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="L9" s="36" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="52">
         <v>8</v>
       </c>
@@ -4819,23 +4820,25 @@
       <c r="H10" s="54">
         <v>127</v>
       </c>
-      <c r="I10" s="52" t="str">
-        <f>RIGHT(DEC2BIN(H10,10),9)</f>
-        <v>001111111</v>
+      <c r="I10" s="54" t="s">
+        <v>37</v>
       </c>
       <c r="J10" s="52" t="str">
-        <f>MID(I10,1,1)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="K10" s="52" t="str">
-        <f>MID(I10,1,2)</f>
-        <v>00</v>
+        <f>MID(I10,1,2)&amp;" NA"</f>
+        <v>10 NA</v>
       </c>
       <c r="L10" s="52" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="39">
         <v>9</v>
       </c>
@@ -4861,15 +4864,15 @@
         <v>-127</v>
       </c>
       <c r="I11" s="39" t="str">
-        <f>RIGHT(DEC2BIN(H11,10),9)</f>
+        <f t="shared" si="0"/>
         <v>110000001</v>
       </c>
       <c r="J11" s="39" t="str">
-        <f>MID(I11,1,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K11" s="39" t="str">
-        <f>MID(I11,1,2)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L11" s="39" t="s">
@@ -4877,49 +4880,50 @@
       </c>
       <c r="M11" s="68"/>
     </row>
-    <row r="12" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="39">
         <v>10</v>
       </c>
-      <c r="B12" s="39">
+      <c r="B12" s="52">
         <v>5</v>
       </c>
-      <c r="C12" s="39">
-        <v>1</v>
-      </c>
-      <c r="D12" s="39" t="s">
+      <c r="C12" s="52">
+        <v>1</v>
+      </c>
+      <c r="D12" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="41" t="s">
+      <c r="E12" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="39">
+      <c r="F12" s="52">
         <v>-128</v>
       </c>
-      <c r="G12" s="40" t="s">
+      <c r="G12" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="40">
+      <c r="H12" s="54">
         <v>129</v>
       </c>
-      <c r="I12" s="39" t="str">
-        <f>RIGHT(DEC2BIN(H12,10),9)</f>
-        <v>010000001</v>
-      </c>
-      <c r="J12" s="39" t="str">
-        <f>MID(I12,1,1)</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="39" t="str">
-        <f>MID(I12,1,2)</f>
-        <v>01</v>
-      </c>
-      <c r="L12" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="M12" s="68"/>
-    </row>
-    <row r="13" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K12" s="52" t="str">
+        <f>MID(I12,1,2)&amp;" NA"</f>
+        <v>11 NA</v>
+      </c>
+      <c r="L12" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="M12" s="68" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>11</v>
       </c>
@@ -4945,22 +4949,22 @@
         <v>128</v>
       </c>
       <c r="I13" s="42" t="str">
-        <f>RIGHT(DEC2BIN(H13,10),9)</f>
+        <f t="shared" si="0"/>
         <v>010000000</v>
       </c>
       <c r="J13" s="42" t="str">
-        <f>MID(I13,1,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K13" s="42" t="str">
-        <f>MID(I13,1,2)</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="L13" s="42" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>12</v>
       </c>
@@ -4986,22 +4990,22 @@
         <v>-126</v>
       </c>
       <c r="I14" s="42" t="str">
-        <f>RIGHT(DEC2BIN(H14,10),9)</f>
+        <f t="shared" si="0"/>
         <v>110000010</v>
       </c>
       <c r="J14" s="42" t="str">
-        <f>MID(I14,1,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K14" s="42" t="str">
-        <f>MID(I14,1,2)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L14" s="42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>13</v>
       </c>
@@ -5027,60 +5031,62 @@
         <v>-1</v>
       </c>
       <c r="I15" s="11" t="str">
-        <f>RIGHT(DEC2BIN(H15,10),9)</f>
+        <f t="shared" si="0"/>
         <v>111111111</v>
       </c>
       <c r="J15" s="11" t="str">
-        <f>MID(I15,1,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K15" s="11" t="str">
-        <f>MID(I15,1,2)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L15" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>14</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="52">
         <v>7</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="52">
         <v>127</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="52">
         <v>-128</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="54">
         <v>255</v>
       </c>
-      <c r="I16" s="11" t="str">
-        <f>RIGHT(DEC2BIN(H16,10),9)</f>
-        <v>011111111</v>
-      </c>
-      <c r="J16" s="11" t="str">
-        <f>MID(I16,1,1)</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="11" t="str">
-        <f>MID(I16,1,2)</f>
-        <v>01</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>1</v>
+      <c r="I16" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K16" s="52" t="str">
+        <f>MID(I16,1,2)&amp;" NA"</f>
+        <v>11 NA</v>
+      </c>
+      <c r="L16" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="M16" s="68" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5109,15 +5115,15 @@
         <v>126</v>
       </c>
       <c r="I17" s="14" t="str">
-        <f>RIGHT(DEC2BIN(H17,10),9)</f>
+        <f t="shared" si="0"/>
         <v>001111110</v>
       </c>
       <c r="J17" s="14" t="str">
-        <f>MID(I17,1,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K17" s="14" t="str">
-        <f>MID(I17,1,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="L17" s="14" t="s">
@@ -5150,15 +5156,15 @@
         <v>128</v>
       </c>
       <c r="I18" s="14" t="str">
-        <f>RIGHT(DEC2BIN(H18,10),9)</f>
+        <f t="shared" si="0"/>
         <v>010000000</v>
       </c>
       <c r="J18" s="14" t="str">
-        <f>MID(I18,1,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K18" s="14" t="str">
-        <f>MID(I18,1,2)</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="L18" s="14" t="s">
@@ -5191,15 +5197,15 @@
         <v>128</v>
       </c>
       <c r="I19" s="17" t="str">
-        <f>RIGHT(DEC2BIN(H19,10),9)</f>
+        <f t="shared" si="0"/>
         <v>010000000</v>
       </c>
       <c r="J19" s="17" t="str">
-        <f>MID(I19,1,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K19" s="17" t="str">
-        <f>MID(I19,1,2)</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="L19" s="17" t="s">
@@ -5232,15 +5238,15 @@
         <v>126</v>
       </c>
       <c r="I20" s="17" t="str">
-        <f>RIGHT(DEC2BIN(H20,10),9)</f>
+        <f t="shared" si="0"/>
         <v>001111110</v>
       </c>
       <c r="J20" s="17" t="str">
-        <f>MID(I20,1,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K20" s="17" t="str">
-        <f>MID(I20,1,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="L20" s="17" t="s">
@@ -5273,15 +5279,15 @@
         <v>0</v>
       </c>
       <c r="I21" s="45" t="str">
-        <f>RIGHT(DEC2BIN(H21,10),9)</f>
+        <f t="shared" si="0"/>
         <v>000000000</v>
       </c>
       <c r="J21" s="45" t="str">
-        <f>MID(I21,1,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K21" s="45" t="str">
-        <f>MID(I21,1,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="L21" s="45" t="s">
@@ -5314,15 +5320,15 @@
         <v>-2</v>
       </c>
       <c r="I22" s="45" t="str">
-        <f>RIGHT(DEC2BIN(H22,10),9)</f>
+        <f t="shared" si="0"/>
         <v>111111110</v>
       </c>
       <c r="J22" s="45" t="str">
-        <f>MID(I22,1,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K22" s="45" t="str">
-        <f>MID(I22,1,2)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L22" s="45" t="s">
@@ -5355,15 +5361,15 @@
         <v>126</v>
       </c>
       <c r="I23" s="48" t="str">
-        <f>RIGHT(DEC2BIN(H23,10),9)</f>
+        <f t="shared" si="0"/>
         <v>001111110</v>
       </c>
       <c r="J23" s="48" t="str">
-        <f>MID(I23,1,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K23" s="48" t="str">
-        <f>MID(I23,1,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="L23" s="48" t="s">
@@ -5396,15 +5402,15 @@
         <v>-128</v>
       </c>
       <c r="I24" s="48" t="str">
-        <f>RIGHT(DEC2BIN(H24,10),9)</f>
+        <f t="shared" si="0"/>
         <v>110000000</v>
       </c>
       <c r="J24" s="48" t="str">
-        <f>MID(I24,1,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K24" s="48" t="str">
-        <f>MID(I24,1,2)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L24" s="48" t="s">
@@ -5437,15 +5443,15 @@
         <v>0</v>
       </c>
       <c r="I25" s="20" t="str">
-        <f>RIGHT(DEC2BIN(H25,10),9)</f>
+        <f t="shared" si="0"/>
         <v>000000000</v>
       </c>
       <c r="J25" s="20" t="str">
-        <f>MID(I25,1,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K25" s="20" t="str">
-        <f>MID(I25,1,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="L25" s="20" t="s">
@@ -5478,15 +5484,15 @@
         <v>2</v>
       </c>
       <c r="I26" s="20" t="str">
-        <f>RIGHT(DEC2BIN(H26,10),9)</f>
+        <f t="shared" si="0"/>
         <v>000000010</v>
       </c>
       <c r="J26" s="20" t="str">
-        <f>MID(I26,1,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K26" s="20" t="str">
-        <f>MID(I26,1,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="L26" s="20" t="s">
@@ -5494,75 +5500,75 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="66" t="str" cm="1">
+      <c r="A28" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A28" ca="1">"void TesteSoma"&amp;INDIRECT("A"&amp;K28+2)&amp;"(CuTest *tc){"</f>
         <v>void TesteSoma3(CuTest *tc){</v>
       </c>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
       <c r="K28" s="51">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="66" t="str" cm="1">
+      <c r="A29" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A29" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;3+(K28-1)*2)&amp;""";"</f>
         <v>char * input1 = "10000000";</v>
       </c>
-      <c r="B29" s="66"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="65"/>
       <c r="E29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="66" t="str" cm="1">
+      <c r="A30" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A30" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;3+(K28-1)*2)&amp;""";"</f>
         <v>char * input2 = "01111111";</v>
       </c>
-      <c r="B30" s="66"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="66"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
       <c r="K30" s="23"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="66"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
       <c r="K31" s="23"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="66" t="str" cm="1">
+      <c r="A32" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A32" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;3+(K28-1)*2)&amp;""";"</f>
         <v>char * expected = "111111111";</v>
       </c>
-      <c r="B32" s="66"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="66"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
       <c r="K32" s="23"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="66"/>
-      <c r="C33" s="66"/>
-      <c r="D33" s="66"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="65"/>
       <c r="K33" s="23"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="66"/>
-      <c r="C34" s="66"/>
-      <c r="D34" s="66"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
       <c r="K34" s="23"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -5573,70 +5579,70 @@
       <c r="K35" s="23"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="66" t="str" cm="1">
+      <c r="A36" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A36" ca="1">"void TesteSub"&amp;INDIRECT("A"&amp;K28+2)&amp;"(CuTest *tc){"</f>
         <v>void TesteSub3(CuTest *tc){</v>
       </c>
-      <c r="B36" s="66"/>
-      <c r="C36" s="66"/>
-      <c r="D36" s="66"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
       <c r="K36" s="23"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="66" t="str" cm="1">
+      <c r="A37" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A37" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;4+(K28-1)*2)&amp;""";"</f>
         <v>char * input1 = "10000000";</v>
       </c>
-      <c r="B37" s="66"/>
-      <c r="C37" s="66"/>
-      <c r="D37" s="66"/>
+      <c r="B37" s="65"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="65"/>
       <c r="K37" s="23"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="66" t="str" cm="1">
+      <c r="A38" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A38" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;4+(K28-1)*2)&amp;""";"</f>
         <v>char * input2 = "01111111";</v>
       </c>
-      <c r="B38" s="66"/>
-      <c r="C38" s="66"/>
-      <c r="D38" s="66"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
       <c r="K38" s="23"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="66"/>
-      <c r="C39" s="66"/>
-      <c r="D39" s="66"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="65"/>
       <c r="K39" s="23"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="66" t="str" cm="1">
+      <c r="A40" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A40" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;4+(K28-1)*2)&amp;""";"</f>
         <v>char * expected = "100000001";</v>
       </c>
-      <c r="B40" s="66"/>
-      <c r="C40" s="66"/>
-      <c r="D40" s="66"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="65"/>
       <c r="K40" s="23"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="66"/>
-      <c r="C41" s="66"/>
-      <c r="D41" s="66"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="65"/>
       <c r="K41" s="23"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="66"/>
-      <c r="C42" s="66"/>
-      <c r="D42" s="66"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
       <c r="K42" s="23"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -5647,70 +5653,70 @@
       <c r="K43" s="23"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="65" t="str" cm="1">
+      <c r="A44" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A44" ca="1">"void TesteSoma"&amp;INDIRECT("A"&amp;K28+3)&amp;"(CuTest *tc){"</f>
         <v>void TesteSoma4(CuTest *tc){</v>
       </c>
-      <c r="B44" s="65"/>
-      <c r="C44" s="65"/>
-      <c r="D44" s="65"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="66"/>
+      <c r="D44" s="66"/>
       <c r="K44" s="23"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="65" t="str" cm="1">
+      <c r="A45" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A45" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;5+(K28-1)*2)&amp;""";"</f>
         <v>char * input1 = "11111111";</v>
       </c>
-      <c r="B45" s="65"/>
-      <c r="C45" s="65"/>
-      <c r="D45" s="65"/>
+      <c r="B45" s="66"/>
+      <c r="C45" s="66"/>
+      <c r="D45" s="66"/>
       <c r="K45" s="23"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="65" t="str" cm="1">
+      <c r="A46" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A46" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;5+(K28-1)*2)&amp;""";"</f>
         <v>char * input2 = "10000000";</v>
       </c>
-      <c r="B46" s="65"/>
-      <c r="C46" s="65"/>
-      <c r="D46" s="65"/>
+      <c r="B46" s="66"/>
+      <c r="C46" s="66"/>
+      <c r="D46" s="66"/>
       <c r="K46" s="23"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="65" t="s">
+      <c r="A47" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="65"/>
-      <c r="C47" s="65"/>
-      <c r="D47" s="65"/>
+      <c r="B47" s="66"/>
+      <c r="C47" s="66"/>
+      <c r="D47" s="66"/>
       <c r="K47" s="23"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="65" t="str" cm="1">
+      <c r="A48" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A48" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;5+(K28-1)*2)&amp;""";"</f>
         <v>char * expected = "101111111";</v>
       </c>
-      <c r="B48" s="65"/>
-      <c r="C48" s="65"/>
-      <c r="D48" s="65"/>
+      <c r="B48" s="66"/>
+      <c r="C48" s="66"/>
+      <c r="D48" s="66"/>
       <c r="K48" s="23"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="65" t="s">
+      <c r="A49" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="B49" s="65"/>
-      <c r="C49" s="65"/>
-      <c r="D49" s="65"/>
+      <c r="B49" s="66"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="66"/>
       <c r="K49" s="23"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="65" t="s">
+      <c r="A50" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="65"/>
-      <c r="C50" s="65"/>
-      <c r="D50" s="65"/>
+      <c r="B50" s="66"/>
+      <c r="C50" s="66"/>
+      <c r="D50" s="66"/>
       <c r="K50" s="23"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -5721,66 +5727,66 @@
       <c r="K51" s="23"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="65" t="str" cm="1">
+      <c r="A52" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A52" ca="1">"void TesteSub"&amp;INDIRECT("A"&amp;K28+3)&amp;"(CuTest *tc){"</f>
         <v>void TesteSub4(CuTest *tc){</v>
       </c>
-      <c r="B52" s="65"/>
-      <c r="C52" s="65"/>
-      <c r="D52" s="65"/>
+      <c r="B52" s="66"/>
+      <c r="C52" s="66"/>
+      <c r="D52" s="66"/>
       <c r="K52" s="23"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="65" t="str" cm="1">
+      <c r="A53" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A53" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;6+(K28-1)*2)&amp;""";"</f>
         <v>char * input1 = "11111111";</v>
       </c>
-      <c r="B53" s="65"/>
-      <c r="C53" s="65"/>
-      <c r="D53" s="65"/>
+      <c r="B53" s="66"/>
+      <c r="C53" s="66"/>
+      <c r="D53" s="66"/>
       <c r="K53" s="23"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="65" t="str" cm="1">
+      <c r="A54" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A54" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;6+(K28-1)*2)&amp;""";"</f>
         <v>char * input2 = "10000000";</v>
       </c>
-      <c r="B54" s="65"/>
-      <c r="C54" s="65"/>
-      <c r="D54" s="65"/>
+      <c r="B54" s="66"/>
+      <c r="C54" s="66"/>
+      <c r="D54" s="66"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="65" t="s">
+      <c r="A55" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="65"/>
-      <c r="C55" s="65"/>
-      <c r="D55" s="65"/>
+      <c r="B55" s="66"/>
+      <c r="C55" s="66"/>
+      <c r="D55" s="66"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="65" t="str" cm="1">
+      <c r="A56" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A56" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;6+(K28-1)*2)&amp;""";"</f>
-        <v>char * expected = "001111111";</v>
-      </c>
-      <c r="B56" s="65"/>
-      <c r="C56" s="65"/>
-      <c r="D56" s="65"/>
+        <v>char * expected = "101111111";</v>
+      </c>
+      <c r="B56" s="66"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="66"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="65" t="s">
+      <c r="A57" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="B57" s="65"/>
-      <c r="C57" s="65"/>
-      <c r="D57" s="65"/>
+      <c r="B57" s="66"/>
+      <c r="C57" s="66"/>
+      <c r="D57" s="66"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="65" t="s">
+      <c r="A58" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B58" s="65"/>
-      <c r="C58" s="65"/>
-      <c r="D58" s="65"/>
+      <c r="B58" s="66"/>
+      <c r="C58" s="66"/>
+      <c r="D58" s="66"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="60"/>
@@ -5799,23 +5805,8 @@
     <sortCondition ref="B3:B26"/>
     <sortCondition ref="E3:E26"/>
   </sortState>
-  <mergeCells count="33">
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
+  <mergeCells count="32">
+    <mergeCell ref="A45:D45"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A47:D47"/>
     <mergeCell ref="A37:D37"/>
@@ -5832,7 +5823,21 @@
     <mergeCell ref="A52:D52"/>
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adicionado o arquivo da licença do software de teste unitário
Adicionado o arquivo license_CuTest.txt referente à licença de uso do software de teste unitário Cutest (https://cutest.sourceforge.net/) e outras mudanças cosméticas.
</commit_message>
<xml_diff>
--- a/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
+++ b/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3162c0a97888194f/Documentos/GitHub/algoritmos/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="916" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2ACF37C3-393F-4491-98D0-5134FBAFEC64}"/>
+  <xr:revisionPtr revIDLastSave="920" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FE43E44-26AF-4843-AB8E-504B4FCA11E0}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="4485" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
+    <workbookView xWindow="3750" yWindow="825" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="numeros_binarios_8bits" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="45">
   <si>
     <t>op</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t xml:space="preserve">(v2 = c2)&amp;(msb = 1): erro </t>
+  </si>
+  <si>
+    <t>Ação</t>
   </si>
 </sst>
 </file>
@@ -357,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -432,22 +435,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="dashed">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -627,16 +621,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutro" xfId="2" builtinId="28"/>
@@ -4447,8 +4440,8 @@
   </sheetPr>
   <dimension ref="A2:M59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4464,7 +4457,7 @@
     <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.85546875" customWidth="1"/>
     <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -4507,6 +4500,9 @@
       <c r="L2" s="10" t="s">
         <v>11</v>
       </c>
+      <c r="M2" s="10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
@@ -4548,6 +4544,7 @@
       <c r="L3" s="27" t="s">
         <v>1</v>
       </c>
+      <c r="M3" s="27"/>
     </row>
     <row r="4" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
@@ -4589,6 +4586,7 @@
       <c r="L4" s="27" t="s">
         <v>6</v>
       </c>
+      <c r="M4" s="27"/>
     </row>
     <row r="5" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
@@ -4630,6 +4628,7 @@
       <c r="L5" s="30" t="s">
         <v>6</v>
       </c>
+      <c r="M5" s="30"/>
     </row>
     <row r="6" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
@@ -4671,6 +4670,7 @@
       <c r="L6" s="30" t="s">
         <v>1</v>
       </c>
+      <c r="M6" s="30"/>
     </row>
     <row r="7" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
@@ -4712,6 +4712,7 @@
       <c r="L7" s="33" t="s">
         <v>6</v>
       </c>
+      <c r="M7" s="33"/>
     </row>
     <row r="8" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
@@ -4753,6 +4754,7 @@
       <c r="L8" s="33" t="s">
         <v>1</v>
       </c>
+      <c r="M8" s="33"/>
     </row>
     <row r="9" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36">
@@ -4794,6 +4796,7 @@
       <c r="L9" s="36" t="s">
         <v>1</v>
       </c>
+      <c r="M9" s="36"/>
     </row>
     <row r="10" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="52">
@@ -4834,7 +4837,7 @@
       <c r="L10" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="52" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4878,7 +4881,7 @@
       <c r="L11" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="M11" s="68"/>
+      <c r="M11" s="39"/>
     </row>
     <row r="12" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="39">
@@ -4919,7 +4922,7 @@
       <c r="L12" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="M12" s="68" t="s">
+      <c r="M12" s="52" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4963,6 +4966,7 @@
       <c r="L13" s="42" t="s">
         <v>1</v>
       </c>
+      <c r="M13" s="42"/>
     </row>
     <row r="14" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
@@ -5004,6 +5008,7 @@
       <c r="L14" s="42" t="s">
         <v>6</v>
       </c>
+      <c r="M14" s="42"/>
     </row>
     <row r="15" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
@@ -5045,6 +5050,7 @@
       <c r="L15" s="11" t="s">
         <v>6</v>
       </c>
+      <c r="M15" s="11"/>
     </row>
     <row r="16" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
@@ -5085,11 +5091,11 @@
       <c r="L16" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="M16" s="68" t="s">
+      <c r="M16" s="52" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>15</v>
       </c>
@@ -5129,8 +5135,9 @@
       <c r="L17" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M17" s="14"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>16</v>
       </c>
@@ -5170,8 +5177,9 @@
       <c r="L18" s="14" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M18" s="14"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>17</v>
       </c>
@@ -5211,8 +5219,9 @@
       <c r="L19" s="17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M19" s="17"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>18</v>
       </c>
@@ -5252,8 +5261,9 @@
       <c r="L20" s="17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M20" s="17"/>
+    </row>
+    <row r="21" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="45">
         <v>19</v>
       </c>
@@ -5293,8 +5303,9 @@
       <c r="L21" s="45" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M21" s="45"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="45">
         <v>20</v>
       </c>
@@ -5334,8 +5345,9 @@
       <c r="L22" s="45" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M22" s="45"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="48">
         <v>21</v>
       </c>
@@ -5375,8 +5387,9 @@
       <c r="L23" s="48" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M23" s="48"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="48">
         <v>22</v>
       </c>
@@ -5416,8 +5429,9 @@
       <c r="L24" s="48" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M24" s="48"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>23</v>
       </c>
@@ -5457,8 +5471,9 @@
       <c r="L25" s="20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M25" s="20"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>24</v>
       </c>
@@ -5498,77 +5513,78 @@
       <c r="L26" s="20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="65" t="str" cm="1">
+      <c r="M26" s="20"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A28" ca="1">"void TesteSoma"&amp;INDIRECT("A"&amp;K28+2)&amp;"(CuTest *tc){"</f>
         <v>void TesteSoma3(CuTest *tc){</v>
       </c>
-      <c r="B28" s="65"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="65"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
       <c r="K28" s="51">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="65" t="str" cm="1">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A29" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;3+(K28-1)*2)&amp;""";"</f>
         <v>char * input1 = "10000000";</v>
       </c>
-      <c r="B29" s="65"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="65"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
       <c r="E29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="65" t="str" cm="1">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A30" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;3+(K28-1)*2)&amp;""";"</f>
         <v>char * input2 = "01111111";</v>
       </c>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="65"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
       <c r="K30" s="23"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="65" t="s">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="65"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
       <c r="K31" s="23"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="65" t="str" cm="1">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A32" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;3+(K28-1)*2)&amp;""";"</f>
         <v>char * expected = "111111111";</v>
       </c>
-      <c r="B32" s="65"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="66"/>
       <c r="K32" s="23"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="65" t="s">
+      <c r="A33" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="65"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="65"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
       <c r="K33" s="23"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="65" t="s">
+      <c r="A34" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="65"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
       <c r="K34" s="23"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -5579,70 +5595,70 @@
       <c r="K35" s="23"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="65" t="str" cm="1">
+      <c r="A36" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A36" ca="1">"void TesteSub"&amp;INDIRECT("A"&amp;K28+2)&amp;"(CuTest *tc){"</f>
         <v>void TesteSub3(CuTest *tc){</v>
       </c>
-      <c r="B36" s="65"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="65"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
       <c r="K36" s="23"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="65" t="str" cm="1">
+      <c r="A37" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A37" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;4+(K28-1)*2)&amp;""";"</f>
         <v>char * input1 = "10000000";</v>
       </c>
-      <c r="B37" s="65"/>
-      <c r="C37" s="65"/>
-      <c r="D37" s="65"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
       <c r="K37" s="23"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="65" t="str" cm="1">
+      <c r="A38" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A38" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;4+(K28-1)*2)&amp;""";"</f>
         <v>char * input2 = "01111111";</v>
       </c>
-      <c r="B38" s="65"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="65"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
       <c r="K38" s="23"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="65" t="s">
+      <c r="A39" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="65"/>
-      <c r="C39" s="65"/>
-      <c r="D39" s="65"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="66"/>
+      <c r="D39" s="66"/>
       <c r="K39" s="23"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="65" t="str" cm="1">
+      <c r="A40" s="66" t="str" cm="1">
         <f t="array" aca="1" ref="A40" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;4+(K28-1)*2)&amp;""";"</f>
         <v>char * expected = "100000001";</v>
       </c>
-      <c r="B40" s="65"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="65"/>
+      <c r="B40" s="66"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
       <c r="K40" s="23"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="65" t="s">
+      <c r="A41" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="65"/>
-      <c r="C41" s="65"/>
-      <c r="D41" s="65"/>
+      <c r="B41" s="66"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66"/>
       <c r="K41" s="23"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="65" t="s">
+      <c r="A42" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="65"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="66"/>
       <c r="K42" s="23"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -5653,70 +5669,70 @@
       <c r="K43" s="23"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="66" t="str" cm="1">
+      <c r="A44" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A44" ca="1">"void TesteSoma"&amp;INDIRECT("A"&amp;K28+3)&amp;"(CuTest *tc){"</f>
         <v>void TesteSoma4(CuTest *tc){</v>
       </c>
-      <c r="B44" s="66"/>
-      <c r="C44" s="66"/>
-      <c r="D44" s="66"/>
+      <c r="B44" s="65"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="65"/>
       <c r="K44" s="23"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="66" t="str" cm="1">
+      <c r="A45" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A45" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;5+(K28-1)*2)&amp;""";"</f>
         <v>char * input1 = "11111111";</v>
       </c>
-      <c r="B45" s="66"/>
-      <c r="C45" s="66"/>
-      <c r="D45" s="66"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65"/>
       <c r="K45" s="23"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="66" t="str" cm="1">
+      <c r="A46" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A46" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;5+(K28-1)*2)&amp;""";"</f>
         <v>char * input2 = "10000000";</v>
       </c>
-      <c r="B46" s="66"/>
-      <c r="C46" s="66"/>
-      <c r="D46" s="66"/>
+      <c r="B46" s="65"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="65"/>
       <c r="K46" s="23"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="66"/>
-      <c r="C47" s="66"/>
-      <c r="D47" s="66"/>
+      <c r="B47" s="65"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="65"/>
       <c r="K47" s="23"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="66" t="str" cm="1">
+      <c r="A48" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A48" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;5+(K28-1)*2)&amp;""";"</f>
         <v>char * expected = "101111111";</v>
       </c>
-      <c r="B48" s="66"/>
-      <c r="C48" s="66"/>
-      <c r="D48" s="66"/>
+      <c r="B48" s="65"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="65"/>
       <c r="K48" s="23"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="66" t="s">
+      <c r="A49" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="B49" s="66"/>
-      <c r="C49" s="66"/>
-      <c r="D49" s="66"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="65"/>
       <c r="K49" s="23"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="66" t="s">
+      <c r="A50" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="66"/>
-      <c r="C50" s="66"/>
-      <c r="D50" s="66"/>
+      <c r="B50" s="65"/>
+      <c r="C50" s="65"/>
+      <c r="D50" s="65"/>
       <c r="K50" s="23"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -5727,66 +5743,66 @@
       <c r="K51" s="23"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="66" t="str" cm="1">
+      <c r="A52" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A52" ca="1">"void TesteSub"&amp;INDIRECT("A"&amp;K28+3)&amp;"(CuTest *tc){"</f>
         <v>void TesteSub4(CuTest *tc){</v>
       </c>
-      <c r="B52" s="66"/>
-      <c r="C52" s="66"/>
-      <c r="D52" s="66"/>
+      <c r="B52" s="65"/>
+      <c r="C52" s="65"/>
+      <c r="D52" s="65"/>
       <c r="K52" s="23"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="66" t="str" cm="1">
+      <c r="A53" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A53" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;6+(K28-1)*2)&amp;""";"</f>
         <v>char * input1 = "11111111";</v>
       </c>
-      <c r="B53" s="66"/>
-      <c r="C53" s="66"/>
-      <c r="D53" s="66"/>
+      <c r="B53" s="65"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="65"/>
       <c r="K53" s="23"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="66" t="str" cm="1">
+      <c r="A54" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A54" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;6+(K28-1)*2)&amp;""";"</f>
         <v>char * input2 = "10000000";</v>
       </c>
-      <c r="B54" s="66"/>
-      <c r="C54" s="66"/>
-      <c r="D54" s="66"/>
+      <c r="B54" s="65"/>
+      <c r="C54" s="65"/>
+      <c r="D54" s="65"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="66" t="s">
+      <c r="A55" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="66"/>
-      <c r="C55" s="66"/>
-      <c r="D55" s="66"/>
+      <c r="B55" s="65"/>
+      <c r="C55" s="65"/>
+      <c r="D55" s="65"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="66" t="str" cm="1">
+      <c r="A56" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A56" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;6+(K28-1)*2)&amp;""";"</f>
         <v>char * expected = "101111111";</v>
       </c>
-      <c r="B56" s="66"/>
-      <c r="C56" s="66"/>
-      <c r="D56" s="66"/>
+      <c r="B56" s="65"/>
+      <c r="C56" s="65"/>
+      <c r="D56" s="65"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="66" t="s">
+      <c r="A57" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="B57" s="66"/>
-      <c r="C57" s="66"/>
-      <c r="D57" s="66"/>
+      <c r="B57" s="65"/>
+      <c r="C57" s="65"/>
+      <c r="D57" s="65"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="66" t="s">
+      <c r="A58" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="B58" s="66"/>
-      <c r="C58" s="66"/>
-      <c r="D58" s="66"/>
+      <c r="B58" s="65"/>
+      <c r="C58" s="65"/>
+      <c r="D58" s="65"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="60"/>
@@ -5806,26 +5822,6 @@
     <sortCondition ref="E3:E26"/>
   </sortState>
   <mergeCells count="32">
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A35:D35"/>
     <mergeCell ref="A48:D48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:D29"/>
@@ -5838,6 +5834,26 @@
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A35:D35"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Funcionando com 10 bits
funcionando com 10 bits
</commit_message>
<xml_diff>
--- a/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
+++ b/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3162c0a97888194f/Documentos/GitHub/algoritmos/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="920" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FE43E44-26AF-4843-AB8E-504B4FCA11E0}"/>
+  <xr:revisionPtr revIDLastSave="947" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5B48657-938F-428A-9D34-8399A5F93B2D}"/>
   <bookViews>
-    <workbookView xWindow="3750" yWindow="825" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
+    <workbookView xWindow="1500" yWindow="5295" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="numeros_binarios_8bits" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="42">
   <si>
     <t>op</t>
   </si>
@@ -176,28 +176,19 @@
     <t>sinal b9</t>
   </si>
   <si>
-    <t>101111111</t>
+    <t>Ação</t>
   </si>
   <si>
-    <t>1110000001</t>
+    <t>010000001</t>
   </si>
   <si>
-    <t>1111111111</t>
+    <t>0111111111</t>
   </si>
   <si>
-    <t>overflow</t>
+    <t>001111111</t>
   </si>
   <si>
-    <t>(v2 =  c2)&amp;(msb = 0): resetar msb</t>
-  </si>
-  <si>
-    <t>(v2 = c2)&amp;(msb = 1): erro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(v2 = c2)&amp;(msb = 1): erro </t>
-  </si>
-  <si>
-    <t>Ação</t>
+    <t>00</t>
   </si>
 </sst>
 </file>
@@ -4440,8 +4431,8 @@
   </sheetPr>
   <dimension ref="A2:M59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4501,7 +4492,7 @@
         <v>11</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4530,15 +4521,15 @@
         <v>-129</v>
       </c>
       <c r="I3" s="27" t="str">
-        <f t="shared" ref="I3:I26" si="0">RIGHT(DEC2BIN(H3,10),9)</f>
+        <f>RIGHT(DEC2BIN(H3,10),9)</f>
         <v>101111111</v>
       </c>
       <c r="J3" s="27" t="str">
-        <f t="shared" ref="J3:J26" si="1">MID(I3,1,1)</f>
+        <f t="shared" ref="J3:J26" si="0">MID(I3,1,1)</f>
         <v>1</v>
       </c>
       <c r="K3" s="27" t="str">
-        <f t="shared" ref="K3:K26" si="2">MID(I3,1,2)</f>
+        <f t="shared" ref="K3:K26" si="1">MID(I3,1,2)</f>
         <v>10</v>
       </c>
       <c r="L3" s="27" t="s">
@@ -4572,15 +4563,15 @@
         <v>-127</v>
       </c>
       <c r="I4" s="27" t="str">
+        <f>RIGHT(DEC2BIN(H4,10),9)</f>
+        <v>110000001</v>
+      </c>
+      <c r="J4" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>110000001</v>
-      </c>
-      <c r="J4" s="27" t="str">
+        <v>1</v>
+      </c>
+      <c r="K4" s="27" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K4" s="27" t="str">
-        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L4" s="27" t="s">
@@ -4614,15 +4605,15 @@
         <v>-127</v>
       </c>
       <c r="I5" s="30" t="str">
+        <f>RIGHT(DEC2BIN(H5,10),9)</f>
+        <v>110000001</v>
+      </c>
+      <c r="J5" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>110000001</v>
-      </c>
-      <c r="J5" s="30" t="str">
+        <v>1</v>
+      </c>
+      <c r="K5" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K5" s="30" t="str">
-        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L5" s="30" t="s">
@@ -4656,16 +4647,16 @@
         <v>-129</v>
       </c>
       <c r="I6" s="30" t="str">
+        <f>RIGHT(DEC2BIN(H6,10),10)</f>
+        <v>1101111111</v>
+      </c>
+      <c r="J6" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>101111111</v>
-      </c>
-      <c r="J6" s="30" t="str">
+        <v>1</v>
+      </c>
+      <c r="K6" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K6" s="30" t="str">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L6" s="30" t="s">
         <v>1</v>
@@ -4698,15 +4689,15 @@
         <v>-1</v>
       </c>
       <c r="I7" s="33" t="str">
+        <f t="shared" ref="I4:I26" si="2">RIGHT(DEC2BIN(H7,10),9)</f>
+        <v>111111111</v>
+      </c>
+      <c r="J7" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>111111111</v>
-      </c>
-      <c r="J7" s="33" t="str">
+        <v>1</v>
+      </c>
+      <c r="K7" s="33" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K7" s="33" t="str">
-        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L7" s="33" t="s">
@@ -4740,15 +4731,15 @@
         <v>-255</v>
       </c>
       <c r="I8" s="33" t="str">
+        <f t="shared" si="2"/>
+        <v>100000001</v>
+      </c>
+      <c r="J8" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>100000001</v>
-      </c>
-      <c r="J8" s="33" t="str">
+        <v>1</v>
+      </c>
+      <c r="K8" s="33" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K8" s="33" t="str">
-        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="L8" s="33" t="s">
@@ -4782,15 +4773,15 @@
         <v>-129</v>
       </c>
       <c r="I9" s="36" t="str">
+        <f t="shared" si="2"/>
+        <v>101111111</v>
+      </c>
+      <c r="J9" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>101111111</v>
-      </c>
-      <c r="J9" s="36" t="str">
+        <v>1</v>
+      </c>
+      <c r="K9" s="36" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K9" s="36" t="str">
-        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="L9" s="36" t="s">
@@ -4824,22 +4815,19 @@
         <v>127</v>
       </c>
       <c r="I10" s="54" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J10" s="52" t="str">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K10" s="52" t="str">
-        <f>MID(I10,1,2)&amp;" NA"</f>
-        <v>10 NA</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="54" t="s">
+        <v>41</v>
       </c>
       <c r="L10" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="52" t="s">
-        <v>41</v>
-      </c>
+      <c r="M10" s="52"/>
     </row>
     <row r="11" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="39">
@@ -4867,15 +4855,15 @@
         <v>-127</v>
       </c>
       <c r="I11" s="39" t="str">
+        <f t="shared" si="2"/>
+        <v>110000001</v>
+      </c>
+      <c r="J11" s="39" t="str">
         <f t="shared" si="0"/>
-        <v>110000001</v>
-      </c>
-      <c r="J11" s="39" t="str">
+        <v>1</v>
+      </c>
+      <c r="K11" s="39" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K11" s="39" t="str">
-        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L11" s="39" t="s">
@@ -4884,7 +4872,7 @@
       <c r="M11" s="39"/>
     </row>
     <row r="12" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39">
+      <c r="A12" s="52">
         <v>10</v>
       </c>
       <c r="B12" s="52">
@@ -4912,19 +4900,17 @@
         <v>38</v>
       </c>
       <c r="J12" s="52" t="str">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="K12" s="52" t="str">
-        <f>MID(I12,1,2)&amp;" NA"</f>
-        <v>11 NA</v>
+        <f>MID(I12,1,2)</f>
+        <v>01</v>
       </c>
       <c r="L12" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="M12" s="52" t="s">
-        <v>42</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M12" s="52"/>
     </row>
     <row r="13" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
@@ -4952,15 +4938,15 @@
         <v>128</v>
       </c>
       <c r="I13" s="42" t="str">
+        <f t="shared" si="2"/>
+        <v>010000000</v>
+      </c>
+      <c r="J13" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>010000000</v>
-      </c>
-      <c r="J13" s="42" t="str">
+        <v>0</v>
+      </c>
+      <c r="K13" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="42" t="str">
-        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="L13" s="42" t="s">
@@ -4994,15 +4980,15 @@
         <v>-126</v>
       </c>
       <c r="I14" s="42" t="str">
+        <f t="shared" si="2"/>
+        <v>110000010</v>
+      </c>
+      <c r="J14" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>110000010</v>
-      </c>
-      <c r="J14" s="42" t="str">
+        <v>1</v>
+      </c>
+      <c r="K14" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K14" s="42" t="str">
-        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L14" s="42" t="s">
@@ -5036,15 +5022,15 @@
         <v>-1</v>
       </c>
       <c r="I15" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>111111111</v>
+      </c>
+      <c r="J15" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>111111111</v>
-      </c>
-      <c r="J15" s="11" t="str">
+        <v>1</v>
+      </c>
+      <c r="K15" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K15" s="11" t="str">
-        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L15" s="11" t="s">
@@ -5053,7 +5039,7 @@
       <c r="M15" s="11"/>
     </row>
     <row r="16" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+      <c r="A16" s="52">
         <v>14</v>
       </c>
       <c r="B16" s="52">
@@ -5081,19 +5067,17 @@
         <v>39</v>
       </c>
       <c r="J16" s="52" t="str">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="K16" s="52" t="str">
-        <f>MID(I16,1,2)&amp;" NA"</f>
-        <v>11 NA</v>
+        <f>MID(I16,1,2)</f>
+        <v>01</v>
       </c>
       <c r="L16" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="M16" s="52" t="s">
-        <v>43</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M16" s="52"/>
     </row>
     <row r="17" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
@@ -5121,15 +5105,15 @@
         <v>126</v>
       </c>
       <c r="I17" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>001111110</v>
+      </c>
+      <c r="J17" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>001111110</v>
-      </c>
-      <c r="J17" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="K17" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="14" t="str">
-        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="L17" s="14" t="s">
@@ -5163,15 +5147,15 @@
         <v>128</v>
       </c>
       <c r="I18" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>010000000</v>
+      </c>
+      <c r="J18" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>010000000</v>
-      </c>
-      <c r="J18" s="14" t="str">
+        <v>0</v>
+      </c>
+      <c r="K18" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="14" t="str">
-        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="L18" s="14" t="s">
@@ -5205,15 +5189,15 @@
         <v>128</v>
       </c>
       <c r="I19" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>010000000</v>
+      </c>
+      <c r="J19" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>010000000</v>
-      </c>
-      <c r="J19" s="17" t="str">
+        <v>0</v>
+      </c>
+      <c r="K19" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="17" t="str">
-        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="L19" s="17" t="s">
@@ -5247,15 +5231,15 @@
         <v>126</v>
       </c>
       <c r="I20" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>001111110</v>
+      </c>
+      <c r="J20" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>001111110</v>
-      </c>
-      <c r="J20" s="17" t="str">
+        <v>0</v>
+      </c>
+      <c r="K20" s="17" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="17" t="str">
-        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="L20" s="17" t="s">
@@ -5289,15 +5273,15 @@
         <v>0</v>
       </c>
       <c r="I21" s="45" t="str">
+        <f t="shared" si="2"/>
+        <v>000000000</v>
+      </c>
+      <c r="J21" s="45" t="str">
         <f t="shared" si="0"/>
-        <v>000000000</v>
-      </c>
-      <c r="J21" s="45" t="str">
+        <v>0</v>
+      </c>
+      <c r="K21" s="45" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K21" s="45" t="str">
-        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="L21" s="45" t="s">
@@ -5331,15 +5315,15 @@
         <v>-2</v>
       </c>
       <c r="I22" s="45" t="str">
+        <f t="shared" si="2"/>
+        <v>111111110</v>
+      </c>
+      <c r="J22" s="45" t="str">
         <f t="shared" si="0"/>
-        <v>111111110</v>
-      </c>
-      <c r="J22" s="45" t="str">
+        <v>1</v>
+      </c>
+      <c r="K22" s="45" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K22" s="45" t="str">
-        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L22" s="45" t="s">
@@ -5373,15 +5357,15 @@
         <v>126</v>
       </c>
       <c r="I23" s="48" t="str">
+        <f t="shared" si="2"/>
+        <v>001111110</v>
+      </c>
+      <c r="J23" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>001111110</v>
-      </c>
-      <c r="J23" s="48" t="str">
+        <v>0</v>
+      </c>
+      <c r="K23" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="48" t="str">
-        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="L23" s="48" t="s">
@@ -5415,15 +5399,15 @@
         <v>-128</v>
       </c>
       <c r="I24" s="48" t="str">
+        <f t="shared" si="2"/>
+        <v>110000000</v>
+      </c>
+      <c r="J24" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>110000000</v>
-      </c>
-      <c r="J24" s="48" t="str">
+        <v>1</v>
+      </c>
+      <c r="K24" s="48" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K24" s="48" t="str">
-        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="L24" s="48" t="s">
@@ -5457,15 +5441,15 @@
         <v>0</v>
       </c>
       <c r="I25" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>000000000</v>
+      </c>
+      <c r="J25" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>000000000</v>
-      </c>
-      <c r="J25" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="K25" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="20" t="str">
-        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="L25" s="20" t="s">
@@ -5499,15 +5483,15 @@
         <v>2</v>
       </c>
       <c r="I26" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>000000010</v>
+      </c>
+      <c r="J26" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>000000010</v>
-      </c>
-      <c r="J26" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="K26" s="20" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K26" s="20" t="str">
-        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="L26" s="20" t="s">
@@ -5782,7 +5766,7 @@
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="65" t="str" cm="1">
         <f t="array" aca="1" ref="A56" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;6+(K28-1)*2)&amp;""";"</f>
-        <v>char * expected = "101111111";</v>
+        <v>char * expected = "001111111";</v>
       </c>
       <c r="B56" s="65"/>
       <c r="C56" s="65"/>
@@ -5822,6 +5806,22 @@
     <sortCondition ref="E3:E26"/>
   </sortState>
   <mergeCells count="32">
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A53:D53"/>
     <mergeCell ref="A48:D48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:D29"/>
@@ -5834,26 +5834,10 @@
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A58:D58"/>
     <mergeCell ref="A45:D45"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A47:D47"/>
     <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A35:D35"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Passou no testes de soma e subtração
Passou no testes de soma e subtração
</commit_message>
<xml_diff>
--- a/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
+++ b/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3162c0a97888194f/Documentos/GitHub/algoritmos/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="947" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5B48657-938F-428A-9D34-8399A5F93B2D}"/>
+  <xr:revisionPtr revIDLastSave="952" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA04582F-2538-466D-B4F0-AE0045B217A2}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="5295" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="numeros_binarios_8bits" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="41">
   <si>
     <t>op</t>
   </si>
@@ -174,9 +174,6 @@
   </si>
   <si>
     <t>sinal b9</t>
-  </si>
-  <si>
-    <t>Ação</t>
   </si>
   <si>
     <t>010000001</t>
@@ -432,7 +429,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -575,15 +572,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1004,7 +992,7 @@
       <c r="B2" s="25">
         <v>-129</v>
       </c>
-      <c r="C2" s="56" t="str">
+      <c r="C2" s="53" t="str">
         <f>RIGHT(DEC2BIN(B2,8),10)</f>
         <v>1101111111</v>
       </c>
@@ -1047,7 +1035,7 @@
       <c r="B3">
         <v>-128</v>
       </c>
-      <c r="C3" s="57" t="str">
+      <c r="C3" s="54" t="str">
         <f>RIGHT(DEC2BIN(B3,8),10)</f>
         <v>1110000000</v>
       </c>
@@ -1084,19 +1072,19 @@
         <v>01010100</v>
       </c>
       <c r="P3" s="8"/>
-      <c r="R3" s="59" t="s">
+      <c r="R3" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="59"/>
-      <c r="T3" s="59"/>
-      <c r="U3" s="59"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="56"/>
+      <c r="U3" s="56"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4">
         <v>-127</v>
       </c>
-      <c r="C4" s="58" t="str">
+      <c r="C4" s="55" t="str">
         <f t="shared" ref="C4" si="3">RIGHT(DEC2BIN(B4,8),8)</f>
         <v>10000001</v>
       </c>
@@ -1133,19 +1121,19 @@
         <v>01010101</v>
       </c>
       <c r="P4" s="8"/>
-      <c r="R4" s="59" t="s">
+      <c r="R4" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="S4" s="59"/>
-      <c r="T4" s="59"/>
-      <c r="U4" s="59"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5">
         <v>-126</v>
       </c>
-      <c r="C5" s="58" t="str">
+      <c r="C5" s="55" t="str">
         <f t="shared" ref="C5:C26" si="4">RIGHT(DEC2BIN(B5,8),8)</f>
         <v>10000010</v>
       </c>
@@ -1182,19 +1170,19 @@
         <v>01010110</v>
       </c>
       <c r="P5" s="8"/>
-      <c r="R5" s="59" t="s">
+      <c r="R5" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="S5" s="59"/>
-      <c r="T5" s="59"/>
-      <c r="U5" s="59"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="56"/>
+      <c r="U5" s="56"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6">
         <v>-125</v>
       </c>
-      <c r="C6" s="58" t="str">
+      <c r="C6" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10000011</v>
       </c>
@@ -1237,7 +1225,7 @@
       <c r="B7">
         <v>-124</v>
       </c>
-      <c r="C7" s="58" t="str">
+      <c r="C7" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10000100</v>
       </c>
@@ -1280,7 +1268,7 @@
       <c r="B8">
         <v>-123</v>
       </c>
-      <c r="C8" s="58" t="str">
+      <c r="C8" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10000101</v>
       </c>
@@ -1323,7 +1311,7 @@
       <c r="B9">
         <v>-122</v>
       </c>
-      <c r="C9" s="58" t="str">
+      <c r="C9" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10000110</v>
       </c>
@@ -1373,7 +1361,7 @@
       <c r="B10">
         <v>-121</v>
       </c>
-      <c r="C10" s="58" t="str">
+      <c r="C10" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10000111</v>
       </c>
@@ -1410,7 +1398,7 @@
         <v>01011011</v>
       </c>
       <c r="P10" s="8"/>
-      <c r="T10" s="55">
+      <c r="T10" s="52">
         <v>1110000000</v>
       </c>
       <c r="U10">
@@ -1423,7 +1411,7 @@
       <c r="B11">
         <v>-120</v>
       </c>
-      <c r="C11" s="58" t="str">
+      <c r="C11" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10001000</v>
       </c>
@@ -1466,7 +1454,7 @@
       <c r="B12">
         <v>-119</v>
       </c>
-      <c r="C12" s="58" t="str">
+      <c r="C12" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10001001</v>
       </c>
@@ -1509,7 +1497,7 @@
       <c r="B13">
         <v>-118</v>
       </c>
-      <c r="C13" s="58" t="str">
+      <c r="C13" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10001010</v>
       </c>
@@ -1552,7 +1540,7 @@
       <c r="B14">
         <v>-117</v>
       </c>
-      <c r="C14" s="58" t="str">
+      <c r="C14" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10001011</v>
       </c>
@@ -1595,7 +1583,7 @@
       <c r="B15">
         <v>-116</v>
       </c>
-      <c r="C15" s="58" t="str">
+      <c r="C15" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10001100</v>
       </c>
@@ -1638,7 +1626,7 @@
       <c r="B16">
         <v>-115</v>
       </c>
-      <c r="C16" s="58" t="str">
+      <c r="C16" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10001101</v>
       </c>
@@ -1681,7 +1669,7 @@
       <c r="B17">
         <v>-114</v>
       </c>
-      <c r="C17" s="58" t="str">
+      <c r="C17" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10001110</v>
       </c>
@@ -1724,7 +1712,7 @@
       <c r="B18">
         <v>-113</v>
       </c>
-      <c r="C18" s="58" t="str">
+      <c r="C18" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10001111</v>
       </c>
@@ -1767,7 +1755,7 @@
       <c r="B19">
         <v>-112</v>
       </c>
-      <c r="C19" s="58" t="str">
+      <c r="C19" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10010000</v>
       </c>
@@ -1810,7 +1798,7 @@
       <c r="B20">
         <v>-111</v>
       </c>
-      <c r="C20" s="58" t="str">
+      <c r="C20" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10010001</v>
       </c>
@@ -1853,7 +1841,7 @@
       <c r="B21">
         <v>-110</v>
       </c>
-      <c r="C21" s="58" t="str">
+      <c r="C21" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10010010</v>
       </c>
@@ -1896,7 +1884,7 @@
       <c r="B22">
         <v>-109</v>
       </c>
-      <c r="C22" s="58" t="str">
+      <c r="C22" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10010011</v>
       </c>
@@ -1939,7 +1927,7 @@
       <c r="B23">
         <v>-108</v>
       </c>
-      <c r="C23" s="58" t="str">
+      <c r="C23" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10010100</v>
       </c>
@@ -1982,7 +1970,7 @@
       <c r="B24">
         <v>-107</v>
       </c>
-      <c r="C24" s="58" t="str">
+      <c r="C24" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10010101</v>
       </c>
@@ -2025,7 +2013,7 @@
       <c r="B25">
         <v>-106</v>
       </c>
-      <c r="C25" s="58" t="str">
+      <c r="C25" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10010110</v>
       </c>
@@ -2068,7 +2056,7 @@
       <c r="B26">
         <v>-105</v>
       </c>
-      <c r="C26" s="58" t="str">
+      <c r="C26" s="55" t="str">
         <f t="shared" si="4"/>
         <v>10010111</v>
       </c>
@@ -2111,7 +2099,7 @@
       <c r="B27">
         <v>-104</v>
       </c>
-      <c r="C27" s="58" t="str">
+      <c r="C27" s="55" t="str">
         <f t="shared" ref="C27:C54" si="6">RIGHT(DEC2BIN(B27,8),8)</f>
         <v>10011000</v>
       </c>
@@ -2154,7 +2142,7 @@
       <c r="B28">
         <v>-103</v>
       </c>
-      <c r="C28" s="58" t="str">
+      <c r="C28" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10011001</v>
       </c>
@@ -2197,7 +2185,7 @@
       <c r="B29">
         <v>-102</v>
       </c>
-      <c r="C29" s="58" t="str">
+      <c r="C29" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10011010</v>
       </c>
@@ -2240,7 +2228,7 @@
       <c r="B30">
         <v>-101</v>
       </c>
-      <c r="C30" s="58" t="str">
+      <c r="C30" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10011011</v>
       </c>
@@ -2283,7 +2271,7 @@
       <c r="B31">
         <v>-100</v>
       </c>
-      <c r="C31" s="58" t="str">
+      <c r="C31" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10011100</v>
       </c>
@@ -2326,7 +2314,7 @@
       <c r="B32">
         <v>-99</v>
       </c>
-      <c r="C32" s="58" t="str">
+      <c r="C32" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10011101</v>
       </c>
@@ -2369,7 +2357,7 @@
       <c r="B33">
         <v>-98</v>
       </c>
-      <c r="C33" s="58" t="str">
+      <c r="C33" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10011110</v>
       </c>
@@ -2412,7 +2400,7 @@
       <c r="B34">
         <v>-97</v>
       </c>
-      <c r="C34" s="58" t="str">
+      <c r="C34" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10011111</v>
       </c>
@@ -2455,7 +2443,7 @@
       <c r="B35">
         <v>-96</v>
       </c>
-      <c r="C35" s="58" t="str">
+      <c r="C35" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10100000</v>
       </c>
@@ -2498,7 +2486,7 @@
       <c r="B36">
         <v>-95</v>
       </c>
-      <c r="C36" s="58" t="str">
+      <c r="C36" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10100001</v>
       </c>
@@ -2541,7 +2529,7 @@
       <c r="B37">
         <v>-94</v>
       </c>
-      <c r="C37" s="58" t="str">
+      <c r="C37" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10100010</v>
       </c>
@@ -2584,7 +2572,7 @@
       <c r="B38">
         <v>-93</v>
       </c>
-      <c r="C38" s="58" t="str">
+      <c r="C38" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10100011</v>
       </c>
@@ -2627,7 +2615,7 @@
       <c r="B39">
         <v>-92</v>
       </c>
-      <c r="C39" s="58" t="str">
+      <c r="C39" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10100100</v>
       </c>
@@ -2670,7 +2658,7 @@
       <c r="B40">
         <v>-91</v>
       </c>
-      <c r="C40" s="58" t="str">
+      <c r="C40" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10100101</v>
       </c>
@@ -2713,7 +2701,7 @@
       <c r="B41">
         <v>-90</v>
       </c>
-      <c r="C41" s="58" t="str">
+      <c r="C41" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10100110</v>
       </c>
@@ -2756,7 +2744,7 @@
       <c r="B42">
         <v>-89</v>
       </c>
-      <c r="C42" s="58" t="str">
+      <c r="C42" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10100111</v>
       </c>
@@ -2799,7 +2787,7 @@
       <c r="B43">
         <v>-88</v>
       </c>
-      <c r="C43" s="58" t="str">
+      <c r="C43" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10101000</v>
       </c>
@@ -2842,7 +2830,7 @@
       <c r="B44">
         <v>-87</v>
       </c>
-      <c r="C44" s="58" t="str">
+      <c r="C44" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10101001</v>
       </c>
@@ -2885,7 +2873,7 @@
       <c r="B45">
         <v>-86</v>
       </c>
-      <c r="C45" s="58" t="str">
+      <c r="C45" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10101010</v>
       </c>
@@ -2928,7 +2916,7 @@
       <c r="B46">
         <v>-85</v>
       </c>
-      <c r="C46" s="58" t="str">
+      <c r="C46" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10101011</v>
       </c>
@@ -2971,7 +2959,7 @@
       <c r="B47">
         <v>-84</v>
       </c>
-      <c r="C47" s="58" t="str">
+      <c r="C47" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10101100</v>
       </c>
@@ -3014,7 +3002,7 @@
       <c r="B48">
         <v>-83</v>
       </c>
-      <c r="C48" s="58" t="str">
+      <c r="C48" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10101101</v>
       </c>
@@ -3057,7 +3045,7 @@
       <c r="B49">
         <v>-82</v>
       </c>
-      <c r="C49" s="58" t="str">
+      <c r="C49" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10101110</v>
       </c>
@@ -3100,7 +3088,7 @@
       <c r="B50">
         <v>-81</v>
       </c>
-      <c r="C50" s="58" t="str">
+      <c r="C50" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10101111</v>
       </c>
@@ -3143,7 +3131,7 @@
       <c r="B51">
         <v>-80</v>
       </c>
-      <c r="C51" s="58" t="str">
+      <c r="C51" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10110000</v>
       </c>
@@ -3186,7 +3174,7 @@
       <c r="B52">
         <v>-79</v>
       </c>
-      <c r="C52" s="58" t="str">
+      <c r="C52" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10110001</v>
       </c>
@@ -3229,7 +3217,7 @@
       <c r="B53">
         <v>-78</v>
       </c>
-      <c r="C53" s="58" t="str">
+      <c r="C53" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10110010</v>
       </c>
@@ -3272,7 +3260,7 @@
       <c r="B54">
         <v>-77</v>
       </c>
-      <c r="C54" s="58" t="str">
+      <c r="C54" s="55" t="str">
         <f t="shared" si="6"/>
         <v>10110011</v>
       </c>
@@ -3353,29 +3341,29 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
     </row>
     <row r="3" spans="1:22" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
@@ -3700,31 +3688,31 @@
       </c>
     </row>
     <row r="9" spans="1:22" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="62" t="s">
+      <c r="L9" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="63"/>
-      <c r="N9" s="63"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="63"/>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="63"/>
-      <c r="S9" s="63"/>
-      <c r="T9" s="63"/>
-      <c r="U9" s="64"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="60"/>
+      <c r="R9" s="60"/>
+      <c r="S9" s="60"/>
+      <c r="T9" s="60"/>
+      <c r="U9" s="61"/>
       <c r="V9" s="3"/>
     </row>
     <row r="10" spans="1:22" ht="21" x14ac:dyDescent="0.35">
@@ -3929,29 +3917,29 @@
       <c r="U16" s="1"/>
     </row>
     <row r="17" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="62"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="64"/>
+      <c r="A17" s="59"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="61"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="62" t="s">
+      <c r="L17" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="M17" s="63"/>
-      <c r="N17" s="63"/>
-      <c r="O17" s="63"/>
-      <c r="P17" s="63"/>
-      <c r="Q17" s="63"/>
-      <c r="R17" s="63"/>
-      <c r="S17" s="63"/>
-      <c r="T17" s="63"/>
-      <c r="U17" s="64"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="60"/>
+      <c r="P17" s="60"/>
+      <c r="Q17" s="60"/>
+      <c r="R17" s="60"/>
+      <c r="S17" s="60"/>
+      <c r="T17" s="60"/>
+      <c r="U17" s="61"/>
     </row>
     <row r="18" spans="1:21" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
@@ -4155,31 +4143,31 @@
       <c r="U24" s="1"/>
     </row>
     <row r="25" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="62" t="s">
+      <c r="A25" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="63"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="63"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="64"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="61"/>
       <c r="K25" s="2"/>
-      <c r="L25" s="62" t="s">
+      <c r="L25" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="M25" s="63"/>
-      <c r="N25" s="63"/>
-      <c r="O25" s="63"/>
-      <c r="P25" s="63"/>
-      <c r="Q25" s="63"/>
-      <c r="R25" s="63"/>
-      <c r="S25" s="63"/>
-      <c r="T25" s="63"/>
-      <c r="U25" s="64"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="60"/>
+      <c r="P25" s="60"/>
+      <c r="Q25" s="60"/>
+      <c r="R25" s="60"/>
+      <c r="S25" s="60"/>
+      <c r="T25" s="60"/>
+      <c r="U25" s="61"/>
     </row>
     <row r="26" spans="1:21" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
@@ -4383,29 +4371,29 @@
       <c r="U32" s="1"/>
     </row>
     <row r="33" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A33" s="62"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="63"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="64"/>
+      <c r="A33" s="59"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="61"/>
       <c r="K33" s="2"/>
-      <c r="L33" s="62" t="s">
+      <c r="L33" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="M33" s="63"/>
-      <c r="N33" s="63"/>
-      <c r="O33" s="63"/>
-      <c r="P33" s="63"/>
-      <c r="Q33" s="63"/>
-      <c r="R33" s="63"/>
-      <c r="S33" s="63"/>
-      <c r="T33" s="63"/>
-      <c r="U33" s="64"/>
+      <c r="M33" s="60"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="60"/>
+      <c r="R33" s="60"/>
+      <c r="S33" s="60"/>
+      <c r="T33" s="60"/>
+      <c r="U33" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4429,10 +4417,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A2:M59"/>
+  <dimension ref="A2:L59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4448,13 +4436,12 @@
     <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
@@ -4491,11 +4478,8 @@
       <c r="L2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <v>1</v>
       </c>
@@ -4535,9 +4519,8 @@
       <c r="L3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="27"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <v>2</v>
       </c>
@@ -4577,9 +4560,8 @@
       <c r="L4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="27"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>3</v>
       </c>
@@ -4619,9 +4601,8 @@
       <c r="L5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="30"/>
-    </row>
-    <row r="6" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>4</v>
       </c>
@@ -4647,8 +4628,8 @@
         <v>-129</v>
       </c>
       <c r="I6" s="30" t="str">
-        <f>RIGHT(DEC2BIN(H6,10),10)</f>
-        <v>1101111111</v>
+        <f>RIGHT(DEC2BIN(H6,10),9)</f>
+        <v>101111111</v>
       </c>
       <c r="J6" s="30" t="str">
         <f t="shared" si="0"/>
@@ -4656,14 +4637,13 @@
       </c>
       <c r="K6" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L6" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="30"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
         <v>5</v>
       </c>
@@ -4689,7 +4669,7 @@
         <v>-1</v>
       </c>
       <c r="I7" s="33" t="str">
-        <f t="shared" ref="I4:I26" si="2">RIGHT(DEC2BIN(H7,10),9)</f>
+        <f t="shared" ref="I7:I26" si="2">RIGHT(DEC2BIN(H7,10),9)</f>
         <v>111111111</v>
       </c>
       <c r="J7" s="33" t="str">
@@ -4703,9 +4683,8 @@
       <c r="L7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="33"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
         <v>6</v>
       </c>
@@ -4745,9 +4724,8 @@
       <c r="L8" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="M8" s="33"/>
-    </row>
-    <row r="9" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36">
         <v>7</v>
       </c>
@@ -4787,49 +4765,47 @@
       <c r="L9" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="M9" s="36"/>
-    </row>
-    <row r="10" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52">
+    </row>
+    <row r="10" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="36">
         <v>8</v>
       </c>
-      <c r="B10" s="52">
+      <c r="B10" s="36">
         <v>4</v>
       </c>
-      <c r="C10" s="52">
+      <c r="C10" s="36">
         <v>-1</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="D10" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="52">
+      <c r="F10" s="36">
         <v>-128</v>
       </c>
-      <c r="G10" s="54" t="s">
+      <c r="G10" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="54">
+      <c r="H10" s="38">
         <v>127</v>
       </c>
-      <c r="I10" s="54" t="s">
+      <c r="I10" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="J10" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="L10" s="52" t="s">
+      <c r="L10" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="52"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="39">
         <v>9</v>
       </c>
@@ -4869,50 +4845,48 @@
       <c r="L11" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="M11" s="39"/>
-    </row>
-    <row r="12" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="52">
+    </row>
+    <row r="12" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="39">
         <v>10</v>
       </c>
-      <c r="B12" s="52">
+      <c r="B12" s="39">
         <v>5</v>
       </c>
-      <c r="C12" s="52">
-        <v>1</v>
-      </c>
-      <c r="D12" s="52" t="s">
+      <c r="C12" s="39">
+        <v>1</v>
+      </c>
+      <c r="D12" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="53" t="s">
+      <c r="E12" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="52">
+      <c r="F12" s="39">
         <v>-128</v>
       </c>
-      <c r="G12" s="54" t="s">
+      <c r="G12" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="54">
+      <c r="H12" s="40">
         <v>129</v>
       </c>
-      <c r="I12" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="52" t="str">
+      <c r="I12" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="39" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K12" s="52" t="str">
+      <c r="K12" s="39" t="str">
         <f>MID(I12,1,2)</f>
         <v>01</v>
       </c>
-      <c r="L12" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="M12" s="52"/>
-    </row>
-    <row r="13" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L12" s="39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>11</v>
       </c>
@@ -4952,9 +4926,8 @@
       <c r="L13" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="M13" s="42"/>
-    </row>
-    <row r="14" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>12</v>
       </c>
@@ -4994,9 +4967,8 @@
       <c r="L14" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="M14" s="42"/>
-    </row>
-    <row r="15" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>13</v>
       </c>
@@ -5036,50 +5008,48 @@
       <c r="L15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M15" s="11"/>
-    </row>
-    <row r="16" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52">
+    </row>
+    <row r="16" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
         <v>14</v>
       </c>
-      <c r="B16" s="52">
+      <c r="B16" s="11">
         <v>7</v>
       </c>
-      <c r="C16" s="52">
+      <c r="C16" s="11">
         <v>127</v>
       </c>
-      <c r="D16" s="54" t="s">
+      <c r="D16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="53" t="s">
+      <c r="E16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="52">
+      <c r="F16" s="11">
         <v>-128</v>
       </c>
-      <c r="G16" s="54" t="s">
+      <c r="G16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="54">
+      <c r="H16" s="12">
         <v>255</v>
       </c>
-      <c r="I16" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="52" t="str">
+      <c r="I16" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="11" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K16" s="52" t="str">
+      <c r="K16" s="11" t="str">
         <f>MID(I16,1,2)</f>
         <v>01</v>
       </c>
-      <c r="L16" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="M16" s="52"/>
-    </row>
-    <row r="17" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>15</v>
       </c>
@@ -5119,9 +5089,8 @@
       <c r="L17" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="M17" s="14"/>
-    </row>
-    <row r="18" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>16</v>
       </c>
@@ -5161,9 +5130,8 @@
       <c r="L18" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="M18" s="14"/>
-    </row>
-    <row r="19" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>17</v>
       </c>
@@ -5203,9 +5171,8 @@
       <c r="L19" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="M19" s="17"/>
-    </row>
-    <row r="20" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>18</v>
       </c>
@@ -5245,9 +5212,8 @@
       <c r="L20" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="M20" s="17"/>
-    </row>
-    <row r="21" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="45">
         <v>19</v>
       </c>
@@ -5287,9 +5253,8 @@
       <c r="L21" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="M21" s="45"/>
-    </row>
-    <row r="22" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="45">
         <v>20</v>
       </c>
@@ -5329,9 +5294,8 @@
       <c r="L22" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="M22" s="45"/>
-    </row>
-    <row r="23" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="48">
         <v>21</v>
       </c>
@@ -5371,9 +5335,8 @@
       <c r="L23" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="M23" s="48"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="48">
         <v>22</v>
       </c>
@@ -5413,9 +5376,8 @@
       <c r="L24" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="M24" s="48"/>
-    </row>
-    <row r="25" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>23</v>
       </c>
@@ -5455,9 +5417,8 @@
       <c r="L25" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="M25" s="20"/>
-    </row>
-    <row r="26" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>24</v>
       </c>
@@ -5497,302 +5458,301 @@
       <c r="L26" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="M26" s="20"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="66" t="str" cm="1">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="63" t="str" cm="1">
         <f t="array" aca="1" ref="A28" ca="1">"void TesteSoma"&amp;INDIRECT("A"&amp;K28+2)&amp;"(CuTest *tc){"</f>
         <v>void TesteSoma3(CuTest *tc){</v>
       </c>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
       <c r="K28" s="51">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="66" t="str" cm="1">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="63" t="str" cm="1">
         <f t="array" aca="1" ref="A29" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;3+(K28-1)*2)&amp;""";"</f>
         <v>char * input1 = "10000000";</v>
       </c>
-      <c r="B29" s="66"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
       <c r="E29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="66" t="str" cm="1">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="63" t="str" cm="1">
         <f t="array" aca="1" ref="A30" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;3+(K28-1)*2)&amp;""";"</f>
         <v>char * input2 = "01111111";</v>
       </c>
-      <c r="B30" s="66"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="66"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
       <c r="K30" s="23"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="66" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="66"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="63"/>
       <c r="K31" s="23"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="66" t="str" cm="1">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="63" t="str" cm="1">
         <f t="array" aca="1" ref="A32" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;3+(K28-1)*2)&amp;""";"</f>
         <v>char * expected = "111111111";</v>
       </c>
-      <c r="B32" s="66"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="66"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
       <c r="K32" s="23"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="66"/>
-      <c r="C33" s="66"/>
-      <c r="D33" s="66"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
       <c r="K33" s="23"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="66"/>
-      <c r="C34" s="66"/>
-      <c r="D34" s="66"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
       <c r="K34" s="23"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="67"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
+      <c r="A35" s="64"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
       <c r="K35" s="23"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="66" t="str" cm="1">
+      <c r="A36" s="63" t="str" cm="1">
         <f t="array" aca="1" ref="A36" ca="1">"void TesteSub"&amp;INDIRECT("A"&amp;K28+2)&amp;"(CuTest *tc){"</f>
         <v>void TesteSub3(CuTest *tc){</v>
       </c>
-      <c r="B36" s="66"/>
-      <c r="C36" s="66"/>
-      <c r="D36" s="66"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
       <c r="K36" s="23"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="66" t="str" cm="1">
+      <c r="A37" s="63" t="str" cm="1">
         <f t="array" aca="1" ref="A37" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;4+(K28-1)*2)&amp;""";"</f>
         <v>char * input1 = "10000000";</v>
       </c>
-      <c r="B37" s="66"/>
-      <c r="C37" s="66"/>
-      <c r="D37" s="66"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
       <c r="K37" s="23"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="66" t="str" cm="1">
+      <c r="A38" s="63" t="str" cm="1">
         <f t="array" aca="1" ref="A38" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;4+(K28-1)*2)&amp;""";"</f>
         <v>char * input2 = "01111111";</v>
       </c>
-      <c r="B38" s="66"/>
-      <c r="C38" s="66"/>
-      <c r="D38" s="66"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
       <c r="K38" s="23"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="66"/>
-      <c r="C39" s="66"/>
-      <c r="D39" s="66"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="63"/>
+      <c r="D39" s="63"/>
       <c r="K39" s="23"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="66" t="str" cm="1">
+      <c r="A40" s="63" t="str" cm="1">
         <f t="array" aca="1" ref="A40" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;4+(K28-1)*2)&amp;""";"</f>
         <v>char * expected = "100000001";</v>
       </c>
-      <c r="B40" s="66"/>
-      <c r="C40" s="66"/>
-      <c r="D40" s="66"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
       <c r="K40" s="23"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="66"/>
-      <c r="C41" s="66"/>
-      <c r="D41" s="66"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="63"/>
       <c r="K41" s="23"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="66"/>
-      <c r="C42" s="66"/>
-      <c r="D42" s="66"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
       <c r="K42" s="23"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="60"/>
-      <c r="B43" s="60"/>
-      <c r="C43" s="60"/>
-      <c r="D43" s="60"/>
+      <c r="A43" s="57"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
       <c r="K43" s="23"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="65" t="str" cm="1">
+      <c r="A44" s="62" t="str" cm="1">
         <f t="array" aca="1" ref="A44" ca="1">"void TesteSoma"&amp;INDIRECT("A"&amp;K28+3)&amp;"(CuTest *tc){"</f>
         <v>void TesteSoma4(CuTest *tc){</v>
       </c>
-      <c r="B44" s="65"/>
-      <c r="C44" s="65"/>
-      <c r="D44" s="65"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
       <c r="K44" s="23"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="65" t="str" cm="1">
+      <c r="A45" s="62" t="str" cm="1">
         <f t="array" aca="1" ref="A45" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;5+(K28-1)*2)&amp;""";"</f>
         <v>char * input1 = "11111111";</v>
       </c>
-      <c r="B45" s="65"/>
-      <c r="C45" s="65"/>
-      <c r="D45" s="65"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
       <c r="K45" s="23"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="65" t="str" cm="1">
+      <c r="A46" s="62" t="str" cm="1">
         <f t="array" aca="1" ref="A46" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;5+(K28-1)*2)&amp;""";"</f>
         <v>char * input2 = "10000000";</v>
       </c>
-      <c r="B46" s="65"/>
-      <c r="C46" s="65"/>
-      <c r="D46" s="65"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="62"/>
       <c r="K46" s="23"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="65" t="s">
+      <c r="A47" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="65"/>
-      <c r="C47" s="65"/>
-      <c r="D47" s="65"/>
+      <c r="B47" s="62"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="62"/>
       <c r="K47" s="23"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="65" t="str" cm="1">
+      <c r="A48" s="62" t="str" cm="1">
         <f t="array" aca="1" ref="A48" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;5+(K28-1)*2)&amp;""";"</f>
         <v>char * expected = "101111111";</v>
       </c>
-      <c r="B48" s="65"/>
-      <c r="C48" s="65"/>
-      <c r="D48" s="65"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="62"/>
       <c r="K48" s="23"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="65" t="s">
+      <c r="A49" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="B49" s="65"/>
-      <c r="C49" s="65"/>
-      <c r="D49" s="65"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="62"/>
       <c r="K49" s="23"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="65" t="s">
+      <c r="A50" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="65"/>
-      <c r="C50" s="65"/>
-      <c r="D50" s="65"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="62"/>
       <c r="K50" s="23"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="60"/>
-      <c r="B51" s="60"/>
-      <c r="C51" s="60"/>
-      <c r="D51" s="60"/>
+      <c r="A51" s="57"/>
+      <c r="B51" s="57"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
       <c r="K51" s="23"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="65" t="str" cm="1">
+      <c r="A52" s="62" t="str" cm="1">
         <f t="array" aca="1" ref="A52" ca="1">"void TesteSub"&amp;INDIRECT("A"&amp;K28+3)&amp;"(CuTest *tc){"</f>
         <v>void TesteSub4(CuTest *tc){</v>
       </c>
-      <c r="B52" s="65"/>
-      <c r="C52" s="65"/>
-      <c r="D52" s="65"/>
+      <c r="B52" s="62"/>
+      <c r="C52" s="62"/>
+      <c r="D52" s="62"/>
       <c r="K52" s="23"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="65" t="str" cm="1">
+      <c r="A53" s="62" t="str" cm="1">
         <f t="array" aca="1" ref="A53" ca="1">"char * input1 = """&amp;INDIRECT("D"&amp;6+(K28-1)*2)&amp;""";"</f>
         <v>char * input1 = "11111111";</v>
       </c>
-      <c r="B53" s="65"/>
-      <c r="C53" s="65"/>
-      <c r="D53" s="65"/>
+      <c r="B53" s="62"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="62"/>
       <c r="K53" s="23"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="65" t="str" cm="1">
+      <c r="A54" s="62" t="str" cm="1">
         <f t="array" aca="1" ref="A54" ca="1">"char * input2 = """&amp;INDIRECT("G"&amp;6+(K28-1)*2)&amp;""";"</f>
         <v>char * input2 = "10000000";</v>
       </c>
-      <c r="B54" s="65"/>
-      <c r="C54" s="65"/>
-      <c r="D54" s="65"/>
+      <c r="B54" s="62"/>
+      <c r="C54" s="62"/>
+      <c r="D54" s="62"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="65" t="s">
+      <c r="A55" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="65"/>
-      <c r="C55" s="65"/>
-      <c r="D55" s="65"/>
+      <c r="B55" s="62"/>
+      <c r="C55" s="62"/>
+      <c r="D55" s="62"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="65" t="str" cm="1">
+      <c r="A56" s="62" t="str" cm="1">
         <f t="array" aca="1" ref="A56" ca="1">"char * expected = """&amp;INDIRECT("i"&amp;6+(K28-1)*2)&amp;""";"</f>
         <v>char * expected = "001111111";</v>
       </c>
-      <c r="B56" s="65"/>
-      <c r="C56" s="65"/>
-      <c r="D56" s="65"/>
+      <c r="B56" s="62"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="62"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="65" t="s">
+      <c r="A57" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="B57" s="65"/>
-      <c r="C57" s="65"/>
-      <c r="D57" s="65"/>
+      <c r="B57" s="62"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="62"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="65" t="s">
+      <c r="A58" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="B58" s="65"/>
-      <c r="C58" s="65"/>
-      <c r="D58" s="65"/>
+      <c r="B58" s="62"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="62"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="60"/>
-      <c r="B59" s="60"/>
-      <c r="C59" s="60"/>
-      <c r="D59" s="60"/>
+      <c r="A59" s="57"/>
+      <c r="B59" s="57"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="57"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:L26" xr:uid="{CED239D7-98B0-43DB-AD6A-A78832542F2A}">
@@ -5806,22 +5766,6 @@
     <sortCondition ref="E3:E26"/>
   </sortState>
   <mergeCells count="32">
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A53:D53"/>
     <mergeCell ref="A48:D48"/>
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A29:D29"/>
@@ -5838,6 +5782,22 @@
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A47:D47"/>
     <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A35:D35"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Conversor Binario para Ternario para Binario
Commiti inicial do conversor binário - ternário - binário
</commit_message>
<xml_diff>
--- a/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
+++ b/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/tabela_erros_calculadora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3162c0a97888194f/Documentos/GitHub/algoritmos/calculadora_oito_bits/calculadora_oito_bits/Arquivos_adicionais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1038" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62E7B428-60A6-4A31-AD8E-12CBC8C2A479}"/>
+  <xr:revisionPtr revIDLastSave="1039" documentId="8_{EA0D546C-BB91-448C-898A-C4FFF4CCA0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D881D4C0-5F75-4BB2-B1D6-0125A7E4E898}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
+    <workbookView xWindow="7320" yWindow="615" windowWidth="21600" windowHeight="11385" xr2:uid="{B453242F-16CD-49D7-9737-6112DA311A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela_erros_soma_subtração" sheetId="4" r:id="rId1"/>
@@ -614,6 +614,12 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -625,12 +631,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -979,8 +979,8 @@
   </sheetPr>
   <dimension ref="B2:R60"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,12 +1039,12 @@
       <c r="M2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="56" t="s">
+      <c r="O2" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
     </row>
     <row r="3" spans="2:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="27">
@@ -1086,12 +1086,12 @@
       <c r="M3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="56" t="s">
+      <c r="O3" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="56"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
     </row>
     <row r="4" spans="2:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="27">
@@ -1133,12 +1133,12 @@
       <c r="M4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="56" t="s">
+      <c r="O4" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="56"/>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="58"/>
+      <c r="R4" s="58"/>
     </row>
     <row r="5" spans="2:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="30">
@@ -1180,12 +1180,12 @@
       <c r="M5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="56" t="s">
+      <c r="O5" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="P5" s="56"/>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="56"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
     </row>
     <row r="6" spans="2:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="30">
@@ -1268,12 +1268,12 @@
       <c r="M7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="59" t="s">
+      <c r="O7" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="59"/>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="61"/>
+      <c r="R7" s="61"/>
     </row>
     <row r="8" spans="2:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="33">
@@ -1315,10 +1315,10 @@
       <c r="M8" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="O8" s="59"/>
-      <c r="P8" s="59"/>
-      <c r="Q8" s="59"/>
-      <c r="R8" s="59"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="61"/>
     </row>
     <row r="9" spans="2:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="36">
@@ -1360,10 +1360,10 @@
       <c r="M9" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="59"/>
-      <c r="P9" s="59"/>
-      <c r="Q9" s="59"/>
-      <c r="R9" s="59"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="61"/>
     </row>
     <row r="10" spans="2:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="36">
@@ -1403,10 +1403,10 @@
       <c r="M10" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="59"/>
-      <c r="P10" s="59"/>
-      <c r="Q10" s="59"/>
-      <c r="R10" s="59"/>
+      <c r="O10" s="61"/>
+      <c r="P10" s="61"/>
+      <c r="Q10" s="61"/>
+      <c r="R10" s="61"/>
     </row>
     <row r="11" spans="2:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="39">
@@ -1488,12 +1488,12 @@
       <c r="M12" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="O12" s="59" t="s">
+      <c r="O12" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="59"/>
-      <c r="R12" s="59"/>
+      <c r="P12" s="61"/>
+      <c r="Q12" s="61"/>
+      <c r="R12" s="61"/>
     </row>
     <row r="13" spans="2:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="42">
@@ -1535,10 +1535,10 @@
       <c r="M13" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="59"/>
-      <c r="R13" s="59"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="61"/>
+      <c r="Q13" s="61"/>
+      <c r="R13" s="61"/>
     </row>
     <row r="14" spans="2:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="42">
@@ -1580,10 +1580,10 @@
       <c r="M14" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="O14" s="59"/>
-      <c r="P14" s="59"/>
-      <c r="Q14" s="59"/>
-      <c r="R14" s="59"/>
+      <c r="O14" s="61"/>
+      <c r="P14" s="61"/>
+      <c r="Q14" s="61"/>
+      <c r="R14" s="61"/>
     </row>
     <row r="15" spans="2:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
@@ -1625,10 +1625,10 @@
       <c r="M15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="59"/>
+      <c r="O15" s="61"/>
+      <c r="P15" s="61"/>
+      <c r="Q15" s="61"/>
+      <c r="R15" s="61"/>
     </row>
     <row r="16" spans="2:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
@@ -2081,305 +2081,305 @@
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="58"/>
-      <c r="D28" s="58"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
       <c r="E28" s="55">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="61" t="str" cm="1">
+      <c r="B29" s="56" t="str" cm="1">
         <f t="array" aca="1" ref="B29" ca="1">"void TesteSoma"&amp;INDIRECT("b"&amp;E28+2)&amp;"(CuTest *tc){"</f>
-        <v>void TesteSoma3(CuTest *tc){</v>
-      </c>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
+        <v>void TesteSoma5(CuTest *tc){</v>
+      </c>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="61" t="str" cm="1">
+      <c r="B30" s="56" t="str" cm="1">
         <f t="array" aca="1" ref="B30" ca="1">"char * input1 = """&amp;INDIRECT("e"&amp;3+(E28-1)*2)&amp;""";"</f>
-        <v>char * input1 = "10000000";</v>
-      </c>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="61"/>
+        <v>char * input1 = "00000001";</v>
+      </c>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
       <c r="L30" s="23"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="61" t="str" cm="1">
+      <c r="B31" s="56" t="str" cm="1">
         <f t="array" aca="1" ref="B31" ca="1">"char * input2 = """&amp;INDIRECT("h"&amp;3+(E28-1)*2)&amp;""";"</f>
+        <v>char * input2 = "10000000";</v>
+      </c>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="L31" s="23"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="L32" s="23"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="56" t="str" cm="1">
+        <f t="array" aca="1" ref="B33" ca="1">"char * expected = """&amp;INDIRECT("j"&amp;3+(E28-1)*2)&amp;""";"</f>
+        <v>char * expected = "110000001";</v>
+      </c>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="L33" s="23"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="L34" s="23"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="L35" s="23"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="L36" s="23"/>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="56" t="str" cm="1">
+        <f t="array" aca="1" ref="B37" ca="1">"void TesteSub"&amp;INDIRECT("b"&amp;E28+2)&amp;"(CuTest *tc){"</f>
+        <v>void TesteSub5(CuTest *tc){</v>
+      </c>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="L37" s="23"/>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="56" t="str" cm="1">
+        <f t="array" aca="1" ref="B38" ca="1">"char * input1 = """&amp;INDIRECT("e"&amp;4+(E28-1)*2)&amp;""";"</f>
+        <v>char * input1 = "00000001";</v>
+      </c>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="L38" s="23"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="56" t="str" cm="1">
+        <f t="array" aca="1" ref="B39" ca="1">"char * input2 = """&amp;INDIRECT("h"&amp;4+(E28-1)*2)&amp;""";"</f>
+        <v>char * input2 = "10000000";</v>
+      </c>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="L39" s="23"/>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="56"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="56"/>
+      <c r="L40" s="23"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="56" t="str" cm="1">
+        <f t="array" aca="1" ref="B41" ca="1">"char * expected = """&amp;INDIRECT("j"&amp;4+(E28-1)*2)&amp;""";"</f>
+        <v>char * expected = "010000001";</v>
+      </c>
+      <c r="C41" s="56"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56"/>
+      <c r="L41" s="23"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="L42" s="23"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="56"/>
+      <c r="D43" s="56"/>
+      <c r="E43" s="56"/>
+      <c r="L43" s="23"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="57"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="L44" s="23"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="56" t="str" cm="1">
+        <f t="array" aca="1" ref="B45" ca="1">"void TesteSoma"&amp;INDIRECT("b"&amp;E28+3)&amp;"(CuTest *tc){"</f>
+        <v>void TesteSoma6(CuTest *tc){</v>
+      </c>
+      <c r="C45" s="56"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="56"/>
+      <c r="L45" s="23"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="56" t="str" cm="1">
+        <f t="array" aca="1" ref="B46" ca="1">"char * input1 = """&amp;INDIRECT("e"&amp;5+(E28-1)*2)&amp;""";"</f>
+        <v>char * input1 = "00000001";</v>
+      </c>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="L46" s="23"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="56" t="str" cm="1">
+        <f t="array" aca="1" ref="B47" ca="1">"char * input2 = """&amp;INDIRECT("h"&amp;5+(E28-1)*2)&amp;""";"</f>
         <v>char * input2 = "01111111";</v>
       </c>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="L31" s="23"/>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="61" t="s">
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="L47" s="23"/>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="L32" s="23"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="61" t="str" cm="1">
-        <f t="array" aca="1" ref="B33" ca="1">"char * expected = """&amp;INDIRECT("j"&amp;3+(E28-1)*2)&amp;""";"</f>
-        <v>char * expected = "111111111";</v>
-      </c>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="L33" s="23"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="61" t="s">
+      <c r="C48" s="56"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+      <c r="L48" s="23"/>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" s="56" t="str" cm="1">
+        <f t="array" aca="1" ref="B49" ca="1">"char * expected = """&amp;INDIRECT("j"&amp;5+(E28-1)*2)&amp;""";"</f>
+        <v>char * expected = "010000000";</v>
+      </c>
+      <c r="C49" s="56"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56"/>
+      <c r="L49" s="23"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
-      <c r="L34" s="23"/>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="61" t="s">
+      <c r="C50" s="56"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56"/>
+      <c r="L50" s="23"/>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="L35" s="23"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="60"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
-      <c r="L36" s="23"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="61" t="str" cm="1">
-        <f t="array" aca="1" ref="B37" ca="1">"void TesteSub"&amp;INDIRECT("b"&amp;E28+2)&amp;"(CuTest *tc){"</f>
-        <v>void TesteSub3(CuTest *tc){</v>
-      </c>
-      <c r="C37" s="61"/>
-      <c r="D37" s="61"/>
-      <c r="E37" s="61"/>
-      <c r="L37" s="23"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="61" t="str" cm="1">
-        <f t="array" aca="1" ref="B38" ca="1">"char * input1 = """&amp;INDIRECT("e"&amp;4+(E28-1)*2)&amp;""";"</f>
-        <v>char * input1 = "10000000";</v>
-      </c>
-      <c r="C38" s="61"/>
-      <c r="D38" s="61"/>
-      <c r="E38" s="61"/>
-      <c r="L38" s="23"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B39" s="61" t="str" cm="1">
-        <f t="array" aca="1" ref="B39" ca="1">"char * input2 = """&amp;INDIRECT("h"&amp;4+(E28-1)*2)&amp;""";"</f>
+      <c r="C51" s="56"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="L51" s="23"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="57"/>
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="L52" s="23"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="56" t="str" cm="1">
+        <f t="array" aca="1" ref="B53" ca="1">"void TesteSub"&amp;INDIRECT("b"&amp;E28+3)&amp;"(CuTest *tc){"</f>
+        <v>void TesteSub6(CuTest *tc){</v>
+      </c>
+      <c r="C53" s="56"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="56"/>
+      <c r="L53" s="23"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B54" s="56" t="str" cm="1">
+        <f t="array" aca="1" ref="B54" ca="1">"char * input1 = """&amp;INDIRECT("e"&amp;6+(E28-1)*2)&amp;""";"</f>
+        <v>char * input1 = "00000001";</v>
+      </c>
+      <c r="C54" s="56"/>
+      <c r="D54" s="56"/>
+      <c r="E54" s="56"/>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B55" s="56" t="str" cm="1">
+        <f t="array" aca="1" ref="B55" ca="1">"char * input2 = """&amp;INDIRECT("h"&amp;6+(E28-1)*2)&amp;""";"</f>
         <v>char * input2 = "01111111";</v>
       </c>
-      <c r="C39" s="61"/>
-      <c r="D39" s="61"/>
-      <c r="E39" s="61"/>
-      <c r="L39" s="23"/>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="61" t="s">
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="61"/>
-      <c r="D40" s="61"/>
-      <c r="E40" s="61"/>
-      <c r="L40" s="23"/>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="61" t="str" cm="1">
-        <f t="array" aca="1" ref="B41" ca="1">"char * expected = """&amp;INDIRECT("j"&amp;4+(E28-1)*2)&amp;""";"</f>
-        <v>char * expected = "100000001";</v>
-      </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="L41" s="23"/>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="61" t="s">
+      <c r="C56" s="56"/>
+      <c r="D56" s="56"/>
+      <c r="E56" s="56"/>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B57" s="56" t="str" cm="1">
+        <f t="array" aca="1" ref="B57" ca="1">"char * expected = """&amp;INDIRECT("j"&amp;6+(E28-1)*2)&amp;""";"</f>
+        <v>char * expected = "110000010";</v>
+      </c>
+      <c r="C57" s="56"/>
+      <c r="D57" s="56"/>
+      <c r="E57" s="56"/>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B58" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="61"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="61"/>
-      <c r="L42" s="23"/>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="61" t="s">
+      <c r="C58" s="56"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="56"/>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B59" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="61"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="61"/>
-      <c r="L43" s="23"/>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="60"/>
-      <c r="C44" s="60"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="60"/>
-      <c r="L44" s="23"/>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="61" t="str" cm="1">
-        <f t="array" aca="1" ref="B45" ca="1">"void TesteSoma"&amp;INDIRECT("b"&amp;E28+3)&amp;"(CuTest *tc){"</f>
-        <v>void TesteSoma4(CuTest *tc){</v>
-      </c>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="61"/>
-      <c r="L45" s="23"/>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="61" t="str" cm="1">
-        <f t="array" aca="1" ref="B46" ca="1">"char * input1 = """&amp;INDIRECT("e"&amp;5+(E28-1)*2)&amp;""";"</f>
-        <v>char * input1 = "11111111";</v>
-      </c>
-      <c r="C46" s="61"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="61"/>
-      <c r="L46" s="23"/>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="61" t="str" cm="1">
-        <f t="array" aca="1" ref="B47" ca="1">"char * input2 = """&amp;INDIRECT("h"&amp;5+(E28-1)*2)&amp;""";"</f>
-        <v>char * input2 = "10000000";</v>
-      </c>
-      <c r="C47" s="61"/>
-      <c r="D47" s="61"/>
-      <c r="E47" s="61"/>
-      <c r="L47" s="23"/>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="61"/>
-      <c r="D48" s="61"/>
-      <c r="E48" s="61"/>
-      <c r="L48" s="23"/>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B49" s="61" t="str" cm="1">
-        <f t="array" aca="1" ref="B49" ca="1">"char * expected = """&amp;INDIRECT("j"&amp;5+(E28-1)*2)&amp;""";"</f>
-        <v>char * expected = "101111111";</v>
-      </c>
-      <c r="C49" s="61"/>
-      <c r="D49" s="61"/>
-      <c r="E49" s="61"/>
-      <c r="L49" s="23"/>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B50" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="C50" s="61"/>
-      <c r="D50" s="61"/>
-      <c r="E50" s="61"/>
-      <c r="L50" s="23"/>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B51" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="C51" s="61"/>
-      <c r="D51" s="61"/>
-      <c r="E51" s="61"/>
-      <c r="L51" s="23"/>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B52" s="60"/>
-      <c r="C52" s="60"/>
-      <c r="D52" s="60"/>
-      <c r="E52" s="60"/>
-      <c r="L52" s="23"/>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B53" s="61" t="str" cm="1">
-        <f t="array" aca="1" ref="B53" ca="1">"void TesteSub"&amp;INDIRECT("b"&amp;E28+3)&amp;"(CuTest *tc){"</f>
-        <v>void TesteSub4(CuTest *tc){</v>
-      </c>
-      <c r="C53" s="61"/>
-      <c r="D53" s="61"/>
-      <c r="E53" s="61"/>
-      <c r="L53" s="23"/>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B54" s="61" t="str" cm="1">
-        <f t="array" aca="1" ref="B54" ca="1">"char * input1 = """&amp;INDIRECT("e"&amp;6+(E28-1)*2)&amp;""";"</f>
-        <v>char * input1 = "11111111";</v>
-      </c>
-      <c r="C54" s="61"/>
-      <c r="D54" s="61"/>
-      <c r="E54" s="61"/>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B55" s="61" t="str" cm="1">
-        <f t="array" aca="1" ref="B55" ca="1">"char * input2 = """&amp;INDIRECT("h"&amp;6+(E28-1)*2)&amp;""";"</f>
-        <v>char * input2 = "10000000";</v>
-      </c>
-      <c r="C55" s="61"/>
-      <c r="D55" s="61"/>
-      <c r="E55" s="61"/>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B56" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="C56" s="61"/>
-      <c r="D56" s="61"/>
-      <c r="E56" s="61"/>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B57" s="61" t="str" cm="1">
-        <f t="array" aca="1" ref="B57" ca="1">"char * expected = """&amp;INDIRECT("j"&amp;6+(E28-1)*2)&amp;""";"</f>
-        <v>char * expected = "001111111";</v>
-      </c>
-      <c r="C57" s="61"/>
-      <c r="D57" s="61"/>
-      <c r="E57" s="61"/>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="61"/>
-      <c r="D58" s="61"/>
-      <c r="E58" s="61"/>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B59" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="C59" s="61"/>
-      <c r="D59" s="61"/>
-      <c r="E59" s="61"/>
+      <c r="C59" s="56"/>
+      <c r="D59" s="56"/>
+      <c r="E59" s="56"/>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B60" s="57"/>
-      <c r="C60" s="57"/>
-      <c r="D60" s="57"/>
-      <c r="E60" s="57"/>
+      <c r="B60" s="59"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="59"/>
     </row>
   </sheetData>
   <autoFilter ref="C2:M26" xr:uid="{CED239D7-98B0-43DB-AD6A-A78832542F2A}">
@@ -2393,6 +2393,29 @@
     <sortCondition ref="F3:F26"/>
   </sortState>
   <mergeCells count="39">
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="O7:R10"/>
+    <mergeCell ref="O12:R15"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B54:E54"/>
     <mergeCell ref="B49:E49"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:E30"/>
@@ -2409,29 +2432,6 @@
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="B48:E48"/>
     <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="O7:R10"/>
-    <mergeCell ref="O12:R15"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B57:E57"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro" error="Valores válidos entre 1 e 12" sqref="E28" xr:uid="{C26FF554-22CC-44C5-A70B-3F2BC79CFB6D}">
@@ -2451,7 +2451,7 @@
   </sheetPr>
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
@@ -2527,7 +2527,7 @@
         <v>30</v>
       </c>
       <c r="L2" s="6" t="str">
-        <f>DEC2BIN(K2,8)</f>
+        <f t="shared" ref="L2:L30" si="1">DEC2BIN(K2,8)</f>
         <v>00011110</v>
       </c>
       <c r="M2" s="8"/>
@@ -2535,7 +2535,7 @@
         <v>83</v>
       </c>
       <c r="O2" s="6" t="str">
-        <f t="shared" ref="O2:O46" si="1">DEC2BIN(N2,8)</f>
+        <f t="shared" ref="O2:O46" si="2">DEC2BIN(N2,8)</f>
         <v>01010011</v>
       </c>
       <c r="P2" s="8"/>
@@ -2570,7 +2570,7 @@
         <v>31</v>
       </c>
       <c r="L3" s="6" t="str">
-        <f>DEC2BIN(K3,8)</f>
+        <f t="shared" si="1"/>
         <v>00011111</v>
       </c>
       <c r="M3" s="8"/>
@@ -2578,7 +2578,7 @@
         <v>84</v>
       </c>
       <c r="O3" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01010100</v>
       </c>
       <c r="P3" s="8"/>
@@ -2595,7 +2595,7 @@
         <v>-127</v>
       </c>
       <c r="C4" s="54" t="str">
-        <f t="shared" ref="C4" si="2">RIGHT(DEC2BIN(B4,8),8)</f>
+        <f t="shared" ref="C4" si="3">RIGHT(DEC2BIN(B4,8),8)</f>
         <v>10000001</v>
       </c>
       <c r="D4" s="8"/>
@@ -2619,7 +2619,7 @@
         <v>32</v>
       </c>
       <c r="L4" s="6" t="str">
-        <f>DEC2BIN(K4,8)</f>
+        <f t="shared" si="1"/>
         <v>00100000</v>
       </c>
       <c r="M4" s="8"/>
@@ -2627,7 +2627,7 @@
         <v>85</v>
       </c>
       <c r="O4" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01010101</v>
       </c>
       <c r="P4" s="8"/>
@@ -2644,7 +2644,7 @@
         <v>-126</v>
       </c>
       <c r="C5" s="54" t="str">
-        <f t="shared" ref="C5:C26" si="3">RIGHT(DEC2BIN(B5,8),8)</f>
+        <f t="shared" ref="C5:C26" si="4">RIGHT(DEC2BIN(B5,8),8)</f>
         <v>10000010</v>
       </c>
       <c r="D5" s="8"/>
@@ -2668,7 +2668,7 @@
         <v>33</v>
       </c>
       <c r="L5" s="6" t="str">
-        <f>DEC2BIN(K5,8)</f>
+        <f t="shared" si="1"/>
         <v>00100001</v>
       </c>
       <c r="M5" s="8"/>
@@ -2676,7 +2676,7 @@
         <v>86</v>
       </c>
       <c r="O5" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01010110</v>
       </c>
       <c r="P5" s="8"/>
@@ -2693,7 +2693,7 @@
         <v>-125</v>
       </c>
       <c r="C6" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10000011</v>
       </c>
       <c r="D6" s="8"/>
@@ -2717,7 +2717,7 @@
         <v>34</v>
       </c>
       <c r="L6" s="6" t="str">
-        <f>DEC2BIN(K6,8)</f>
+        <f t="shared" si="1"/>
         <v>00100010</v>
       </c>
       <c r="M6" s="8"/>
@@ -2725,7 +2725,7 @@
         <v>87</v>
       </c>
       <c r="O6" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01010111</v>
       </c>
       <c r="P6" s="8"/>
@@ -2742,7 +2742,7 @@
         <v>-124</v>
       </c>
       <c r="C7" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10000100</v>
       </c>
       <c r="D7" s="8"/>
@@ -2758,7 +2758,7 @@
         <v>-18</v>
       </c>
       <c r="I7" s="6" t="str">
-        <f t="shared" ref="I7:I24" si="4">RIGHT(DEC2BIN(H7,8),8)</f>
+        <f t="shared" ref="I7:I24" si="5">RIGHT(DEC2BIN(H7,8),8)</f>
         <v>11101110</v>
       </c>
       <c r="J7" s="8"/>
@@ -2766,7 +2766,7 @@
         <v>35</v>
       </c>
       <c r="L7" s="6" t="str">
-        <f>DEC2BIN(K7,8)</f>
+        <f t="shared" si="1"/>
         <v>00100011</v>
       </c>
       <c r="M7" s="8"/>
@@ -2774,7 +2774,7 @@
         <v>88</v>
       </c>
       <c r="O7" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01011000</v>
       </c>
       <c r="P7" s="8"/>
@@ -2785,7 +2785,7 @@
         <v>-123</v>
       </c>
       <c r="C8" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10000101</v>
       </c>
       <c r="D8" s="8"/>
@@ -2801,7 +2801,7 @@
         <v>-17</v>
       </c>
       <c r="I8" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11101111</v>
       </c>
       <c r="J8" s="8"/>
@@ -2809,7 +2809,7 @@
         <v>36</v>
       </c>
       <c r="L8" s="6" t="str">
-        <f>DEC2BIN(K8,8)</f>
+        <f t="shared" si="1"/>
         <v>00100100</v>
       </c>
       <c r="M8" s="8"/>
@@ -2817,7 +2817,7 @@
         <v>89</v>
       </c>
       <c r="O8" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01011001</v>
       </c>
       <c r="P8" s="8"/>
@@ -2828,7 +2828,7 @@
         <v>-122</v>
       </c>
       <c r="C9" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10000110</v>
       </c>
       <c r="D9" s="8"/>
@@ -2844,7 +2844,7 @@
         <v>-16</v>
       </c>
       <c r="I9" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11110000</v>
       </c>
       <c r="J9" s="8"/>
@@ -2852,7 +2852,7 @@
         <v>37</v>
       </c>
       <c r="L9" s="6" t="str">
-        <f>DEC2BIN(K9,8)</f>
+        <f t="shared" si="1"/>
         <v>00100101</v>
       </c>
       <c r="M9" s="8"/>
@@ -2860,7 +2860,7 @@
         <v>90</v>
       </c>
       <c r="O9" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01011010</v>
       </c>
       <c r="P9" s="8"/>
@@ -2871,7 +2871,7 @@
         <v>-121</v>
       </c>
       <c r="C10" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10000111</v>
       </c>
       <c r="D10" s="8"/>
@@ -2887,7 +2887,7 @@
         <v>-15</v>
       </c>
       <c r="I10" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11110001</v>
       </c>
       <c r="J10" s="8"/>
@@ -2895,7 +2895,7 @@
         <v>38</v>
       </c>
       <c r="L10" s="6" t="str">
-        <f>DEC2BIN(K10,8)</f>
+        <f t="shared" si="1"/>
         <v>00100110</v>
       </c>
       <c r="M10" s="8"/>
@@ -2903,7 +2903,7 @@
         <v>91</v>
       </c>
       <c r="O10" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01011011</v>
       </c>
       <c r="P10" s="8"/>
@@ -2915,7 +2915,7 @@
         <v>-120</v>
       </c>
       <c r="C11" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10001000</v>
       </c>
       <c r="D11" s="8"/>
@@ -2931,7 +2931,7 @@
         <v>-14</v>
       </c>
       <c r="I11" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11110010</v>
       </c>
       <c r="J11" s="8"/>
@@ -2939,7 +2939,7 @@
         <v>39</v>
       </c>
       <c r="L11" s="6" t="str">
-        <f>DEC2BIN(K11,8)</f>
+        <f t="shared" si="1"/>
         <v>00100111</v>
       </c>
       <c r="M11" s="8"/>
@@ -2947,7 +2947,7 @@
         <v>92</v>
       </c>
       <c r="O11" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01011100</v>
       </c>
       <c r="P11" s="8"/>
@@ -2958,7 +2958,7 @@
         <v>-119</v>
       </c>
       <c r="C12" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10001001</v>
       </c>
       <c r="D12" s="8"/>
@@ -2974,7 +2974,7 @@
         <v>-13</v>
       </c>
       <c r="I12" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11110011</v>
       </c>
       <c r="J12" s="8"/>
@@ -2982,7 +2982,7 @@
         <v>40</v>
       </c>
       <c r="L12" s="6" t="str">
-        <f>DEC2BIN(K12,8)</f>
+        <f t="shared" si="1"/>
         <v>00101000</v>
       </c>
       <c r="M12" s="8"/>
@@ -2990,7 +2990,7 @@
         <v>93</v>
       </c>
       <c r="O12" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01011101</v>
       </c>
       <c r="P12" s="8"/>
@@ -3001,7 +3001,7 @@
         <v>-118</v>
       </c>
       <c r="C13" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10001010</v>
       </c>
       <c r="D13" s="8"/>
@@ -3017,7 +3017,7 @@
         <v>-12</v>
       </c>
       <c r="I13" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11110100</v>
       </c>
       <c r="J13" s="8"/>
@@ -3025,7 +3025,7 @@
         <v>41</v>
       </c>
       <c r="L13" s="6" t="str">
-        <f>DEC2BIN(K13,8)</f>
+        <f t="shared" si="1"/>
         <v>00101001</v>
       </c>
       <c r="M13" s="8"/>
@@ -3033,7 +3033,7 @@
         <v>94</v>
       </c>
       <c r="O13" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01011110</v>
       </c>
       <c r="P13" s="8"/>
@@ -3044,7 +3044,7 @@
         <v>-117</v>
       </c>
       <c r="C14" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10001011</v>
       </c>
       <c r="D14" s="8"/>
@@ -3060,7 +3060,7 @@
         <v>-11</v>
       </c>
       <c r="I14" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11110101</v>
       </c>
       <c r="J14" s="8"/>
@@ -3068,7 +3068,7 @@
         <v>42</v>
       </c>
       <c r="L14" s="6" t="str">
-        <f>DEC2BIN(K14,8)</f>
+        <f t="shared" si="1"/>
         <v>00101010</v>
       </c>
       <c r="M14" s="8"/>
@@ -3076,7 +3076,7 @@
         <v>95</v>
       </c>
       <c r="O14" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01011111</v>
       </c>
       <c r="P14" s="8"/>
@@ -3087,7 +3087,7 @@
         <v>-116</v>
       </c>
       <c r="C15" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10001100</v>
       </c>
       <c r="D15" s="8"/>
@@ -3103,7 +3103,7 @@
         <v>-10</v>
       </c>
       <c r="I15" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11110110</v>
       </c>
       <c r="J15" s="8"/>
@@ -3111,7 +3111,7 @@
         <v>43</v>
       </c>
       <c r="L15" s="6" t="str">
-        <f>DEC2BIN(K15,8)</f>
+        <f t="shared" si="1"/>
         <v>00101011</v>
       </c>
       <c r="M15" s="8"/>
@@ -3119,7 +3119,7 @@
         <v>96</v>
       </c>
       <c r="O15" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01100000</v>
       </c>
       <c r="P15" s="8"/>
@@ -3130,7 +3130,7 @@
         <v>-115</v>
       </c>
       <c r="C16" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10001101</v>
       </c>
       <c r="D16" s="8"/>
@@ -3146,7 +3146,7 @@
         <v>-9</v>
       </c>
       <c r="I16" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11110111</v>
       </c>
       <c r="J16" s="8"/>
@@ -3154,7 +3154,7 @@
         <v>44</v>
       </c>
       <c r="L16" s="6" t="str">
-        <f>DEC2BIN(K16,8)</f>
+        <f t="shared" si="1"/>
         <v>00101100</v>
       </c>
       <c r="M16" s="8"/>
@@ -3162,7 +3162,7 @@
         <v>97</v>
       </c>
       <c r="O16" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01100001</v>
       </c>
       <c r="P16" s="8"/>
@@ -3173,7 +3173,7 @@
         <v>-114</v>
       </c>
       <c r="C17" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10001110</v>
       </c>
       <c r="D17" s="8"/>
@@ -3189,7 +3189,7 @@
         <v>-8</v>
       </c>
       <c r="I17" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11111000</v>
       </c>
       <c r="J17" s="8"/>
@@ -3197,7 +3197,7 @@
         <v>45</v>
       </c>
       <c r="L17" s="6" t="str">
-        <f>DEC2BIN(K17,8)</f>
+        <f t="shared" si="1"/>
         <v>00101101</v>
       </c>
       <c r="M17" s="8"/>
@@ -3205,7 +3205,7 @@
         <v>98</v>
       </c>
       <c r="O17" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01100010</v>
       </c>
       <c r="P17" s="8"/>
@@ -3216,7 +3216,7 @@
         <v>-113</v>
       </c>
       <c r="C18" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10001111</v>
       </c>
       <c r="D18" s="8"/>
@@ -3232,7 +3232,7 @@
         <v>-7</v>
       </c>
       <c r="I18" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11111001</v>
       </c>
       <c r="J18" s="8"/>
@@ -3240,7 +3240,7 @@
         <v>46</v>
       </c>
       <c r="L18" s="6" t="str">
-        <f>DEC2BIN(K18,8)</f>
+        <f t="shared" si="1"/>
         <v>00101110</v>
       </c>
       <c r="M18" s="8"/>
@@ -3248,7 +3248,7 @@
         <v>99</v>
       </c>
       <c r="O18" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01100011</v>
       </c>
       <c r="P18" s="8"/>
@@ -3259,7 +3259,7 @@
         <v>-112</v>
       </c>
       <c r="C19" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10010000</v>
       </c>
       <c r="D19" s="8"/>
@@ -3275,7 +3275,7 @@
         <v>-6</v>
       </c>
       <c r="I19" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11111010</v>
       </c>
       <c r="J19" s="8"/>
@@ -3283,7 +3283,7 @@
         <v>47</v>
       </c>
       <c r="L19" s="6" t="str">
-        <f>DEC2BIN(K19,8)</f>
+        <f t="shared" si="1"/>
         <v>00101111</v>
       </c>
       <c r="M19" s="8"/>
@@ -3291,7 +3291,7 @@
         <v>100</v>
       </c>
       <c r="O19" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01100100</v>
       </c>
       <c r="P19" s="8"/>
@@ -3302,7 +3302,7 @@
         <v>-111</v>
       </c>
       <c r="C20" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10010001</v>
       </c>
       <c r="D20" s="8"/>
@@ -3318,7 +3318,7 @@
         <v>-5</v>
       </c>
       <c r="I20" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11111011</v>
       </c>
       <c r="J20" s="8"/>
@@ -3326,7 +3326,7 @@
         <v>48</v>
       </c>
       <c r="L20" s="6" t="str">
-        <f>DEC2BIN(K20,8)</f>
+        <f t="shared" si="1"/>
         <v>00110000</v>
       </c>
       <c r="M20" s="8"/>
@@ -3334,7 +3334,7 @@
         <v>101</v>
       </c>
       <c r="O20" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01100101</v>
       </c>
       <c r="P20" s="8"/>
@@ -3345,7 +3345,7 @@
         <v>-110</v>
       </c>
       <c r="C21" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10010010</v>
       </c>
       <c r="D21" s="8"/>
@@ -3361,7 +3361,7 @@
         <v>-4</v>
       </c>
       <c r="I21" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11111100</v>
       </c>
       <c r="J21" s="8"/>
@@ -3369,7 +3369,7 @@
         <v>49</v>
       </c>
       <c r="L21" s="6" t="str">
-        <f>DEC2BIN(K21,8)</f>
+        <f t="shared" si="1"/>
         <v>00110001</v>
       </c>
       <c r="M21" s="8"/>
@@ -3377,7 +3377,7 @@
         <v>102</v>
       </c>
       <c r="O21" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01100110</v>
       </c>
       <c r="P21" s="8"/>
@@ -3388,7 +3388,7 @@
         <v>-109</v>
       </c>
       <c r="C22" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10010011</v>
       </c>
       <c r="D22" s="8"/>
@@ -3404,7 +3404,7 @@
         <v>-3</v>
       </c>
       <c r="I22" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11111101</v>
       </c>
       <c r="J22" s="8"/>
@@ -3412,7 +3412,7 @@
         <v>50</v>
       </c>
       <c r="L22" s="6" t="str">
-        <f>DEC2BIN(K22,8)</f>
+        <f t="shared" si="1"/>
         <v>00110010</v>
       </c>
       <c r="M22" s="8"/>
@@ -3420,7 +3420,7 @@
         <v>103</v>
       </c>
       <c r="O22" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01100111</v>
       </c>
       <c r="P22" s="8"/>
@@ -3431,7 +3431,7 @@
         <v>-108</v>
       </c>
       <c r="C23" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10010100</v>
       </c>
       <c r="D23" s="8"/>
@@ -3447,7 +3447,7 @@
         <v>-2</v>
       </c>
       <c r="I23" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11111110</v>
       </c>
       <c r="J23" s="8"/>
@@ -3455,7 +3455,7 @@
         <v>51</v>
       </c>
       <c r="L23" s="6" t="str">
-        <f>DEC2BIN(K23,8)</f>
+        <f t="shared" si="1"/>
         <v>00110011</v>
       </c>
       <c r="M23" s="8"/>
@@ -3463,7 +3463,7 @@
         <v>104</v>
       </c>
       <c r="O23" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01101000</v>
       </c>
       <c r="P23" s="8"/>
@@ -3474,7 +3474,7 @@
         <v>-107</v>
       </c>
       <c r="C24" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10010101</v>
       </c>
       <c r="D24" s="8"/>
@@ -3490,7 +3490,7 @@
         <v>-1</v>
       </c>
       <c r="I24" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11111111</v>
       </c>
       <c r="J24" s="8"/>
@@ -3498,7 +3498,7 @@
         <v>52</v>
       </c>
       <c r="L24" s="6" t="str">
-        <f>DEC2BIN(K24,8)</f>
+        <f t="shared" si="1"/>
         <v>00110100</v>
       </c>
       <c r="M24" s="8"/>
@@ -3506,7 +3506,7 @@
         <v>105</v>
       </c>
       <c r="O24" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01101001</v>
       </c>
       <c r="P24" s="8"/>
@@ -3517,7 +3517,7 @@
         <v>-106</v>
       </c>
       <c r="C25" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10010110</v>
       </c>
       <c r="D25" s="8"/>
@@ -3533,7 +3533,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="6" t="str">
-        <f t="shared" ref="I25" si="5">DEC2BIN(H25,8)</f>
+        <f t="shared" ref="I25" si="6">DEC2BIN(H25,8)</f>
         <v>00000000</v>
       </c>
       <c r="J25" s="8"/>
@@ -3541,7 +3541,7 @@
         <v>53</v>
       </c>
       <c r="L25" s="6" t="str">
-        <f>DEC2BIN(K25,8)</f>
+        <f t="shared" si="1"/>
         <v>00110101</v>
       </c>
       <c r="M25" s="8"/>
@@ -3549,7 +3549,7 @@
         <v>106</v>
       </c>
       <c r="O25" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01101010</v>
       </c>
       <c r="P25" s="8"/>
@@ -3560,7 +3560,7 @@
         <v>-105</v>
       </c>
       <c r="C26" s="54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10010111</v>
       </c>
       <c r="D26" s="8"/>
@@ -3576,7 +3576,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="6" t="str">
-        <f t="shared" ref="I26:I51" si="6">DEC2BIN(H26,8)</f>
+        <f t="shared" ref="I26:I51" si="7">DEC2BIN(H26,8)</f>
         <v>00000001</v>
       </c>
       <c r="J26" s="8"/>
@@ -3584,7 +3584,7 @@
         <v>54</v>
       </c>
       <c r="L26" s="6" t="str">
-        <f>DEC2BIN(K26,8)</f>
+        <f t="shared" si="1"/>
         <v>00110110</v>
       </c>
       <c r="M26" s="8"/>
@@ -3592,7 +3592,7 @@
         <v>107</v>
       </c>
       <c r="O26" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01101011</v>
       </c>
       <c r="P26" s="8"/>
@@ -3603,7 +3603,7 @@
         <v>-104</v>
       </c>
       <c r="C27" s="54" t="str">
-        <f t="shared" ref="C27:C54" si="7">RIGHT(DEC2BIN(B27,8),8)</f>
+        <f t="shared" ref="C27:C54" si="8">RIGHT(DEC2BIN(B27,8),8)</f>
         <v>10011000</v>
       </c>
       <c r="D27" s="8"/>
@@ -3619,7 +3619,7 @@
         <v>2</v>
       </c>
       <c r="I27" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00000010</v>
       </c>
       <c r="J27" s="8"/>
@@ -3627,7 +3627,7 @@
         <v>55</v>
       </c>
       <c r="L27" s="6" t="str">
-        <f>DEC2BIN(K27,8)</f>
+        <f t="shared" si="1"/>
         <v>00110111</v>
       </c>
       <c r="M27" s="8"/>
@@ -3635,7 +3635,7 @@
         <v>108</v>
       </c>
       <c r="O27" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01101100</v>
       </c>
       <c r="P27" s="8"/>
@@ -3646,7 +3646,7 @@
         <v>-103</v>
       </c>
       <c r="C28" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10011001</v>
       </c>
       <c r="D28" s="8"/>
@@ -3662,7 +3662,7 @@
         <v>3</v>
       </c>
       <c r="I28" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00000011</v>
       </c>
       <c r="J28" s="8"/>
@@ -3670,7 +3670,7 @@
         <v>56</v>
       </c>
       <c r="L28" s="6" t="str">
-        <f>DEC2BIN(K28,8)</f>
+        <f t="shared" si="1"/>
         <v>00111000</v>
       </c>
       <c r="M28" s="8"/>
@@ -3678,7 +3678,7 @@
         <v>109</v>
       </c>
       <c r="O28" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01101101</v>
       </c>
       <c r="P28" s="8"/>
@@ -3689,7 +3689,7 @@
         <v>-102</v>
       </c>
       <c r="C29" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10011010</v>
       </c>
       <c r="D29" s="8"/>
@@ -3705,7 +3705,7 @@
         <v>4</v>
       </c>
       <c r="I29" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00000100</v>
       </c>
       <c r="J29" s="8"/>
@@ -3713,7 +3713,7 @@
         <v>57</v>
       </c>
       <c r="L29" s="6" t="str">
-        <f>DEC2BIN(K29,8)</f>
+        <f t="shared" si="1"/>
         <v>00111001</v>
       </c>
       <c r="M29" s="8"/>
@@ -3721,7 +3721,7 @@
         <v>110</v>
       </c>
       <c r="O29" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01101110</v>
       </c>
       <c r="P29" s="8"/>
@@ -3732,7 +3732,7 @@
         <v>-101</v>
       </c>
       <c r="C30" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10011011</v>
       </c>
       <c r="D30" s="8"/>
@@ -3748,7 +3748,7 @@
         <v>5</v>
       </c>
       <c r="I30" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00000101</v>
       </c>
       <c r="J30" s="8"/>
@@ -3756,7 +3756,7 @@
         <v>58</v>
       </c>
       <c r="L30" s="6" t="str">
-        <f>DEC2BIN(K30,8)</f>
+        <f t="shared" si="1"/>
         <v>00111010</v>
       </c>
       <c r="M30" s="8"/>
@@ -3764,7 +3764,7 @@
         <v>111</v>
       </c>
       <c r="O30" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01101111</v>
       </c>
       <c r="P30" s="8"/>
@@ -3775,7 +3775,7 @@
         <v>-100</v>
       </c>
       <c r="C31" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10011100</v>
       </c>
       <c r="D31" s="8"/>
@@ -3791,7 +3791,7 @@
         <v>6</v>
       </c>
       <c r="I31" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00000110</v>
       </c>
       <c r="J31" s="8"/>
@@ -3799,7 +3799,7 @@
         <v>59</v>
       </c>
       <c r="L31" s="6" t="str">
-        <f t="shared" ref="L31:L54" si="8">DEC2BIN(K31,8)</f>
+        <f t="shared" ref="L31:L54" si="9">DEC2BIN(K31,8)</f>
         <v>00111011</v>
       </c>
       <c r="M31" s="8"/>
@@ -3807,7 +3807,7 @@
         <v>112</v>
       </c>
       <c r="O31" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01110000</v>
       </c>
       <c r="P31" s="8"/>
@@ -3818,7 +3818,7 @@
         <v>-99</v>
       </c>
       <c r="C32" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10011101</v>
       </c>
       <c r="D32" s="8"/>
@@ -3834,7 +3834,7 @@
         <v>7</v>
       </c>
       <c r="I32" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00000111</v>
       </c>
       <c r="J32" s="8"/>
@@ -3842,7 +3842,7 @@
         <v>60</v>
       </c>
       <c r="L32" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>00111100</v>
       </c>
       <c r="M32" s="8"/>
@@ -3850,7 +3850,7 @@
         <v>113</v>
       </c>
       <c r="O32" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01110001</v>
       </c>
       <c r="P32" s="8"/>
@@ -3861,7 +3861,7 @@
         <v>-98</v>
       </c>
       <c r="C33" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10011110</v>
       </c>
       <c r="D33" s="8"/>
@@ -3877,7 +3877,7 @@
         <v>8</v>
       </c>
       <c r="I33" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00001000</v>
       </c>
       <c r="J33" s="8"/>
@@ -3885,7 +3885,7 @@
         <v>61</v>
       </c>
       <c r="L33" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>00111101</v>
       </c>
       <c r="M33" s="8"/>
@@ -3893,7 +3893,7 @@
         <v>114</v>
       </c>
       <c r="O33" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01110010</v>
       </c>
       <c r="P33" s="8"/>
@@ -3904,7 +3904,7 @@
         <v>-97</v>
       </c>
       <c r="C34" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10011111</v>
       </c>
       <c r="D34" s="8"/>
@@ -3912,7 +3912,7 @@
         <v>-44</v>
       </c>
       <c r="F34" s="6" t="str">
-        <f t="shared" ref="F34:F54" si="9">RIGHT(DEC2BIN(E34,8),8)</f>
+        <f t="shared" ref="F34:F54" si="10">RIGHT(DEC2BIN(E34,8),8)</f>
         <v>11010100</v>
       </c>
       <c r="G34" s="8"/>
@@ -3920,7 +3920,7 @@
         <v>9</v>
       </c>
       <c r="I34" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00001001</v>
       </c>
       <c r="J34" s="8"/>
@@ -3928,7 +3928,7 @@
         <v>62</v>
       </c>
       <c r="L34" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>00111110</v>
       </c>
       <c r="M34" s="8"/>
@@ -3936,7 +3936,7 @@
         <v>115</v>
       </c>
       <c r="O34" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01110011</v>
       </c>
       <c r="P34" s="8"/>
@@ -3947,7 +3947,7 @@
         <v>-96</v>
       </c>
       <c r="C35" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10100000</v>
       </c>
       <c r="D35" s="8"/>
@@ -3955,7 +3955,7 @@
         <v>-43</v>
       </c>
       <c r="F35" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11010101</v>
       </c>
       <c r="G35" s="8"/>
@@ -3963,7 +3963,7 @@
         <v>10</v>
       </c>
       <c r="I35" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00001010</v>
       </c>
       <c r="J35" s="8"/>
@@ -3971,7 +3971,7 @@
         <v>63</v>
       </c>
       <c r="L35" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>00111111</v>
       </c>
       <c r="M35" s="8"/>
@@ -3979,7 +3979,7 @@
         <v>116</v>
       </c>
       <c r="O35" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01110100</v>
       </c>
       <c r="P35" s="8"/>
@@ -3990,7 +3990,7 @@
         <v>-95</v>
       </c>
       <c r="C36" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10100001</v>
       </c>
       <c r="D36" s="8"/>
@@ -3998,7 +3998,7 @@
         <v>-42</v>
       </c>
       <c r="F36" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11010110</v>
       </c>
       <c r="G36" s="8"/>
@@ -4006,7 +4006,7 @@
         <v>11</v>
       </c>
       <c r="I36" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00001011</v>
       </c>
       <c r="J36" s="8"/>
@@ -4014,7 +4014,7 @@
         <v>64</v>
       </c>
       <c r="L36" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01000000</v>
       </c>
       <c r="M36" s="8"/>
@@ -4022,7 +4022,7 @@
         <v>117</v>
       </c>
       <c r="O36" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01110101</v>
       </c>
       <c r="P36" s="8"/>
@@ -4033,7 +4033,7 @@
         <v>-94</v>
       </c>
       <c r="C37" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10100010</v>
       </c>
       <c r="D37" s="8"/>
@@ -4041,7 +4041,7 @@
         <v>-41</v>
       </c>
       <c r="F37" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11010111</v>
       </c>
       <c r="G37" s="8"/>
@@ -4049,7 +4049,7 @@
         <v>12</v>
       </c>
       <c r="I37" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00001100</v>
       </c>
       <c r="J37" s="8"/>
@@ -4057,7 +4057,7 @@
         <v>65</v>
       </c>
       <c r="L37" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01000001</v>
       </c>
       <c r="M37" s="8"/>
@@ -4065,7 +4065,7 @@
         <v>118</v>
       </c>
       <c r="O37" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01110110</v>
       </c>
       <c r="P37" s="8"/>
@@ -4076,7 +4076,7 @@
         <v>-93</v>
       </c>
       <c r="C38" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10100011</v>
       </c>
       <c r="D38" s="8"/>
@@ -4084,7 +4084,7 @@
         <v>-40</v>
       </c>
       <c r="F38" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11011000</v>
       </c>
       <c r="G38" s="8"/>
@@ -4092,7 +4092,7 @@
         <v>13</v>
       </c>
       <c r="I38" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00001101</v>
       </c>
       <c r="J38" s="8"/>
@@ -4100,7 +4100,7 @@
         <v>66</v>
       </c>
       <c r="L38" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01000010</v>
       </c>
       <c r="M38" s="8"/>
@@ -4108,7 +4108,7 @@
         <v>119</v>
       </c>
       <c r="O38" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01110111</v>
       </c>
       <c r="P38" s="8"/>
@@ -4119,7 +4119,7 @@
         <v>-92</v>
       </c>
       <c r="C39" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10100100</v>
       </c>
       <c r="D39" s="8"/>
@@ -4127,7 +4127,7 @@
         <v>-39</v>
       </c>
       <c r="F39" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11011001</v>
       </c>
       <c r="G39" s="8"/>
@@ -4135,7 +4135,7 @@
         <v>14</v>
       </c>
       <c r="I39" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00001110</v>
       </c>
       <c r="J39" s="8"/>
@@ -4143,7 +4143,7 @@
         <v>67</v>
       </c>
       <c r="L39" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01000011</v>
       </c>
       <c r="M39" s="8"/>
@@ -4151,7 +4151,7 @@
         <v>120</v>
       </c>
       <c r="O39" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01111000</v>
       </c>
       <c r="P39" s="8"/>
@@ -4162,7 +4162,7 @@
         <v>-91</v>
       </c>
       <c r="C40" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10100101</v>
       </c>
       <c r="D40" s="8"/>
@@ -4170,7 +4170,7 @@
         <v>-38</v>
       </c>
       <c r="F40" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11011010</v>
       </c>
       <c r="G40" s="8"/>
@@ -4178,7 +4178,7 @@
         <v>15</v>
       </c>
       <c r="I40" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00001111</v>
       </c>
       <c r="J40" s="8"/>
@@ -4186,7 +4186,7 @@
         <v>68</v>
       </c>
       <c r="L40" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01000100</v>
       </c>
       <c r="M40" s="8"/>
@@ -4194,7 +4194,7 @@
         <v>121</v>
       </c>
       <c r="O40" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01111001</v>
       </c>
       <c r="P40" s="8"/>
@@ -4205,7 +4205,7 @@
         <v>-90</v>
       </c>
       <c r="C41" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10100110</v>
       </c>
       <c r="D41" s="8"/>
@@ -4213,7 +4213,7 @@
         <v>-37</v>
       </c>
       <c r="F41" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11011011</v>
       </c>
       <c r="G41" s="8"/>
@@ -4221,7 +4221,7 @@
         <v>16</v>
       </c>
       <c r="I41" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00010000</v>
       </c>
       <c r="J41" s="8"/>
@@ -4229,7 +4229,7 @@
         <v>69</v>
       </c>
       <c r="L41" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01000101</v>
       </c>
       <c r="M41" s="8"/>
@@ -4237,7 +4237,7 @@
         <v>122</v>
       </c>
       <c r="O41" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01111010</v>
       </c>
       <c r="P41" s="8"/>
@@ -4248,7 +4248,7 @@
         <v>-89</v>
       </c>
       <c r="C42" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10100111</v>
       </c>
       <c r="D42" s="8"/>
@@ -4256,7 +4256,7 @@
         <v>-36</v>
       </c>
       <c r="F42" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11011100</v>
       </c>
       <c r="G42" s="8"/>
@@ -4264,7 +4264,7 @@
         <v>17</v>
       </c>
       <c r="I42" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00010001</v>
       </c>
       <c r="J42" s="8"/>
@@ -4272,7 +4272,7 @@
         <v>70</v>
       </c>
       <c r="L42" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01000110</v>
       </c>
       <c r="M42" s="8"/>
@@ -4280,7 +4280,7 @@
         <v>123</v>
       </c>
       <c r="O42" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01111011</v>
       </c>
       <c r="P42" s="8"/>
@@ -4291,7 +4291,7 @@
         <v>-88</v>
       </c>
       <c r="C43" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10101000</v>
       </c>
       <c r="D43" s="8"/>
@@ -4299,7 +4299,7 @@
         <v>-35</v>
       </c>
       <c r="F43" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11011101</v>
       </c>
       <c r="G43" s="8"/>
@@ -4307,7 +4307,7 @@
         <v>18</v>
       </c>
       <c r="I43" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00010010</v>
       </c>
       <c r="J43" s="8"/>
@@ -4315,7 +4315,7 @@
         <v>71</v>
       </c>
       <c r="L43" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01000111</v>
       </c>
       <c r="M43" s="8"/>
@@ -4323,7 +4323,7 @@
         <v>124</v>
       </c>
       <c r="O43" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01111100</v>
       </c>
       <c r="P43" s="8"/>
@@ -4334,7 +4334,7 @@
         <v>-87</v>
       </c>
       <c r="C44" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10101001</v>
       </c>
       <c r="D44" s="8"/>
@@ -4342,7 +4342,7 @@
         <v>-34</v>
       </c>
       <c r="F44" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11011110</v>
       </c>
       <c r="G44" s="8"/>
@@ -4350,7 +4350,7 @@
         <v>19</v>
       </c>
       <c r="I44" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00010011</v>
       </c>
       <c r="J44" s="8"/>
@@ -4358,7 +4358,7 @@
         <v>72</v>
       </c>
       <c r="L44" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01001000</v>
       </c>
       <c r="M44" s="8"/>
@@ -4366,7 +4366,7 @@
         <v>125</v>
       </c>
       <c r="O44" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01111101</v>
       </c>
       <c r="P44" s="8"/>
@@ -4377,7 +4377,7 @@
         <v>-86</v>
       </c>
       <c r="C45" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10101010</v>
       </c>
       <c r="D45" s="8"/>
@@ -4385,7 +4385,7 @@
         <v>-33</v>
       </c>
       <c r="F45" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11011111</v>
       </c>
       <c r="G45" s="8"/>
@@ -4393,7 +4393,7 @@
         <v>20</v>
       </c>
       <c r="I45" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00010100</v>
       </c>
       <c r="J45" s="8"/>
@@ -4401,7 +4401,7 @@
         <v>73</v>
       </c>
       <c r="L45" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01001001</v>
       </c>
       <c r="M45" s="8"/>
@@ -4409,7 +4409,7 @@
         <v>126</v>
       </c>
       <c r="O45" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01111110</v>
       </c>
       <c r="P45" s="8"/>
@@ -4420,7 +4420,7 @@
         <v>-85</v>
       </c>
       <c r="C46" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10101011</v>
       </c>
       <c r="D46" s="8"/>
@@ -4428,7 +4428,7 @@
         <v>-32</v>
       </c>
       <c r="F46" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11100000</v>
       </c>
       <c r="G46" s="8"/>
@@ -4436,7 +4436,7 @@
         <v>21</v>
       </c>
       <c r="I46" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00010101</v>
       </c>
       <c r="J46" s="8"/>
@@ -4444,7 +4444,7 @@
         <v>74</v>
       </c>
       <c r="L46" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01001010</v>
       </c>
       <c r="M46" s="8"/>
@@ -4452,7 +4452,7 @@
         <v>127</v>
       </c>
       <c r="O46" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>01111111</v>
       </c>
       <c r="P46" s="8"/>
@@ -4463,7 +4463,7 @@
         <v>-84</v>
       </c>
       <c r="C47" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10101100</v>
       </c>
       <c r="D47" s="8"/>
@@ -4471,7 +4471,7 @@
         <v>-31</v>
       </c>
       <c r="F47" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11100001</v>
       </c>
       <c r="G47" s="8"/>
@@ -4479,7 +4479,7 @@
         <v>22</v>
       </c>
       <c r="I47" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00010110</v>
       </c>
       <c r="J47" s="8"/>
@@ -4487,7 +4487,7 @@
         <v>75</v>
       </c>
       <c r="L47" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01001011</v>
       </c>
       <c r="M47" s="8"/>
@@ -4506,7 +4506,7 @@
         <v>-83</v>
       </c>
       <c r="C48" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10101101</v>
       </c>
       <c r="D48" s="8"/>
@@ -4514,7 +4514,7 @@
         <v>-30</v>
       </c>
       <c r="F48" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11100010</v>
       </c>
       <c r="G48" s="8"/>
@@ -4522,7 +4522,7 @@
         <v>23</v>
       </c>
       <c r="I48" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00010111</v>
       </c>
       <c r="J48" s="8"/>
@@ -4530,7 +4530,7 @@
         <v>76</v>
       </c>
       <c r="L48" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01001100</v>
       </c>
       <c r="M48" s="8"/>
@@ -4538,7 +4538,7 @@
         <v>129</v>
       </c>
       <c r="O48" s="26" t="str">
-        <f t="shared" ref="O48:O54" si="10">DEC2BIN(N48,8)</f>
+        <f t="shared" ref="O48:O54" si="11">DEC2BIN(N48,8)</f>
         <v>10000001</v>
       </c>
       <c r="P48" s="8"/>
@@ -4549,7 +4549,7 @@
         <v>-82</v>
       </c>
       <c r="C49" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10101110</v>
       </c>
       <c r="D49" s="8"/>
@@ -4557,7 +4557,7 @@
         <v>-29</v>
       </c>
       <c r="F49" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11100011</v>
       </c>
       <c r="G49" s="8"/>
@@ -4565,7 +4565,7 @@
         <v>24</v>
       </c>
       <c r="I49" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00011000</v>
       </c>
       <c r="J49" s="8"/>
@@ -4573,7 +4573,7 @@
         <v>77</v>
       </c>
       <c r="L49" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01001101</v>
       </c>
       <c r="M49" s="8"/>
@@ -4581,7 +4581,7 @@
         <v>130</v>
       </c>
       <c r="O49" s="26" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10000010</v>
       </c>
       <c r="P49" s="8"/>
@@ -4592,7 +4592,7 @@
         <v>-81</v>
       </c>
       <c r="C50" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10101111</v>
       </c>
       <c r="D50" s="8"/>
@@ -4600,7 +4600,7 @@
         <v>-28</v>
       </c>
       <c r="F50" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11100100</v>
       </c>
       <c r="G50" s="8"/>
@@ -4608,7 +4608,7 @@
         <v>25</v>
       </c>
       <c r="I50" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00011001</v>
       </c>
       <c r="J50" s="8"/>
@@ -4616,7 +4616,7 @@
         <v>78</v>
       </c>
       <c r="L50" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01001110</v>
       </c>
       <c r="M50" s="8"/>
@@ -4624,7 +4624,7 @@
         <v>131</v>
       </c>
       <c r="O50" s="26" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10000011</v>
       </c>
       <c r="P50" s="8"/>
@@ -4635,7 +4635,7 @@
         <v>-80</v>
       </c>
       <c r="C51" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10110000</v>
       </c>
       <c r="D51" s="8"/>
@@ -4643,7 +4643,7 @@
         <v>-27</v>
       </c>
       <c r="F51" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11100101</v>
       </c>
       <c r="G51" s="8"/>
@@ -4651,7 +4651,7 @@
         <v>26</v>
       </c>
       <c r="I51" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>00011010</v>
       </c>
       <c r="J51" s="8"/>
@@ -4659,7 +4659,7 @@
         <v>79</v>
       </c>
       <c r="L51" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01001111</v>
       </c>
       <c r="M51" s="8"/>
@@ -4667,7 +4667,7 @@
         <v>132</v>
       </c>
       <c r="O51" s="26" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10000100</v>
       </c>
       <c r="P51" s="8"/>
@@ -4678,7 +4678,7 @@
         <v>-79</v>
       </c>
       <c r="C52" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10110001</v>
       </c>
       <c r="D52" s="8"/>
@@ -4686,7 +4686,7 @@
         <v>-26</v>
       </c>
       <c r="F52" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11100110</v>
       </c>
       <c r="G52" s="8"/>
@@ -4702,7 +4702,7 @@
         <v>80</v>
       </c>
       <c r="L52" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01010000</v>
       </c>
       <c r="M52" s="8"/>
@@ -4710,7 +4710,7 @@
         <v>133</v>
       </c>
       <c r="O52" s="26" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10000101</v>
       </c>
       <c r="P52" s="8"/>
@@ -4721,7 +4721,7 @@
         <v>-78</v>
       </c>
       <c r="C53" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10110010</v>
       </c>
       <c r="D53" s="8"/>
@@ -4729,7 +4729,7 @@
         <v>-25</v>
       </c>
       <c r="F53" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11100111</v>
       </c>
       <c r="G53" s="8"/>
@@ -4745,7 +4745,7 @@
         <v>81</v>
       </c>
       <c r="L53" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01010001</v>
       </c>
       <c r="M53" s="8"/>
@@ -4753,7 +4753,7 @@
         <v>134</v>
       </c>
       <c r="O53" s="26" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10000110</v>
       </c>
       <c r="P53" s="8"/>
@@ -4764,7 +4764,7 @@
         <v>-77</v>
       </c>
       <c r="C54" s="54" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10110011</v>
       </c>
       <c r="D54" s="8"/>
@@ -4772,7 +4772,7 @@
         <v>-24</v>
       </c>
       <c r="F54" s="6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11101000</v>
       </c>
       <c r="G54" s="8"/>
@@ -4788,7 +4788,7 @@
         <v>82</v>
       </c>
       <c r="L54" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>01010010</v>
       </c>
       <c r="M54" s="8"/>
@@ -4796,7 +4796,7 @@
         <v>135</v>
       </c>
       <c r="O54" s="26" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10000111</v>
       </c>
       <c r="P54" s="8"/>
@@ -4845,29 +4845,29 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
     </row>
     <row r="3" spans="1:22" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">

</xml_diff>